<commit_message>
PDF generation is in progress
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -16,12 +16,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$G$159</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="324">
   <si>
     <t>Reports</t>
   </si>
@@ -1001,6 +1000,18 @@
   </si>
   <si>
     <t>Done (have added current date as source date for live sites)</t>
+  </si>
+  <si>
+    <t>Investigator name is pending</t>
+  </si>
+  <si>
+    <t>Need clarification from clients</t>
+  </si>
+  <si>
+    <t>partially done. Need to display and sort by 'Match Count'</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -2136,8 +2147,8 @@
   </sheetPr>
   <dimension ref="A1:G218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="D156" sqref="D156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2876,6 +2887,9 @@
       <c r="C77" t="s">
         <v>317</v>
       </c>
+      <c r="D77" t="s">
+        <v>322</v>
+      </c>
       <c r="E77">
         <v>1</v>
       </c>
@@ -2931,6 +2945,9 @@
       <c r="B84" s="7" t="s">
         <v>196</v>
       </c>
+      <c r="D84" t="s">
+        <v>321</v>
+      </c>
       <c r="E84">
         <v>2</v>
       </c>
@@ -2987,6 +3004,9 @@
       <c r="B91" s="9" t="s">
         <v>269</v>
       </c>
+      <c r="D91" t="s">
+        <v>320</v>
+      </c>
       <c r="E91">
         <v>1</v>
       </c>
@@ -3221,6 +3241,9 @@
       <c r="B129" s="7" t="s">
         <v>267</v>
       </c>
+      <c r="D129" t="s">
+        <v>323</v>
+      </c>
       <c r="E129">
         <v>1</v>
       </c>
@@ -3355,6 +3378,9 @@
       </c>
       <c r="C147" s="12" t="s">
         <v>150</v>
+      </c>
+      <c r="D147" s="12" t="s">
+        <v>323</v>
       </c>
       <c r="E147" s="12">
         <v>1</v>

</xml_diff>

<commit_message>
updates - LIveScan Extraction changes
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-405" yWindow="885" windowWidth="20130" windowHeight="11760" tabRatio="375" activeTab="3"/>
+    <workbookView xWindow="180" yWindow="420" windowWidth="20130" windowHeight="11760" tabRatio="375" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="Actions - Post - Demo1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$I$238</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$I$239</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="366">
   <si>
     <t>Reports</t>
   </si>
@@ -1272,6 +1272,9 @@
   </si>
   <si>
     <t>Restore</t>
+  </si>
+  <si>
+    <t>Delete Confirm Error Image</t>
   </si>
 </sst>
 </file>
@@ -2445,13 +2448,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I247"/>
+  <dimension ref="A1:I248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="D73" sqref="D73"/>
+      <selection pane="bottomRight" activeCell="B154" sqref="B154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4641,7 +4644,7 @@
         <v>340</v>
       </c>
       <c r="G170">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H170" s="6"/>
     </row>
@@ -4650,10 +4653,10 @@
         <v>338</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>343</v>
+        <v>365</v>
       </c>
       <c r="G171">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H171" s="6"/>
     </row>
@@ -4662,7 +4665,7 @@
         <v>338</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G172">
         <v>3</v>
@@ -4674,7 +4677,7 @@
         <v>338</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="G173">
         <v>3</v>
@@ -4682,74 +4685,75 @@
       <c r="H173" s="6"/>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" s="12"/>
+      <c r="A174" s="12" t="s">
+        <v>338</v>
+      </c>
       <c r="B174" s="7" t="s">
-        <v>359</v>
+        <v>342</v>
+      </c>
+      <c r="G174">
+        <v>3</v>
       </c>
       <c r="H174" s="6"/>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="12"/>
       <c r="B175" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H175" s="6"/>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="12"/>
+      <c r="B176" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="H175" s="6"/>
-    </row>
-    <row r="176" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B176" s="17" t="s">
+      <c r="H176" s="6"/>
+    </row>
+    <row r="177" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B177" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="H176" s="6"/>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B177" s="15" t="s">
+      <c r="H177" s="6"/>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B178" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="H177" s="6"/>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B178" s="7" t="s">
+      <c r="H178" s="6"/>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B179" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="G178">
-        <v>2</v>
-      </c>
-      <c r="H178" s="6"/>
-    </row>
-    <row r="179" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="12" t="s">
-        <v>320</v>
-      </c>
-      <c r="B179" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="C179" s="15"/>
-      <c r="D179" s="15"/>
-      <c r="H179" s="14"/>
-    </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G179">
+        <v>2</v>
+      </c>
+      <c r="H179" s="6"/>
+    </row>
+    <row r="180" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="B180" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E180" t="s">
-        <v>135</v>
-      </c>
-      <c r="G180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B180" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="C180" s="15"/>
+      <c r="D180" s="15"/>
+      <c r="H180" s="14"/>
+    </row>
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>320</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>333</v>
+        <v>136</v>
+      </c>
+      <c r="E181" t="s">
+        <v>135</v>
       </c>
       <c r="G181">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -4757,10 +4761,10 @@
         <v>320</v>
       </c>
       <c r="B182" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G182">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -4768,53 +4772,53 @@
         <v>320</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>257</v>
+        <v>334</v>
       </c>
       <c r="G183">
         <v>2</v>
       </c>
-      <c r="H183" s="6"/>
-    </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
         <v>320</v>
       </c>
       <c r="B184" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G184">
+        <v>2</v>
+      </c>
+      <c r="H184" s="6"/>
+    </row>
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="12" t="s">
+        <v>320</v>
+      </c>
+      <c r="B185" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="G184">
-        <v>0</v>
-      </c>
-      <c r="I184" t="s">
+      <c r="G185">
+        <v>0</v>
+      </c>
+      <c r="I185" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A185" s="12"/>
-      <c r="B185" s="7" t="s">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186" s="12"/>
+      <c r="B186" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="G185">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A186" s="12" t="s">
-        <v>302</v>
-      </c>
-      <c r="B186" s="8" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="B187" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G187">
-        <v>0</v>
+      <c r="B187" s="8" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -4822,30 +4826,22 @@
         <v>302</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E188" t="s">
-        <v>135</v>
+        <v>303</v>
       </c>
       <c r="G188">
         <v>0</v>
-      </c>
-      <c r="H188" s="6">
-        <v>42702</v>
-      </c>
-      <c r="I188" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="B189" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C189" s="9"/>
-      <c r="D189" s="9"/>
+      <c r="B189" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E189" t="s">
+        <v>135</v>
+      </c>
       <c r="G189">
         <v>0</v>
       </c>
@@ -4860,17 +4856,19 @@
       <c r="A190" s="12" t="s">
         <v>302</v>
       </c>
-      <c r="B190" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E190" t="s">
-        <v>135</v>
-      </c>
+      <c r="B190" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C190" s="9"/>
+      <c r="D190" s="9"/>
       <c r="G190">
         <v>0</v>
       </c>
       <c r="H190" s="6">
         <v>42702</v>
+      </c>
+      <c r="I190" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -4878,13 +4876,16 @@
         <v>302</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="E191" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G191">
         <v>0</v>
+      </c>
+      <c r="H191" s="6">
+        <v>42702</v>
       </c>
     </row>
     <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -4892,7 +4893,7 @@
         <v>302</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E192" t="s">
         <v>137</v>
@@ -4900,184 +4901,190 @@
       <c r="G192">
         <v>0</v>
       </c>
-      <c r="H192" s="6">
-        <v>42697</v>
-      </c>
-      <c r="I192" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>302</v>
       </c>
       <c r="B193" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E193" t="s">
+        <v>137</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193" s="6">
+        <v>42697</v>
+      </c>
+      <c r="I193" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B194" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="G193">
-        <v>2</v>
-      </c>
-      <c r="H193" s="6"/>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A194" s="12"/>
-      <c r="B194" s="13" t="s">
+      <c r="G194">
+        <v>2</v>
+      </c>
+      <c r="H194" s="6"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195" s="12"/>
+      <c r="B195" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="H194" s="6"/>
-    </row>
-    <row r="195" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B195" s="17" t="s">
+      <c r="H195" s="6"/>
+    </row>
+    <row r="196" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B196" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C195" s="17"/>
-      <c r="D195" s="17"/>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B196" s="8" t="s">
+      <c r="C196" s="17"/>
+      <c r="D196" s="17"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B197" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="G196">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
+      <c r="G197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
         <v>318</v>
       </c>
-      <c r="C197" s="7" t="s">
+      <c r="C198" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="D197" s="28">
+      <c r="D198" s="28">
         <v>42775</v>
       </c>
-      <c r="G197">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B198" s="7" t="s">
+      <c r="G198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B199" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="G198">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B199" t="s">
+      <c r="G199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
         <v>310</v>
       </c>
-      <c r="C199" s="7" t="s">
+      <c r="C200" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="D199" s="28">
+      <c r="D200" s="28">
         <v>42775</v>
       </c>
-      <c r="G199">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H200" s="6"/>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B201" s="8" t="s">
+      <c r="G200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H201" s="6"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B202" s="8" t="s">
         <v>361</v>
       </c>
-      <c r="H201" s="6"/>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B202" s="7" t="s">
+      <c r="H202" s="6"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B203" s="7" t="s">
         <v>362</v>
-      </c>
-      <c r="G202">
-        <v>3</v>
-      </c>
-      <c r="H202" s="6"/>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B203" s="7" t="s">
-        <v>363</v>
       </c>
       <c r="G203">
         <v>3</v>
       </c>
       <c r="H203" s="6"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B204" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G204">
         <v>3</v>
       </c>
       <c r="H204" s="6"/>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B205" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="G205">
+        <v>3</v>
+      </c>
       <c r="H205" s="6"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B206" s="8" t="s">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H206" s="6"/>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B207" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C206" s="8"/>
-      <c r="D206" s="8"/>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A207">
-        <v>1</v>
-      </c>
-      <c r="B207" s="7" t="s">
+      <c r="C207" s="8"/>
+      <c r="D207" s="8"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>1</v>
+      </c>
+      <c r="B208" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="E207" t="s">
+      <c r="E208" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A208">
-        <v>2</v>
-      </c>
-      <c r="B208" s="7" t="s">
+    <row r="209" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>2</v>
+      </c>
+      <c r="B209" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="E208" t="s">
+      <c r="E209" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209">
-        <v>3</v>
-      </c>
-      <c r="B209" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E209" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210">
+        <v>3</v>
+      </c>
+      <c r="B210" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E210" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211">
         <v>4</v>
       </c>
-      <c r="B210" s="7" t="s">
+      <c r="B211" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>176</v>
       </c>
-      <c r="B211" s="7" t="s">
+      <c r="B212" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="E211" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B212" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="E212" t="s">
         <v>213</v>
@@ -5085,7 +5092,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B213" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E213" t="s">
         <v>213</v>
@@ -5093,207 +5100,201 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B214" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E214" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B215" s="7" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="E215" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="216" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B216" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="E216" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B217" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="E216" t="s">
+      <c r="E217" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B217" s="10" t="s">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B218" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C217" s="10"/>
-      <c r="D217" s="10"/>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B218" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="E218" t="s">
-        <v>216</v>
-      </c>
+      <c r="C218" s="10"/>
+      <c r="D218" s="10"/>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B219" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
+      </c>
+      <c r="E219" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B220" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B221" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B221" s="7" t="s">
+    <row r="222" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B222" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B222" s="7" t="s">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B223" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B223" s="7" t="s">
+    <row r="224" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B224" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E223" t="s">
+      <c r="E224" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="7" t="s">
+    <row r="225" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B225" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B225" s="7" t="s">
+    <row r="226" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B226" s="7" t="s">
         <v>196</v>
-      </c>
-      <c r="E225" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B226" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="E226" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B227" s="10" t="s">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B227" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E227" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B228" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="C227" s="10"/>
-      <c r="D227" s="10"/>
-    </row>
-    <row r="228" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B228" s="7" t="s">
+      <c r="C228" s="10"/>
+      <c r="D228" s="10"/>
+    </row>
+    <row r="229" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B229" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="E228" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="229" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B229" s="7" t="s">
-        <v>191</v>
       </c>
       <c r="E229" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B230" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E230" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B231" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B231" s="7" t="s">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B232" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A232">
-        <v>1</v>
-      </c>
-      <c r="B232" s="7" t="s">
+    <row r="233" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>1</v>
+      </c>
+      <c r="B233" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="G232">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A233">
-        <v>2</v>
-      </c>
-      <c r="B233" s="7" t="s">
+      <c r="G233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>2</v>
+      </c>
+      <c r="B234" s="7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B234" s="7" t="s">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B235" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="G234">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B235" s="7" t="s">
+      <c r="G235">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B236" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="G235">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B236" s="7" t="s">
+      <c r="G236">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B237" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="G236">
+      <c r="G237">
         <v>3</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B237" s="7" t="s">
+    <row r="238" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B238" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="G237">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B238" s="7" t="s">
+      <c r="G238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B239" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="G238">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E239" s="20"/>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B240" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E240" t="s">
-        <v>221</v>
-      </c>
-      <c r="G240">
-        <v>0</v>
-      </c>
-      <c r="H240" t="s">
-        <v>146</v>
-      </c>
+      <c r="G239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E240" s="20"/>
     </row>
     <row r="241" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B241" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E241" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G241">
         <v>0</v>
@@ -5304,10 +5305,10 @@
     </row>
     <row r="242" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B242" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E242" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G242">
         <v>0</v>
@@ -5316,9 +5317,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="243" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="243" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B243" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
+      </c>
+      <c r="E243" t="s">
+        <v>223</v>
       </c>
       <c r="G243">
         <v>0</v>
@@ -5327,9 +5331,9 @@
         <v>146</v>
       </c>
     </row>
-    <row r="244" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B244" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G244">
         <v>0</v>
@@ -5340,7 +5344,7 @@
     </row>
     <row r="245" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B245" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G245">
         <v>0</v>
@@ -5349,13 +5353,24 @@
         <v>146</v>
       </c>
     </row>
-    <row r="247" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B247" s="7" t="s">
+    <row r="246" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B246" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G246">
+        <v>0</v>
+      </c>
+      <c r="H246" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="248" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B248" s="7" t="s">
         <v>220</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:I238">
+  <autoFilter ref="A7:I239">
     <filterColumn colId="6">
       <filters blank="1">
         <filter val="1"/>

</xml_diff>

<commit_message>
Live Scan related changes.  Add Matching REcords function Alternate developed for Live Scan.  Tested Ok New Proj DDAS.LiveSiteExtractor - added, tested, Ok
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -13,14 +13,14 @@
     <sheet name="Actions - Post - Demo1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$I$247</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$I$250</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="380">
   <si>
     <t>Reports</t>
   </si>
@@ -1308,6 +1308,15 @@
   </si>
   <si>
     <t xml:space="preserve">Enhancement  </t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Status Color displays grey immediately on first Save.</t>
+  </si>
+  <si>
+    <t>Devp / Staging / - flag under ICON flag</t>
   </si>
 </sst>
 </file>
@@ -2481,13 +2490,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I256"/>
+  <dimension ref="A1:I259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B83" sqref="B83"/>
+      <selection pane="bottomRight" activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2702,7 @@
         <v>250</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
@@ -2832,7 +2841,7 @@
       <c r="C25" s="13"/>
       <c r="D25" s="20"/>
       <c r="G25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2894,7 +2903,7 @@
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
       <c r="G30" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2920,7 +2929,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="G32">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2933,6 +2942,9 @@
       <c r="F33" t="s">
         <v>322</v>
       </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
@@ -3062,6 +3074,9 @@
       <c r="F42" t="s">
         <v>322</v>
       </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
@@ -3073,6 +3088,9 @@
       <c r="F43" t="s">
         <v>322</v>
       </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
@@ -3136,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="9" t="s">
         <v>369</v>
@@ -3147,7 +3165,7 @@
         <v>322</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3187,7 +3205,7 @@
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
       <c r="G52" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3274,7 +3292,7 @@
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
       <c r="G58">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -3287,7 +3305,7 @@
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="G59">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -3516,7 +3534,7 @@
         <v>135</v>
       </c>
       <c r="G75" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H75" s="27"/>
     </row>
@@ -3531,7 +3549,7 @@
         <v>135</v>
       </c>
       <c r="G76">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H76" s="6"/>
     </row>
@@ -3548,7 +3566,7 @@
         <v>275</v>
       </c>
       <c r="G77" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H77" s="14"/>
     </row>
@@ -3563,7 +3581,7 @@
         <v>140</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H78" s="6"/>
     </row>
@@ -3633,7 +3651,7 @@
       </c>
       <c r="H82" s="6"/>
     </row>
-    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>2</v>
       </c>
@@ -3648,246 +3666,248 @@
         <v>322</v>
       </c>
       <c r="G83" s="12">
+        <v>0</v>
+      </c>
+      <c r="H83" s="6"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="12"/>
+      <c r="B84" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="D84" s="28"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="6"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="12"/>
+      <c r="B85" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="D85" s="28"/>
+      <c r="F85" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="G85" s="12">
         <v>1</v>
       </c>
-      <c r="H83" s="6"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" s="8" t="s">
+      <c r="H85" s="6"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>366</v>
       </c>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="G84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B85" s="7" t="s">
+      <c r="C86" s="8"/>
+      <c r="D86" s="8"/>
+      <c r="G86" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="G85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="22" t="s">
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B88" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="C86" s="20" t="s">
+      <c r="C88" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D86" s="20">
+      <c r="D88" s="20">
         <v>42760</v>
       </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" s="7" t="s">
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="G87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88" s="7" t="s">
+      <c r="G89">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
-      <c r="B89" s="7" t="s">
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="12"/>
+      <c r="B91" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F91" t="s">
         <v>370</v>
       </c>
-      <c r="G89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="12"/>
-      <c r="B90" s="7" t="s">
-        <v>368</v>
-      </c>
-      <c r="F90" t="s">
-        <v>322</v>
-      </c>
-      <c r="G90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
       <c r="G91">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B92" s="9" t="s">
+      <c r="A92" s="12"/>
+      <c r="B92" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="F92" t="s">
+        <v>322</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="C93" s="8"/>
+      <c r="D93" s="8"/>
+      <c r="G93" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="9" t="s">
         <v>240</v>
-      </c>
-      <c r="C92" s="9"/>
-      <c r="D92" s="9"/>
-      <c r="G92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B93" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="C93" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="D93" s="20">
-        <v>42760</v>
-      </c>
-      <c r="G93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B94" s="10" t="s">
-        <v>237</v>
       </c>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="G94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B95" s="7" t="s">
+      <c r="B95" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="C95" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D95" s="20">
+        <v>42760</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="G96" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="G95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B96" s="21" t="s">
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="C96" s="20" t="s">
+      <c r="C98" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="D96" s="20">
+      <c r="D98" s="20">
         <v>42760</v>
       </c>
-      <c r="G96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
-      <c r="B97" s="21" t="s">
-        <v>346</v>
-      </c>
-      <c r="C97" s="20"/>
-      <c r="D97" s="20"/>
-    </row>
-    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A98" s="12"/>
-      <c r="B98" s="21" t="s">
-        <v>344</v>
-      </c>
-      <c r="C98" s="20"/>
-      <c r="D98" s="20"/>
+      <c r="G98">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="21" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C99" s="20"/>
       <c r="D99" s="20"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B100" s="8" t="s">
+    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A100" s="12"/>
+      <c r="B100" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C100" s="20"/>
+      <c r="D100" s="20"/>
+    </row>
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="12"/>
+      <c r="B101" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="C101" s="20"/>
+      <c r="D101" s="20"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-    </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B101" s="7" t="s">
+      <c r="C102" s="8"/>
+      <c r="D102" s="8"/>
+    </row>
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="G101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>244</v>
-      </c>
-      <c r="G102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>270</v>
-      </c>
       <c r="G103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -3895,167 +3915,161 @@
         <v>2</v>
       </c>
       <c r="B104" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="G105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="G104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="7" t="s">
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="G105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="8" t="s">
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-    </row>
-    <row r="107" spans="1:7" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="23" t="s">
+      <c r="C108" s="8"/>
+      <c r="D108" s="8"/>
+    </row>
+    <row r="109" spans="1:7" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="23" t="s">
         <v>281</v>
       </c>
-      <c r="C107" s="13" t="s">
+      <c r="C109" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="D107" s="20">
+      <c r="D109" s="20">
         <v>42760</v>
       </c>
-      <c r="E107" s="12" t="s">
+      <c r="E109" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="G107" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B108" s="24" t="s">
+      <c r="G109" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="C108" s="13" t="s">
+      <c r="C110" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="D108" s="20">
+      <c r="D110" s="20">
         <v>42760</v>
       </c>
-      <c r="E108" s="20" t="s">
+      <c r="E110" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="G108" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="19" t="s">
+      <c r="G110" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="19" t="s">
         <v>373</v>
       </c>
-      <c r="C109" s="13"/>
-      <c r="D109" s="20"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="12" t="s">
+      <c r="C111" s="13"/>
+      <c r="D111" s="20"/>
+      <c r="E111" s="20"/>
+      <c r="F111" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="G109" s="12">
+      <c r="G111" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B110" s="7" t="s">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E112" t="s">
         <v>140</v>
       </c>
-      <c r="G110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" s="9" t="s">
+      <c r="G112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C111" s="9"/>
-      <c r="D111" s="9"/>
-      <c r="G111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="C112" s="9"/>
-      <c r="D112" s="9"/>
-      <c r="G112">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E113" t="s">
-        <v>135</v>
-      </c>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
       <c r="G113">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B114" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E114" t="s">
-        <v>140</v>
-      </c>
+      <c r="B114" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
       <c r="G114">
         <v>3</v>
       </c>
-      <c r="H114" s="6">
-        <v>42702</v>
-      </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
+      </c>
+      <c r="E115" t="s">
+        <v>135</v>
       </c>
       <c r="G115">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -4063,7 +4077,16 @@
         <v>2</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
+      </c>
+      <c r="E116" t="s">
+        <v>140</v>
+      </c>
+      <c r="G116">
+        <v>3</v>
+      </c>
+      <c r="H116" s="6">
+        <v>42702</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -4071,7 +4094,10 @@
         <v>2</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>125</v>
+        <v>121</v>
+      </c>
+      <c r="G117">
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -4079,7 +4105,7 @@
         <v>2</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -4087,7 +4113,7 @@
         <v>2</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4095,7 +4121,7 @@
         <v>2</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4103,272 +4129,265 @@
         <v>2</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B124" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="C122" s="8"/>
-      <c r="D122" s="8"/>
-    </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B123" s="7" t="s">
+      <c r="C124" s="8"/>
+      <c r="D124" s="8"/>
+    </row>
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B125" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="G123">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B124" s="7" t="s">
+      <c r="G125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="G124">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B125" s="7" t="s">
+      <c r="G126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B127" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="G125">
+      <c r="G127">
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B126" s="8" t="s">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="12"/>
+      <c r="B128" s="7" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="8" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B127" t="s">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" t="s">
         <v>306</v>
       </c>
-      <c r="C127" s="7" t="s">
+      <c r="C130" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="D127" s="28">
+      <c r="D130" s="28">
         <v>42775</v>
       </c>
-      <c r="G127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B128" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B129" t="s">
-        <v>318</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="D129" s="28">
-        <v>42775</v>
-      </c>
-      <c r="G129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>133</v>
+      <c r="G130">
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B131" s="7" t="s">
-        <v>356</v>
+      <c r="B131" t="s">
+        <v>308</v>
+      </c>
+      <c r="G131">
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B132" s="7" t="s">
-        <v>168</v>
+      <c r="B132" t="s">
+        <v>318</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D132" s="28">
+        <v>42775</v>
       </c>
       <c r="G132">
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="C133" s="17"/>
-      <c r="D133" s="17"/>
+      <c r="B133" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G133">
+        <v>3</v>
+      </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B134" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="C134" s="8"/>
-      <c r="D134" s="8"/>
+      <c r="B134" s="7" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B135" s="9" t="s">
+      <c r="B135" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A136" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B136" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C136" s="17"/>
+      <c r="D136" s="17"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C137" s="8"/>
+      <c r="D137" s="8"/>
+    </row>
+    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="9" t="s">
         <v>298</v>
       </c>
-      <c r="G135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B136" s="9" t="s">
+      <c r="G138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="G136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="12"/>
-      <c r="B137" s="9" t="s">
+      <c r="G139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="12"/>
+      <c r="B140" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="G137">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A138" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B138" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C138" s="17"/>
-      <c r="D138" s="17"/>
-    </row>
-    <row r="139" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A139" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B139" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="C139" s="17"/>
-      <c r="D139" s="17"/>
-    </row>
-    <row r="140" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A140" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="C140" s="17"/>
-      <c r="D140" s="17"/>
+      <c r="G140">
+        <v>0</v>
+      </c>
     </row>
     <row r="141" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A141" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B141" s="9"/>
+      <c r="B141" s="17" t="s">
+        <v>1</v>
+      </c>
       <c r="C141" s="17"/>
       <c r="D141" s="17"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A142" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
-    </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+      <c r="C142" s="17"/>
+      <c r="D142" s="17"/>
+    </row>
+    <row r="143" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A143" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="C143" s="9"/>
-      <c r="D143" s="9"/>
-      <c r="G143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+      <c r="C143" s="17"/>
+      <c r="D143" s="17"/>
+    </row>
+    <row r="144" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A144" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B144" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="C144" s="9"/>
-      <c r="D144" s="9"/>
-      <c r="G144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B144" s="9"/>
+      <c r="C144" s="17"/>
+      <c r="D144" s="17"/>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B145" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="G145">
-        <v>0</v>
-      </c>
+      <c r="B145" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C145" s="8"/>
+      <c r="D145" s="8"/>
     </row>
     <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B146" s="7" t="s">
-        <v>241</v>
-      </c>
+      <c r="B146" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
       <c r="G146">
         <v>0</v>
       </c>
@@ -4377,149 +4396,138 @@
       <c r="A147" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B147" s="7" t="s">
-        <v>235</v>
-      </c>
+      <c r="B147" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
       <c r="G147">
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A148" s="12"/>
-      <c r="B148" s="10" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A149" s="12"/>
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B148" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="12" t="s">
+        <v>1</v>
+      </c>
       <c r="B149" s="7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B150" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
-      <c r="G150" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B151" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="12" t="s">
-        <v>1</v>
-      </c>
+      <c r="B150" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="G150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A151" s="12"/>
+      <c r="B151" s="10" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A152" s="12"/>
       <c r="B152" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="E152" t="s">
-        <v>140</v>
-      </c>
-      <c r="G152">
-        <v>0</v>
-      </c>
-      <c r="H152" s="6">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B153" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="G153">
-        <v>0</v>
-      </c>
-      <c r="H153" s="6"/>
+      <c r="B153" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
+      <c r="G153" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B154" s="7" t="s">
-        <v>229</v>
-      </c>
-      <c r="F154" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="G154">
         <v>0</v>
       </c>
-      <c r="H154" s="6"/>
-    </row>
-    <row r="155" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B155" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C155" s="13"/>
-      <c r="D155" s="13"/>
-      <c r="G155" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B155" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="E155" t="s">
+        <v>140</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155" s="6">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B156" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="C156" s="13"/>
-      <c r="D156" s="13"/>
-      <c r="F156" t="s">
-        <v>140</v>
-      </c>
-      <c r="G156" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B156" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156" s="6"/>
+    </row>
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B157" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="C157" s="13"/>
-      <c r="D157" s="13"/>
+      <c r="B157" s="7" t="s">
+        <v>229</v>
+      </c>
       <c r="F157" t="s">
         <v>140</v>
       </c>
-      <c r="G157" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G157">
+        <v>0</v>
+      </c>
+      <c r="H157" s="6"/>
+    </row>
+    <row r="158" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B158" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="F158" t="s">
-        <v>140</v>
-      </c>
-      <c r="G158">
+      <c r="B158" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C158" s="13"/>
+      <c r="D158" s="13"/>
+      <c r="G158" s="12">
         <v>0</v>
       </c>
     </row>
@@ -4528,97 +4536,98 @@
         <v>1</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>123</v>
+        <v>256</v>
       </c>
       <c r="C159" s="13"/>
       <c r="D159" s="13"/>
+      <c r="F159" t="s">
+        <v>140</v>
+      </c>
       <c r="G159" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B160" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="G160">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B160" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="C160" s="13"/>
+      <c r="D160" s="13"/>
+      <c r="F160" t="s">
+        <v>140</v>
+      </c>
+      <c r="G160" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B161" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C161" s="13"/>
-      <c r="D161" s="13"/>
-      <c r="E161" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="G161" s="12">
-        <v>0</v>
-      </c>
-      <c r="H161" s="14">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F161" t="s">
+        <v>140</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="12" t="s">
+        <v>1</v>
+      </c>
       <c r="B162" s="13" t="s">
-        <v>348</v>
+        <v>123</v>
       </c>
       <c r="C162" s="13"/>
       <c r="D162" s="13"/>
       <c r="G162" s="12">
-        <v>1</v>
-      </c>
-      <c r="H162" s="14"/>
-    </row>
-    <row r="163" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B163" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="C163" s="15"/>
-      <c r="D163" s="15"/>
-      <c r="E163" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="G163" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H163" s="14"/>
-    </row>
-    <row r="164" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B164" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="C164" s="15"/>
-      <c r="D164" s="15"/>
+      <c r="B164" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C164" s="13"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="12" t="s">
+        <v>135</v>
+      </c>
       <c r="G164" s="12">
-        <v>2</v>
-      </c>
-      <c r="H164" s="14"/>
-    </row>
-    <row r="165" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H164" s="14">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B165" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C165" s="13"/>
+      <c r="D165" s="13"/>
+      <c r="G165" s="12">
         <v>1</v>
-      </c>
-      <c r="B165" s="19" t="s">
-        <v>349</v>
-      </c>
-      <c r="C165" s="15"/>
-      <c r="D165" s="15"/>
-      <c r="G165" s="12">
-        <v>0</v>
       </c>
       <c r="H165" s="14"/>
     </row>
@@ -4626,41 +4635,44 @@
       <c r="A166" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B166" s="19" t="s">
-        <v>328</v>
+      <c r="B166" s="15" t="s">
+        <v>261</v>
       </c>
       <c r="C166" s="15"/>
       <c r="D166" s="15"/>
+      <c r="E166" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G166" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="H166" s="14"/>
     </row>
     <row r="167" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B167" s="15" t="s">
-        <v>263</v>
+      <c r="B167" s="19" t="s">
+        <v>297</v>
       </c>
       <c r="C167" s="15"/>
       <c r="D167" s="15"/>
-      <c r="E167" s="12" t="s">
-        <v>135</v>
-      </c>
       <c r="G167" s="12">
         <v>2</v>
       </c>
       <c r="H167" s="14"/>
     </row>
-    <row r="168" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B168" s="19" t="s">
-        <v>331</v>
+        <v>349</v>
       </c>
       <c r="C168" s="15"/>
       <c r="D168" s="15"/>
       <c r="G168" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H168" s="14"/>
     </row>
@@ -4668,8 +4680,8 @@
       <c r="A169" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B169" s="15" t="s">
-        <v>329</v>
+      <c r="B169" s="19" t="s">
+        <v>328</v>
       </c>
       <c r="C169" s="15"/>
       <c r="D169" s="15"/>
@@ -4680,79 +4692,88 @@
         <v>1</v>
       </c>
       <c r="B170" s="15" t="s">
-        <v>330</v>
+        <v>263</v>
       </c>
       <c r="C170" s="15"/>
       <c r="D170" s="15"/>
+      <c r="E170" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G170" s="12">
+        <v>2</v>
+      </c>
       <c r="H170" s="14"/>
     </row>
     <row r="171" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B171" s="15" t="s">
-        <v>273</v>
+      <c r="B171" s="19" t="s">
+        <v>331</v>
       </c>
       <c r="C171" s="15"/>
       <c r="D171" s="15"/>
+      <c r="G171" s="12">
+        <v>1</v>
+      </c>
       <c r="H171" s="14"/>
     </row>
-    <row r="172" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B172" s="18" t="s">
+      <c r="B172" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="C172" s="15"/>
+      <c r="D172" s="15"/>
+      <c r="H172" s="14"/>
+    </row>
+    <row r="173" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B173" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="C173" s="15"/>
+      <c r="D173" s="15"/>
+      <c r="H173" s="14"/>
+    </row>
+    <row r="174" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="C174" s="15"/>
+      <c r="D174" s="15"/>
+      <c r="H174" s="14"/>
+    </row>
+    <row r="175" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B175" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="C172" s="18"/>
-      <c r="D172" s="18"/>
-      <c r="E172" s="3" t="s">
+      <c r="C175" s="18"/>
+      <c r="D175" s="18"/>
+      <c r="E175" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H172" s="27"/>
-    </row>
-    <row r="173" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A173" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="B173" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="H173" s="6"/>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A174" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="B174" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="G174">
+      <c r="G175" s="3">
         <v>3</v>
       </c>
-      <c r="H174" s="6"/>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A175" s="12" t="s">
-        <v>337</v>
-      </c>
-      <c r="B175" s="7" t="s">
-        <v>325</v>
-      </c>
-      <c r="G175">
-        <v>3</v>
-      </c>
-      <c r="H175" s="6"/>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H175" s="27"/>
+    </row>
+    <row r="176" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A176" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="B176" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="G176">
-        <v>3</v>
+      <c r="B176" s="17" t="s">
+        <v>323</v>
       </c>
       <c r="H176" s="6"/>
     </row>
@@ -4761,22 +4782,22 @@
         <v>337</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="G177">
         <v>3</v>
       </c>
       <c r="H177" s="6"/>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>337</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="G178">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H178" s="6"/>
     </row>
@@ -4785,10 +4806,10 @@
         <v>337</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="G179">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H179" s="6"/>
     </row>
@@ -4797,22 +4818,22 @@
         <v>337</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="G180">
         <v>3</v>
       </c>
       <c r="H180" s="6"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>337</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G181">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H181" s="6"/>
     </row>
@@ -4821,125 +4842,126 @@
         <v>337</v>
       </c>
       <c r="B182" s="7" t="s">
+        <v>364</v>
+      </c>
+      <c r="G182">
+        <v>2</v>
+      </c>
+      <c r="H182" s="6"/>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A183" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B183" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="G183">
+        <v>3</v>
+      </c>
+      <c r="H183" s="6"/>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A184" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B184" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="G184">
+        <v>3</v>
+      </c>
+      <c r="H184" s="6"/>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A185" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B185" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="G182">
+      <c r="G185">
         <v>3</v>
       </c>
-      <c r="H182" s="6"/>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A183" s="12"/>
-      <c r="B183" s="7" t="s">
+      <c r="H185" s="6"/>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A186" s="12"/>
+      <c r="B186" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="H183" s="6"/>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A184" s="12"/>
-      <c r="B184" s="7" t="s">
+      <c r="H186" s="6"/>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A187" s="12"/>
+      <c r="B187" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="H184" s="6"/>
-    </row>
-    <row r="185" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B185" s="17" t="s">
+      <c r="H187" s="6"/>
+    </row>
+    <row r="188" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B188" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="H185" s="6"/>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B186" s="15" t="s">
+      <c r="H188" s="6"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B189" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="H186" s="6"/>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B187" s="7" t="s">
+      <c r="H189" s="6"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B190" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="G187">
-        <v>2</v>
-      </c>
-      <c r="H187" s="6"/>
-    </row>
-    <row r="188" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="B188" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="C188" s="15"/>
-      <c r="D188" s="15"/>
-      <c r="H188" s="14"/>
-    </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="B189" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E189" t="s">
-        <v>135</v>
-      </c>
-      <c r="G189">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A190" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="B190" s="7" t="s">
-        <v>332</v>
-      </c>
       <c r="G190">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H190" s="6"/>
+    </row>
+    <row r="191" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="B191" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="G191">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B191" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C191" s="15"/>
+      <c r="D191" s="15"/>
+      <c r="H191" s="14"/>
+    </row>
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="12" t="s">
         <v>319</v>
       </c>
       <c r="B192" s="7" t="s">
-        <v>257</v>
+        <v>136</v>
+      </c>
+      <c r="E192" t="s">
+        <v>135</v>
       </c>
       <c r="G192">
-        <v>2</v>
-      </c>
-      <c r="H192" s="6"/>
-    </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>319</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>122</v>
+        <v>332</v>
       </c>
       <c r="G193">
-        <v>0</v>
-      </c>
-      <c r="I193" t="s">
-        <v>146</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A194" s="12"/>
+      <c r="A194" s="12" t="s">
+        <v>319</v>
+      </c>
       <c r="B194" s="7" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="G194">
         <v>2</v>
@@ -4947,60 +4969,45 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B195" s="8" t="s">
-        <v>301</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="B195" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="G195">
+        <v>2</v>
+      </c>
+      <c r="H195" s="6"/>
     </row>
     <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>302</v>
+        <v>122</v>
       </c>
       <c r="G196">
         <v>0</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="12" t="s">
-        <v>301</v>
-      </c>
+      <c r="I196" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="12"/>
       <c r="B197" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E197" t="s">
-        <v>135</v>
+        <v>350</v>
       </c>
       <c r="G197">
-        <v>0</v>
-      </c>
-      <c r="H197" s="6">
-        <v>42702</v>
-      </c>
-      <c r="I197" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="B198" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C198" s="9"/>
-      <c r="D198" s="9"/>
-      <c r="G198">
-        <v>0</v>
-      </c>
-      <c r="H198" s="6">
-        <v>42702</v>
-      </c>
-      <c r="I198" t="s">
-        <v>146</v>
+      <c r="B198" s="8" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -5008,16 +5015,10 @@
         <v>301</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E199" t="s">
-        <v>135</v>
+        <v>302</v>
       </c>
       <c r="G199">
         <v>0</v>
-      </c>
-      <c r="H199" s="6">
-        <v>42702</v>
       </c>
     </row>
     <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
@@ -5025,447 +5026,464 @@
         <v>301</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E200" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G200">
         <v>0</v>
+      </c>
+      <c r="H200" s="6">
+        <v>42702</v>
+      </c>
+      <c r="I200" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="B201" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E201" t="s">
-        <v>137</v>
-      </c>
+      <c r="B201" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C201" s="9"/>
+      <c r="D201" s="9"/>
       <c r="G201">
         <v>0</v>
       </c>
       <c r="H201" s="6">
-        <v>42697</v>
+        <v>42702</v>
       </c>
       <c r="I201" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
         <v>301</v>
       </c>
       <c r="B202" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E202" t="s">
+        <v>135</v>
+      </c>
+      <c r="G202">
+        <v>0</v>
+      </c>
+      <c r="H202" s="6">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B203" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E203" t="s">
+        <v>137</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B204" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E204" t="s">
+        <v>137</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
+      <c r="H204" s="6">
+        <v>42697</v>
+      </c>
+      <c r="I204" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B205" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="G202">
-        <v>2</v>
-      </c>
-      <c r="H202" s="6"/>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A203" s="12"/>
-      <c r="B203" s="13" t="s">
+      <c r="G205">
+        <v>2</v>
+      </c>
+      <c r="H205" s="6"/>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="12"/>
+      <c r="B206" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="H203" s="6"/>
-    </row>
-    <row r="204" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B204" s="17" t="s">
+      <c r="H206" s="6"/>
+    </row>
+    <row r="207" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B207" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C204" s="17"/>
-      <c r="D204" s="17"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B205" s="8" t="s">
+      <c r="C207" s="17"/>
+      <c r="D207" s="17"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B208" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="G205">
+      <c r="G208">
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B206" t="s">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
         <v>317</v>
       </c>
-      <c r="C206" s="7" t="s">
+      <c r="C209" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="D206" s="28">
+      <c r="D209" s="28">
         <v>42775</v>
       </c>
-      <c r="G206">
+      <c r="G209">
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B207" s="7" t="s">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B210" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="G207">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B208" t="s">
+      <c r="G210">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
         <v>309</v>
       </c>
-      <c r="C208" s="7" t="s">
+      <c r="C211" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="D208" s="28">
+      <c r="D211" s="28">
         <v>42775</v>
       </c>
-      <c r="G208">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H209" s="6"/>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B210" s="8" t="s">
+      <c r="G211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H212" s="6"/>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B213" s="8" t="s">
         <v>360</v>
       </c>
-      <c r="H210" s="6"/>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B211" s="7" t="s">
+      <c r="H213" s="6"/>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B214" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="G211">
+      <c r="G214">
         <v>3</v>
       </c>
-      <c r="H211" s="6"/>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B212" s="7" t="s">
+      <c r="H214" s="6"/>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B215" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="G212">
+      <c r="G215">
         <v>3</v>
       </c>
-      <c r="H212" s="6"/>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B213" s="7" t="s">
+      <c r="H215" s="6"/>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B216" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="G213">
+      <c r="G216">
         <v>3</v>
       </c>
-      <c r="H213" s="6"/>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H214" s="6"/>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B215" s="8" t="s">
+      <c r="H216" s="6"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H217" s="6"/>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B218" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C215" s="8"/>
-      <c r="D215" s="8"/>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A216">
-        <v>1</v>
-      </c>
-      <c r="B216" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E216" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A217">
-        <v>2</v>
-      </c>
-      <c r="B217" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E217" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A218">
-        <v>3</v>
-      </c>
-      <c r="B218" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E218" t="s">
-        <v>212</v>
-      </c>
+      <c r="C218" s="8"/>
+      <c r="D218" s="8"/>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219">
+        <v>1</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E219" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>2</v>
+      </c>
+      <c r="B220" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E220" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>3</v>
+      </c>
+      <c r="B221" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E221" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A222">
         <v>4</v>
       </c>
-      <c r="B219" s="7" t="s">
+      <c r="B222" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>176</v>
       </c>
-      <c r="B220" s="7" t="s">
+      <c r="B223" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="E220" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B221" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="E221" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B222" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="E222" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B223" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="E223" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="224" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B224" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E224" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="225" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B225" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E225" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="226" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B226" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E226" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="227" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B227" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E227" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="225" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B225" s="7" t="s">
+    <row r="228" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B228" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E228" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="226" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B226" s="10" t="s">
+    <row r="229" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B229" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C226" s="10"/>
-      <c r="D226" s="10"/>
-    </row>
-    <row r="227" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B227" s="7" t="s">
+      <c r="C229" s="10"/>
+      <c r="D229" s="10"/>
+    </row>
+    <row r="230" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B230" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E230" t="s">
         <v>216</v>
-      </c>
-    </row>
-    <row r="228" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B228" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="229" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B229" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="230" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B230" s="7" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="231" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B231" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="232" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B232" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="233" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B233" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="234" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B234" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="232" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B232" s="7" t="s">
+    <row r="235" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B235" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E232" t="s">
+      <c r="E235" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="233" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B233" s="7" t="s">
+    <row r="236" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B236" s="7" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="234" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B234" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="E234" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="235" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B235" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E235" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="236" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B236" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C236" s="10"/>
-      <c r="D236" s="10"/>
     </row>
     <row r="237" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B237" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E237" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="238" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B238" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="E238" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="239" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B239" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C239" s="10"/>
+      <c r="D239" s="10"/>
+    </row>
+    <row r="240" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B240" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E240" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="238" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B238" s="7" t="s">
+    <row r="241" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B241" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E241" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="239" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B239" s="7" t="s">
+    <row r="242" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B242" s="7" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="240" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B240" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A241">
-        <v>1</v>
-      </c>
-      <c r="B241" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G241">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A242">
-        <v>2</v>
-      </c>
-      <c r="B242" s="7" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B243" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>1</v>
+      </c>
+      <c r="B244" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="G244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>2</v>
+      </c>
+      <c r="B245" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B246" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="G243">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B244" s="7" t="s">
+      <c r="G246">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B247" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="G244">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B245" s="7" t="s">
+      <c r="G247">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B248" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="G245">
+      <c r="G248">
         <v>3</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="7" t="s">
+    <row r="249" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B249" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="G246">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="7" t="s">
+      <c r="G249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B250" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="G247">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E248" s="20"/>
-    </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B249" s="7" t="s">
+      <c r="G250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E251" s="20"/>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B252" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E249" t="s">
+      <c r="E252" t="s">
         <v>221</v>
-      </c>
-      <c r="G249">
-        <v>0</v>
-      </c>
-      <c r="H249" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B250" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E250" t="s">
-        <v>222</v>
-      </c>
-      <c r="G250">
-        <v>0</v>
-      </c>
-      <c r="H250" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B251" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E251" t="s">
-        <v>223</v>
-      </c>
-      <c r="G251">
-        <v>0</v>
-      </c>
-      <c r="H251" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="252" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B252" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="G252">
         <v>0</v>
@@ -5476,7 +5494,10 @@
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B253" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
+      </c>
+      <c r="E253" t="s">
+        <v>222</v>
       </c>
       <c r="G253">
         <v>0</v>
@@ -5487,7 +5508,10 @@
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B254" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
+      </c>
+      <c r="E254" t="s">
+        <v>223</v>
       </c>
       <c r="G254">
         <v>0</v>
@@ -5496,15 +5520,48 @@
         <v>146</v>
       </c>
     </row>
+    <row r="255" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B255" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
+      <c r="H255" t="s">
+        <v>146</v>
+      </c>
+    </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B256" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G256">
+        <v>0</v>
+      </c>
+      <c r="H256" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="257" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B257" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G257">
+        <v>0</v>
+      </c>
+      <c r="H257" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="259" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B259" s="7" t="s">
         <v>220</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:I247">
+  <autoFilter ref="A7:I250">
     <filterColumn colId="5">
-      <filters blank="1">
+      <filters>
         <filter val="Bug"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
no changes, files saved during testing
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -13,14 +13,14 @@
     <sheet name="Actions - Post - Demo1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$I$250</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$I$261</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="387">
   <si>
     <t>Reports</t>
   </si>
@@ -1317,6 +1317,27 @@
   </si>
   <si>
     <t>Devp / Staging / - flag under ICON flag</t>
+  </si>
+  <si>
+    <t>Did not work as a windows Service, decided to use console app.</t>
+  </si>
+  <si>
+    <t>Console App</t>
+  </si>
+  <si>
+    <t>Server Disk free disk space</t>
+  </si>
+  <si>
+    <t>Mongo service - running status</t>
+  </si>
+  <si>
+    <t>Mongo Service - stop / start</t>
+  </si>
+  <si>
+    <t>Indexes</t>
+  </si>
+  <si>
+    <t>Clarity Logo</t>
   </si>
 </sst>
 </file>
@@ -2487,16 +2508,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I259"/>
+  <dimension ref="A1:I263"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B182" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B162" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B190" sqref="B190"/>
+      <selection pane="bottomRight" activeCell="B175" sqref="B175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2581,7 +2602,7 @@
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>2</v>
       </c>
@@ -2607,7 +2628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2637,7 +2658,7 @@
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
@@ -2651,7 +2672,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>2</v>
       </c>
@@ -2671,7 +2692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>2</v>
       </c>
@@ -2705,7 +2726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>2</v>
       </c>
@@ -2718,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>2</v>
       </c>
@@ -2734,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>2</v>
       </c>
@@ -2748,7 +2769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>2</v>
       </c>
@@ -2764,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -2778,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -2795,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>2</v>
       </c>
@@ -2813,7 +2834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
@@ -2854,7 +2875,7 @@
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>2</v>
       </c>
@@ -2867,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>2</v>
       </c>
@@ -2969,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>2</v>
       </c>
@@ -2982,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>2</v>
       </c>
@@ -2995,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>2</v>
       </c>
@@ -3008,7 +3029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>2</v>
       </c>
@@ -3021,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>2</v>
       </c>
@@ -3041,7 +3062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>2</v>
       </c>
@@ -3102,7 +3123,7 @@
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>2</v>
       </c>
@@ -3115,7 +3136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>2</v>
       </c>
@@ -3128,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>2</v>
       </c>
@@ -3141,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>2</v>
       </c>
@@ -3154,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="9" t="s">
         <v>369</v>
@@ -3168,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="9" t="s">
         <v>375</v>
@@ -3208,7 +3229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>2</v>
       </c>
@@ -3219,7 +3240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="12" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>2</v>
       </c>
@@ -3239,7 +3260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="12" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>2</v>
       </c>
@@ -3269,7 +3290,7 @@
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>2</v>
       </c>
@@ -3308,7 +3329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>2</v>
       </c>
@@ -3321,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>2</v>
       </c>
@@ -3334,7 +3355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>2</v>
       </c>
@@ -3347,7 +3368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
         <v>296</v>
       </c>
@@ -3357,7 +3378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>2</v>
       </c>
@@ -3375,7 +3396,7 @@
       </c>
       <c r="H64" s="6"/>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>2</v>
       </c>
@@ -3392,7 +3413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>2</v>
       </c>
@@ -3425,7 +3446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>2</v>
       </c>
@@ -3439,7 +3460,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>2</v>
       </c>
@@ -3455,7 +3476,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>2</v>
       </c>
@@ -3471,7 +3492,7 @@
         <v>42698</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>2</v>
       </c>
@@ -3485,7 +3506,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>2</v>
       </c>
@@ -3497,7 +3518,7 @@
       </c>
       <c r="H72" s="6"/>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>2</v>
       </c>
@@ -3509,7 +3530,7 @@
       </c>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>2</v>
       </c>
@@ -3585,7 +3606,7 @@
       </c>
       <c r="H78" s="6"/>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>2</v>
       </c>
@@ -3597,7 +3618,7 @@
       </c>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>2</v>
       </c>
@@ -3615,7 +3636,7 @@
       </c>
       <c r="H80" s="6"/>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>2</v>
       </c>
@@ -3633,7 +3654,7 @@
       </c>
       <c r="H81" s="6"/>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>2</v>
       </c>
@@ -3651,7 +3672,7 @@
       </c>
       <c r="H82" s="6"/>
     </row>
-    <row r="83" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>2</v>
       </c>
@@ -3707,7 +3728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>2</v>
       </c>
@@ -3718,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>2</v>
       </c>
@@ -3746,7 +3767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>2</v>
       </c>
@@ -3757,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
       <c r="B91" s="7" t="s">
         <v>367</v>
@@ -3769,7 +3790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="7" t="s">
         <v>368</v>
@@ -3794,7 +3815,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>2</v>
       </c>
@@ -3807,7 +3828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>2</v>
       </c>
@@ -3837,7 +3858,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>2</v>
       </c>
@@ -3848,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>2</v>
       </c>
@@ -3899,7 +3920,7 @@
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>2</v>
       </c>
@@ -3910,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>2</v>
       </c>
@@ -3932,7 +3953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
         <v>2</v>
       </c>
@@ -3943,7 +3964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>2</v>
       </c>
@@ -3964,7 +3985,7 @@
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:7" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>2</v>
       </c>
@@ -3984,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
         <v>2</v>
       </c>
@@ -4004,7 +4025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="19" t="s">
         <v>373</v>
       </c>
@@ -4018,7 +4039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
         <v>2</v>
       </c>
@@ -4032,7 +4053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
         <v>2</v>
       </c>
@@ -4158,7 +4179,7 @@
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>2</v>
       </c>
@@ -4169,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
         <v>2</v>
       </c>
@@ -4205,7 +4226,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
         <v>2</v>
       </c>
@@ -4233,7 +4254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
         <v>2</v>
       </c>
@@ -4269,7 +4290,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>2</v>
       </c>
@@ -4300,7 +4321,7 @@
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
         <v>2</v>
       </c>
@@ -4311,7 +4332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
         <v>2</v>
       </c>
@@ -4379,7 +4400,7 @@
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
         <v>1</v>
       </c>
@@ -4392,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
         <v>1</v>
       </c>
@@ -4405,7 +4426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
         <v>1</v>
       </c>
@@ -4416,7 +4437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
         <v>1</v>
       </c>
@@ -4427,7 +4448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
         <v>1</v>
       </c>
@@ -4463,7 +4484,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
         <v>1</v>
       </c>
@@ -4474,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>1</v>
       </c>
@@ -4491,7 +4512,7 @@
         <v>42702</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="12" t="s">
         <v>1</v>
       </c>
@@ -4503,7 +4524,7 @@
       </c>
       <c r="H156" s="6"/>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
         <v>1</v>
       </c>
@@ -4518,7 +4539,7 @@
       </c>
       <c r="H157" s="6"/>
     </row>
-    <row r="158" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12" t="s">
         <v>1</v>
       </c>
@@ -4531,7 +4552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12" t="s">
         <v>1</v>
       </c>
@@ -4547,7 +4568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
         <v>1</v>
       </c>
@@ -4563,7 +4584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
         <v>1</v>
       </c>
@@ -4577,7 +4598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12" t="s">
         <v>1</v>
       </c>
@@ -4590,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>1</v>
       </c>
@@ -4601,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
         <v>1</v>
       </c>
@@ -4662,7 +4683,7 @@
       </c>
       <c r="H167" s="14"/>
     </row>
-    <row r="168" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
         <v>1</v>
       </c>
@@ -4825,7 +4846,7 @@
       </c>
       <c r="H180" s="6"/>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>337</v>
       </c>
@@ -4894,218 +4915,178 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="12"/>
-      <c r="B187" s="7" t="s">
-        <v>359</v>
-      </c>
       <c r="H187" s="6"/>
     </row>
-    <row r="188" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B188" s="17" t="s">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A188" s="12"/>
+      <c r="B188" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="H188" s="6"/>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A189" s="12"/>
+      <c r="B189" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="H189" s="6"/>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A190" s="12"/>
+      <c r="B190" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="H190" s="6"/>
+    </row>
+    <row r="191" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B191" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="H188" s="6"/>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B189" s="15" t="s">
+      <c r="H191" s="6"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B192" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="H189" s="6"/>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B190" s="7" t="s">
+      <c r="H192" s="6"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B193" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="G190">
-        <v>2</v>
-      </c>
-      <c r="H190" s="6"/>
-    </row>
-    <row r="191" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="B191" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="C191" s="15"/>
-      <c r="D191" s="15"/>
-      <c r="H191" s="14"/>
-    </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="B192" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="E192" t="s">
-        <v>135</v>
-      </c>
-      <c r="G192">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="12" t="s">
-        <v>319</v>
-      </c>
-      <c r="B193" s="7" t="s">
-        <v>332</v>
-      </c>
       <c r="G193">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H193" s="6"/>
+    </row>
+    <row r="194" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="B194" s="7" t="s">
-        <v>333</v>
-      </c>
-      <c r="G194">
-        <v>2</v>
-      </c>
+      <c r="B194" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C194" s="15"/>
+      <c r="D194" s="15"/>
+      <c r="H194" s="14"/>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
         <v>319</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>257</v>
+        <v>136</v>
+      </c>
+      <c r="E195" t="s">
+        <v>135</v>
       </c>
       <c r="G195">
-        <v>2</v>
-      </c>
-      <c r="H195" s="6"/>
-    </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
         <v>319</v>
       </c>
       <c r="B196" s="7" t="s">
-        <v>122</v>
+        <v>332</v>
       </c>
       <c r="G196">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I196" t="s">
-        <v>146</v>
+        <v>380</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="12"/>
       <c r="B197" s="7" t="s">
-        <v>350</v>
+        <v>381</v>
       </c>
       <c r="G197">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B198" s="8" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="B198" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="G199">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H199" s="6"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="E200" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G200">
         <v>0</v>
-      </c>
-      <c r="H200" s="6">
-        <v>42702</v>
       </c>
       <c r="I200" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="12" t="s">
-        <v>301</v>
-      </c>
-      <c r="B201" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C201" s="9"/>
-      <c r="D201" s="9"/>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" s="12"/>
+      <c r="B201" s="7" t="s">
+        <v>350</v>
+      </c>
       <c r="G201">
-        <v>0</v>
-      </c>
-      <c r="H201" s="6">
-        <v>42702</v>
-      </c>
-      <c r="I201" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="B202" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E202" t="s">
-        <v>135</v>
-      </c>
-      <c r="G202">
-        <v>0</v>
-      </c>
-      <c r="H202" s="6">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B202" s="8" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
         <v>301</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E203" t="s">
-        <v>137</v>
+        <v>302</v>
       </c>
       <c r="G203">
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
         <v>301</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E204" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G204">
         <v>0</v>
       </c>
       <c r="H204" s="6">
-        <v>42697</v>
+        <v>42702</v>
       </c>
       <c r="I204" t="s">
         <v>146</v>
@@ -5115,425 +5096,460 @@
       <c r="A205" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="B205" s="7" t="s">
+      <c r="B205" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="C205" s="9"/>
+      <c r="D205" s="9"/>
+      <c r="G205">
+        <v>0</v>
+      </c>
+      <c r="H205" s="6">
+        <v>42702</v>
+      </c>
+      <c r="I205" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B206" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E206" t="s">
+        <v>135</v>
+      </c>
+      <c r="G206">
+        <v>0</v>
+      </c>
+      <c r="H206" s="6">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E207" t="s">
+        <v>137</v>
+      </c>
+      <c r="G207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E208" t="s">
+        <v>137</v>
+      </c>
+      <c r="G208">
+        <v>0</v>
+      </c>
+      <c r="H208" s="6">
+        <v>42697</v>
+      </c>
+      <c r="I208" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A209" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="B209" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="G205">
-        <v>2</v>
-      </c>
-      <c r="H205" s="6"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A206" s="12"/>
-      <c r="B206" s="13" t="s">
+      <c r="G209">
+        <v>2</v>
+      </c>
+      <c r="H209" s="6"/>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A210" s="12"/>
+      <c r="B210" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="H206" s="6"/>
-    </row>
-    <row r="207" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B207" s="17" t="s">
+      <c r="G210">
+        <v>9</v>
+      </c>
+      <c r="H210" s="6"/>
+    </row>
+    <row r="211" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="B211" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C207" s="17"/>
-      <c r="D207" s="17"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B208" s="8" t="s">
+      <c r="C211" s="17"/>
+      <c r="D211" s="17"/>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B212" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="G208">
+      <c r="G212">
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
         <v>317</v>
       </c>
-      <c r="C209" s="7" t="s">
+      <c r="C213" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="D209" s="28">
+      <c r="D213" s="28">
         <v>42775</v>
       </c>
-      <c r="G209">
+      <c r="G213">
         <v>1</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B210" s="7" t="s">
-        <v>351</v>
-      </c>
-      <c r="G210">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B211" t="s">
-        <v>309</v>
-      </c>
-      <c r="C211" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="D211" s="28">
-        <v>42775</v>
-      </c>
-      <c r="G211">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H212" s="6"/>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B213" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="H213" s="6"/>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B214" s="7" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="G214">
-        <v>3</v>
-      </c>
-      <c r="H214" s="6"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B215" s="7" t="s">
-        <v>362</v>
+      <c r="B215" t="s">
+        <v>309</v>
+      </c>
+      <c r="C215" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="D215" s="28">
+        <v>42775</v>
       </c>
       <c r="G215">
-        <v>3</v>
-      </c>
-      <c r="H215" s="6"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B216" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="G216">
+        <v>1</v>
+      </c>
+      <c r="H216" s="6"/>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B217" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="H217" s="6"/>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B218" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="G218">
+        <v>3</v>
+      </c>
+      <c r="H218" s="6"/>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B219" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="G219">
+        <v>3</v>
+      </c>
+      <c r="H219" s="6"/>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B220" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="G216">
+      <c r="G220">
         <v>3</v>
       </c>
-      <c r="H216" s="6"/>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H217" s="6"/>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B218" s="8" t="s">
+      <c r="H220" s="6"/>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B221" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="H221" s="6"/>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B222" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="H222" s="6"/>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B223" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="C218" s="8"/>
-      <c r="D218" s="8"/>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A219">
+      <c r="C223" s="8"/>
+      <c r="D223" s="8"/>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A224">
         <v>1</v>
       </c>
-      <c r="B219" s="7" t="s">
+      <c r="B224" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="E219" t="s">
+      <c r="E224" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="220" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A220">
-        <v>2</v>
-      </c>
-      <c r="B220" s="7" t="s">
+    <row r="225" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>2</v>
+      </c>
+      <c r="B225" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="E220" t="s">
+      <c r="E225" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A221">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226">
         <v>3</v>
       </c>
-      <c r="B221" s="7" t="s">
+      <c r="B226" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E221" t="s">
+      <c r="E226" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A222">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227">
         <v>4</v>
       </c>
-      <c r="B222" s="7" t="s">
+      <c r="B227" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>176</v>
       </c>
-      <c r="B223" s="7" t="s">
+      <c r="B228" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E223" t="s">
+      <c r="E228" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B224" s="7" t="s">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B229" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="E224" t="s">
+      <c r="E229" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="225" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B225" s="7" t="s">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B230" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="E225" t="s">
+      <c r="E230" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="226" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B226" s="7" t="s">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B231" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="E226" t="s">
+      <c r="E231" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="227" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B227" s="7" t="s">
+    <row r="232" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B232" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="E227" t="s">
+      <c r="E232" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="228" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B228" s="7" t="s">
+    <row r="233" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B233" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="E228" t="s">
+      <c r="E233" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="229" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B229" s="10" t="s">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B234" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="C229" s="10"/>
-      <c r="D229" s="10"/>
-    </row>
-    <row r="230" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B230" s="7" t="s">
+      <c r="C234" s="10"/>
+      <c r="D234" s="10"/>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B235" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="E230" t="s">
+      <c r="E235" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="231" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B231" s="7" t="s">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B236" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="232" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B232" s="7" t="s">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B237" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="233" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B233" s="7" t="s">
+    <row r="238" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B238" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="234" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B234" s="7" t="s">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B239" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="235" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B235" s="7" t="s">
+    <row r="240" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B240" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E235" t="s">
+      <c r="E240" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="236" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B236" s="7" t="s">
+    <row r="241" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B241" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="237" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B237" s="7" t="s">
+    <row r="242" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B242" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E242" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="238" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B238" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="E238" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="239" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B239" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C239" s="10"/>
-      <c r="D239" s="10"/>
-    </row>
-    <row r="240" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B240" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="E240" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="241" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B241" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="E241" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="242" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B242" s="7" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B243" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A244">
-        <v>1</v>
-      </c>
-      <c r="B244" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="G244">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A245">
-        <v>2</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="E243" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B244" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C244" s="10"/>
+      <c r="D244" s="10"/>
+    </row>
+    <row r="245" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B245" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="E245" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B246" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="G246">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="E246" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B247" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="G247">
-        <v>2</v>
+        <v>188</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B248" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="G248">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="249" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>1</v>
+      </c>
       <c r="B249" s="7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="G249">
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>2</v>
+      </c>
       <c r="B250" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="G250">
-        <v>0</v>
+        <v>199</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E251" s="20"/>
+      <c r="B251" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="G251">
+        <v>2</v>
+      </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B252" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E252" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="G252">
-        <v>0</v>
-      </c>
-      <c r="H252" t="s">
-        <v>146</v>
+        <v>2</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B253" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E253" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="G253">
-        <v>0</v>
-      </c>
-      <c r="H253" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B254" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="E254" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="G254">
         <v>0</v>
       </c>
-      <c r="H254" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="255" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B255" s="7" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="G255">
         <v>0</v>
-      </c>
-      <c r="H255" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B256" s="7" t="s">
-        <v>208</v>
+        <v>204</v>
+      </c>
+      <c r="E256" t="s">
+        <v>221</v>
       </c>
       <c r="G256">
         <v>0</v>
@@ -5544,7 +5560,10 @@
     </row>
     <row r="257" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B257" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
+      </c>
+      <c r="E257" t="s">
+        <v>222</v>
       </c>
       <c r="G257">
         <v>0</v>
@@ -5553,26 +5572,60 @@
         <v>146</v>
       </c>
     </row>
-    <row r="259" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B258" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E258" t="s">
+        <v>223</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
+      <c r="H258" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="259" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B259" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G259">
+        <v>0</v>
+      </c>
+      <c r="H259" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="260" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B260" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G260">
+        <v>0</v>
+      </c>
+      <c r="H260" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="261" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B261" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G261">
+        <v>0</v>
+      </c>
+      <c r="H261" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="263" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B263" s="7" t="s">
         <v>220</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:I250">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="Bug"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="6">
-      <filters blank="1">
-        <filter val="1"/>
-        <filter val="2"/>
-        <filter val="3"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A7:I261"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
WebSite changes - Findings section
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -13,14 +13,14 @@
     <sheet name="Actions - Post - Demo1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$I$266</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$I$269</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="395">
   <si>
     <t>Reports</t>
   </si>
@@ -1350,6 +1350,18 @@
   </si>
   <si>
     <t>Country Specific sites</t>
+  </si>
+  <si>
+    <t>DateOfInspection - lable for DB/Live Site</t>
+  </si>
+  <si>
+    <t>DateOfInspection - Date picker for Manual Sites</t>
+  </si>
+  <si>
+    <t>Clarity/ check with ICON</t>
+  </si>
+  <si>
+    <t>Is An Issue - set default true - reason: Findings is always / most of the time is an Issue.</t>
   </si>
 </sst>
 </file>
@@ -2520,16 +2532,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I268"/>
+  <dimension ref="A1:I271"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B85" sqref="B85"/>
+      <selection pane="bottomRight" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,7 +2626,7 @@
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>2</v>
       </c>
@@ -2627,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
@@ -2640,7 +2652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="12" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>2</v>
       </c>
@@ -2670,7 +2682,7 @@
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>2</v>
       </c>
@@ -2684,7 +2696,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>2</v>
       </c>
@@ -2704,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>2</v>
       </c>
@@ -2727,7 +2739,7 @@
         <v>42767</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>2</v>
       </c>
@@ -2738,7 +2750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>2</v>
       </c>
@@ -2751,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>2</v>
       </c>
@@ -2767,7 +2779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>2</v>
       </c>
@@ -2781,7 +2793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>2</v>
       </c>
@@ -2797,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>2</v>
       </c>
@@ -2811,7 +2823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>2</v>
       </c>
@@ -2828,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>2</v>
       </c>
@@ -2846,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>2</v>
       </c>
@@ -2866,7 +2878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="21" t="s">
         <v>354</v>
@@ -2887,7 +2899,7 @@
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>2</v>
       </c>
@@ -2900,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>2</v>
       </c>
@@ -2913,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>2</v>
       </c>
@@ -2926,7 +2938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>2</v>
       </c>
@@ -2952,7 +2964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>2</v>
       </c>
@@ -2965,7 +2977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="9" t="s">
         <v>370</v>
@@ -3002,7 +3014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>2</v>
       </c>
@@ -3015,7 +3027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>2</v>
       </c>
@@ -3028,7 +3040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>2</v>
       </c>
@@ -3041,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>2</v>
       </c>
@@ -3054,7 +3066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>2</v>
       </c>
@@ -3074,7 +3086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>2</v>
       </c>
@@ -3135,7 +3147,7 @@
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>2</v>
       </c>
@@ -3148,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>2</v>
       </c>
@@ -3161,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>2</v>
       </c>
@@ -3174,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>2</v>
       </c>
@@ -3187,7 +3199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="12"/>
       <c r="B49" s="9" t="s">
         <v>368</v>
@@ -3201,7 +3213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="9" t="s">
         <v>374</v>
@@ -3228,7 +3240,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>2</v>
       </c>
@@ -3241,7 +3253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>2</v>
       </c>
@@ -3252,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="12" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>2</v>
       </c>
@@ -3272,7 +3284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="12" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" s="12" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>2</v>
       </c>
@@ -3302,7 +3314,7 @@
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>2</v>
       </c>
@@ -3315,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>2</v>
       </c>
@@ -3328,7 +3340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>2</v>
       </c>
@@ -3341,7 +3353,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>2</v>
       </c>
@@ -3354,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>2</v>
       </c>
@@ -3367,7 +3379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>2</v>
       </c>
@@ -3380,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
         <v>295</v>
       </c>
@@ -3390,7 +3402,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>2</v>
       </c>
@@ -3408,7 +3420,7 @@
       </c>
       <c r="H64" s="6"/>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>2</v>
       </c>
@@ -3425,7 +3437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>2</v>
       </c>
@@ -3458,7 +3470,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>2</v>
       </c>
@@ -3472,7 +3484,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>2</v>
       </c>
@@ -3488,7 +3500,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>2</v>
       </c>
@@ -3504,7 +3516,7 @@
         <v>42698</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>2</v>
       </c>
@@ -3518,7 +3530,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>2</v>
       </c>
@@ -3530,7 +3542,7 @@
       </c>
       <c r="H72" s="6"/>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>2</v>
       </c>
@@ -3542,7 +3554,7 @@
       </c>
       <c r="H73" s="6"/>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>2</v>
       </c>
@@ -3554,7 +3566,7 @@
       </c>
       <c r="H74" s="6"/>
     </row>
-    <row r="75" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>2</v>
       </c>
@@ -3571,7 +3583,7 @@
       </c>
       <c r="H75" s="27"/>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>2</v>
       </c>
@@ -3586,7 +3598,7 @@
       </c>
       <c r="H76" s="6"/>
     </row>
-    <row r="77" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>2</v>
       </c>
@@ -3603,7 +3615,7 @@
       </c>
       <c r="H77" s="14"/>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>2</v>
       </c>
@@ -3618,7 +3630,7 @@
       </c>
       <c r="H78" s="6"/>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>2</v>
       </c>
@@ -3630,7 +3642,7 @@
       </c>
       <c r="H79" s="6"/>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>2</v>
       </c>
@@ -3648,7 +3660,7 @@
       </c>
       <c r="H80" s="6"/>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>2</v>
       </c>
@@ -3666,7 +3678,7 @@
       </c>
       <c r="H81" s="6"/>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>2</v>
       </c>
@@ -3684,7 +3696,7 @@
       </c>
       <c r="H82" s="6"/>
     </row>
-    <row r="83" spans="1:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>2</v>
       </c>
@@ -3703,155 +3715,161 @@
       </c>
       <c r="H83" s="6"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
-      <c r="B84" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="D84" s="28"/>
+      <c r="B84" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="D84" s="28">
+        <v>42818</v>
+      </c>
+      <c r="E84" t="s">
+        <v>139</v>
+      </c>
       <c r="F84" s="7"/>
       <c r="G84" s="12"/>
       <c r="H84" s="6"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="D85" s="28">
+        <v>42818</v>
+      </c>
+      <c r="E85" t="s">
+        <v>139</v>
+      </c>
+      <c r="F85" s="7"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="6"/>
+    </row>
+    <row r="86" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="12"/>
+      <c r="B86" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="D86" s="28"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="6"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="12"/>
+      <c r="B87" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="D87" s="28"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="6"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="12"/>
+      <c r="B88" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="D85" s="28"/>
-      <c r="F85" s="7" t="s">
+      <c r="D88" s="28"/>
+      <c r="F88" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="G85" s="12">
+      <c r="G88" s="12">
         <v>1</v>
       </c>
-      <c r="H85" s="6"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="8" t="s">
+      <c r="H88" s="6"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="8" t="s">
         <v>365</v>
       </c>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="G86" t="s">
+      <c r="C89" s="8"/>
+      <c r="D89" s="8"/>
+      <c r="G89" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B87" s="7" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="G87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B88" s="22" t="s">
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C91" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="D88" s="20">
+      <c r="D91" s="20">
         <v>42760</v>
       </c>
-      <c r="G88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B89" s="7" t="s">
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="G89">
+      <c r="G92">
         <v>3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="G90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="12"/>
-      <c r="B91" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="F91" t="s">
-        <v>369</v>
-      </c>
-      <c r="G91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
-      <c r="B92" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="F92" t="s">
-        <v>321</v>
-      </c>
-      <c r="G92">
-        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="G93" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="C94" s="9"/>
-      <c r="D94" s="9"/>
+      <c r="B93" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="12"/>
+      <c r="B94" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="F94" t="s">
+        <v>369</v>
+      </c>
       <c r="G94">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95" s="25" t="s">
-        <v>319</v>
-      </c>
-      <c r="C95" s="20" t="s">
-        <v>288</v>
-      </c>
-      <c r="D95" s="20">
-        <v>42760</v>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="12"/>
+      <c r="B95" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="F95" t="s">
+        <v>321</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -3861,32 +3879,34 @@
       <c r="A96" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B96" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="C96" s="9"/>
-      <c r="D96" s="9"/>
+      <c r="B96" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C96" s="8"/>
+      <c r="D96" s="8"/>
       <c r="G96" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B97" s="7" t="s">
-        <v>237</v>
-      </c>
+      <c r="B97" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
       <c r="G97">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B98" s="21" t="s">
-        <v>283</v>
+      <c r="B98" s="25" t="s">
+        <v>319</v>
       </c>
       <c r="C98" s="20" t="s">
         <v>288</v>
@@ -3898,90 +3918,98 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="12"/>
-      <c r="B99" s="21" t="s">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="G99" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A101" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="C101" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D101" s="20">
+        <v>42760</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="12"/>
+      <c r="B102" s="21" t="s">
         <v>345</v>
       </c>
-      <c r="C99" s="20"/>
-      <c r="D99" s="20"/>
-    </row>
-    <row r="100" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="12"/>
-      <c r="B100" s="21" t="s">
+      <c r="C102" s="20"/>
+      <c r="D102" s="20"/>
+    </row>
+    <row r="103" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A103" s="12"/>
+      <c r="B103" s="21" t="s">
         <v>343</v>
       </c>
-      <c r="C100" s="20"/>
-      <c r="D100" s="20"/>
-    </row>
-    <row r="101" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A101" s="12"/>
-      <c r="B101" s="21" t="s">
+      <c r="C103" s="20"/>
+      <c r="D103" s="20"/>
+    </row>
+    <row r="104" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A104" s="12"/>
+      <c r="B104" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="C101" s="20"/>
-      <c r="D101" s="20"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B102" s="8" t="s">
+      <c r="C104" s="20"/>
+      <c r="D104" s="20"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
-    </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" s="7" t="s">
+      <c r="C105" s="8"/>
+      <c r="D105" s="8"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="G103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B104" s="7" t="s">
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="7" t="s">
         <v>243</v>
-      </c>
-      <c r="G104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="G105">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="G106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>223</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -3991,104 +4019,97 @@
       <c r="A108" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B108" s="8" t="s">
+      <c r="B108" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="G108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C108" s="8"/>
-      <c r="D108" s="8"/>
-    </row>
-    <row r="109" spans="1:7" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" s="23" t="s">
+      <c r="C111" s="8"/>
+      <c r="D111" s="8"/>
+    </row>
+    <row r="112" spans="1:7" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="23" t="s">
         <v>280</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C112" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D109" s="20">
+      <c r="D112" s="20">
         <v>42760</v>
       </c>
-      <c r="E109" s="12" t="s">
+      <c r="E112" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="G109" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B110" s="24" t="s">
+      <c r="G112" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A113" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" s="24" t="s">
         <v>293</v>
       </c>
-      <c r="C110" s="13" t="s">
+      <c r="C113" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D110" s="20">
+      <c r="D113" s="20">
         <v>42760</v>
       </c>
-      <c r="E110" s="20" t="s">
+      <c r="E113" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="G110" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="19" t="s">
+      <c r="G113" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="19" t="s">
         <v>372</v>
       </c>
-      <c r="C111" s="13"/>
-      <c r="D111" s="20"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="12" t="s">
+      <c r="C114" s="13"/>
+      <c r="D114" s="20"/>
+      <c r="E114" s="20"/>
+      <c r="F114" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="G111" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E112" t="s">
-        <v>139</v>
-      </c>
-      <c r="G112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C113" s="9"/>
-      <c r="D113" s="9"/>
-      <c r="G113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="C114" s="9"/>
-      <c r="D114" s="9"/>
-      <c r="G114">
-        <v>3</v>
+      <c r="G114" s="12">
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -4096,58 +4117,62 @@
         <v>2</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>387</v>
+        <v>138</v>
       </c>
       <c r="E115" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="G115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="12"/>
-      <c r="B116" s="7" t="s">
-        <v>386</v>
-      </c>
+      <c r="A116" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
       <c r="G116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B117" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E117" t="s">
-        <v>139</v>
-      </c>
+      <c r="B117" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
       <c r="G117">
         <v>3</v>
       </c>
-      <c r="H117" s="6">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>120</v>
+        <v>387</v>
+      </c>
+      <c r="E118" t="s">
+        <v>134</v>
       </c>
       <c r="G118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="12" t="s">
-        <v>2</v>
-      </c>
+      <c r="A119" s="12"/>
       <c r="B119" s="7" t="s">
-        <v>123</v>
+        <v>386</v>
+      </c>
+      <c r="G119">
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -4155,7 +4180,16 @@
         <v>2</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>124</v>
+        <v>119</v>
+      </c>
+      <c r="E120" t="s">
+        <v>139</v>
+      </c>
+      <c r="G120">
+        <v>3</v>
+      </c>
+      <c r="H120" s="6">
+        <v>42702</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -4163,7 +4197,10 @@
         <v>2</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -4171,7 +4208,7 @@
         <v>2</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -4179,7 +4216,7 @@
         <v>2</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -4187,572 +4224,551 @@
         <v>2</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B125" s="8" t="s">
+      <c r="B125" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A127" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
-    </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B126" s="7" t="s">
+      <c r="C128" s="8"/>
+      <c r="D128" s="8"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="G126">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B127" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="G127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B128" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="G128">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A129" s="12"/>
-      <c r="B129" s="7" t="s">
-        <v>378</v>
+      <c r="G129">
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B130" s="8" t="s">
+      <c r="B130" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="G131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="12"/>
+      <c r="B132" s="7" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B133" s="8" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B131" t="s">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B134" t="s">
         <v>305</v>
       </c>
-      <c r="C131" s="7" t="s">
+      <c r="C134" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="D131" s="28">
+      <c r="D134" s="28">
         <v>42775</v>
       </c>
-      <c r="G131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B132" t="s">
-        <v>307</v>
-      </c>
-      <c r="G132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B133" t="s">
-        <v>317</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="D133" s="28">
-        <v>42775</v>
-      </c>
-      <c r="G133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>132</v>
-      </c>
       <c r="G134">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B135" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>307</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B136" s="7" t="s">
-        <v>167</v>
+      <c r="B136" t="s">
+        <v>317</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D136" s="28">
+        <v>42775</v>
       </c>
       <c r="G136">
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B137" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="D137" s="17"/>
+      <c r="B137" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G137">
+        <v>3</v>
+      </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B138" s="8" t="s">
+      <c r="B138" s="7" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A140" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="D140" s="17"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="D138" s="8"/>
-    </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B139" s="9" t="s">
+      <c r="D141" s="8"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B142" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="G139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="G140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="12"/>
-      <c r="B141" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="G141">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A142" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B142" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D142" s="17"/>
+      <c r="G142">
+        <v>0</v>
+      </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B143" s="8" t="s">
-        <v>325</v>
+        <v>2</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="12" t="s">
-        <v>1</v>
-      </c>
+      <c r="A144" s="12"/>
       <c r="B144" s="9" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A145" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B145" s="8" t="s">
+      <c r="B145" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D145" s="17"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B146" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B148" s="8" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A146" s="12"/>
-      <c r="B146" s="9" t="s">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="12"/>
+      <c r="B149" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="C146" s="7" t="s">
+      <c r="C149" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="D146" s="28">
+      <c r="D149" s="28">
         <v>42809</v>
       </c>
-      <c r="G146">
+      <c r="G149">
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A147" s="12"/>
-      <c r="B147" s="9" t="s">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="12"/>
+      <c r="B150" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="C147" s="7" t="s">
+      <c r="C150" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="D147" s="28">
+      <c r="D150" s="28">
         <v>42809</v>
       </c>
-      <c r="G147">
+      <c r="G150">
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A148" s="12"/>
-      <c r="B148" s="9" t="s">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="12"/>
+      <c r="B151" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="D148" s="28">
+      <c r="D151" s="28">
         <v>42809</v>
       </c>
-      <c r="G148">
+      <c r="G151">
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A149" s="12"/>
-      <c r="B149" s="9"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A150" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B150" s="8" t="s">
-        <v>251</v>
-      </c>
-      <c r="C150" s="8"/>
-    </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B151" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="C151" s="9"/>
-      <c r="D151" s="9"/>
-      <c r="G151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B152" s="9" t="s">
-        <v>253</v>
-      </c>
-      <c r="C152" s="9"/>
-      <c r="D152" s="9"/>
-      <c r="G152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="12"/>
+      <c r="B152" s="9"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B153" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="G153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B153" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C153" s="8"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B154" s="7" t="s">
-        <v>240</v>
-      </c>
+      <c r="B154" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
       <c r="G154">
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B155" s="7" t="s">
-        <v>234</v>
-      </c>
+      <c r="B155" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
       <c r="G155">
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" s="12"/>
-      <c r="B156" s="10" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A157" s="12"/>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="12" t="s">
+        <v>1</v>
+      </c>
       <c r="B157" s="7" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B158" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="C158" s="8"/>
-      <c r="D158" s="8"/>
-      <c r="G158" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B159" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="G159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="12" t="s">
-        <v>1</v>
-      </c>
+      <c r="B158" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="12"/>
+      <c r="B159" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="12"/>
       <c r="B160" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="E160" t="s">
-        <v>139</v>
-      </c>
-      <c r="G160">
-        <v>0</v>
-      </c>
-      <c r="H160" s="6">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B161" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="G161">
-        <v>0</v>
-      </c>
-      <c r="H161" s="6"/>
-    </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="C161" s="8"/>
+      <c r="D161" s="8"/>
+      <c r="G161" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>228</v>
-      </c>
-      <c r="F162" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="G162">
         <v>0</v>
       </c>
-      <c r="H162" s="6"/>
-    </row>
-    <row r="163" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B163" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C163" s="13"/>
-      <c r="D163" s="13"/>
-      <c r="G163" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B163" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E163" t="s">
+        <v>139</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
+      <c r="H163" s="6">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B164" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="C164" s="13"/>
-      <c r="D164" s="13"/>
-      <c r="F164" t="s">
-        <v>139</v>
-      </c>
-      <c r="G164" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B164" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164" s="6"/>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B165" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C165" s="13"/>
-      <c r="D165" s="13"/>
+      <c r="B165" s="7" t="s">
+        <v>228</v>
+      </c>
       <c r="F165" t="s">
         <v>139</v>
       </c>
-      <c r="G165" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="H165" s="6"/>
+    </row>
+    <row r="166" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B166" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="F166" t="s">
-        <v>139</v>
-      </c>
-      <c r="G166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B166" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C166" s="13"/>
+      <c r="D166" s="13"/>
+      <c r="G166" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>122</v>
+        <v>255</v>
       </c>
       <c r="C167" s="13"/>
       <c r="D167" s="13"/>
+      <c r="F167" t="s">
+        <v>139</v>
+      </c>
       <c r="G167" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B168" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="G168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C168" s="13"/>
+      <c r="D168" s="13"/>
+      <c r="F168" t="s">
+        <v>139</v>
+      </c>
+      <c r="G168" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B169" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C169" s="13"/>
-      <c r="D169" s="13"/>
-      <c r="E169" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G169" s="12">
-        <v>0</v>
-      </c>
-      <c r="H169" s="14">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B169" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="F169" t="s">
+        <v>139</v>
+      </c>
+      <c r="G169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="12" t="s">
+        <v>1</v>
+      </c>
       <c r="B170" s="13" t="s">
-        <v>347</v>
+        <v>122</v>
       </c>
       <c r="C170" s="13"/>
       <c r="D170" s="13"/>
       <c r="G170" s="12">
-        <v>2</v>
-      </c>
-      <c r="H170" s="14"/>
-    </row>
-    <row r="171" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B171" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="C171" s="15"/>
-      <c r="D171" s="15"/>
-      <c r="E171" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G171" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H171" s="14"/>
-    </row>
-    <row r="172" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B171" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B172" s="19" t="s">
-        <v>296</v>
-      </c>
-      <c r="C172" s="15"/>
-      <c r="D172" s="15"/>
+      <c r="B172" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C172" s="13"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="12" t="s">
+        <v>134</v>
+      </c>
       <c r="G172" s="12">
-        <v>2</v>
-      </c>
-      <c r="H172" s="14"/>
-    </row>
-    <row r="173" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B173" s="19" t="s">
-        <v>348</v>
-      </c>
-      <c r="C173" s="15"/>
-      <c r="D173" s="15"/>
+        <v>0</v>
+      </c>
+      <c r="H172" s="14">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B173" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C173" s="13"/>
+      <c r="D173" s="13"/>
       <c r="G173" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H173" s="14"/>
     </row>
@@ -4760,41 +4776,44 @@
       <c r="A174" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B174" s="19" t="s">
-        <v>327</v>
+      <c r="B174" s="15" t="s">
+        <v>260</v>
       </c>
       <c r="C174" s="15"/>
       <c r="D174" s="15"/>
+      <c r="E174" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G174" s="12" t="s">
+        <v>41</v>
+      </c>
       <c r="H174" s="14"/>
     </row>
-    <row r="175" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B175" s="15" t="s">
-        <v>262</v>
+      <c r="B175" s="19" t="s">
+        <v>296</v>
       </c>
       <c r="C175" s="15"/>
       <c r="D175" s="15"/>
-      <c r="E175" s="12" t="s">
-        <v>134</v>
-      </c>
       <c r="G175" s="12">
         <v>2</v>
       </c>
       <c r="H175" s="14"/>
     </row>
-    <row r="176" spans="1:8" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B176" s="19" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="C176" s="15"/>
       <c r="D176" s="15"/>
       <c r="G176" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H176" s="14"/>
     </row>
@@ -4802,8 +4821,8 @@
       <c r="A177" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B177" s="15" t="s">
-        <v>328</v>
+      <c r="B177" s="19" t="s">
+        <v>327</v>
       </c>
       <c r="C177" s="15"/>
       <c r="D177" s="15"/>
@@ -4814,840 +4833,843 @@
         <v>1</v>
       </c>
       <c r="B178" s="15" t="s">
-        <v>329</v>
+        <v>262</v>
       </c>
       <c r="C178" s="15"/>
       <c r="D178" s="15"/>
+      <c r="E178" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G178" s="12">
+        <v>2</v>
+      </c>
       <c r="H178" s="14"/>
     </row>
     <row r="179" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B179" s="15" t="s">
-        <v>272</v>
+      <c r="B179" s="19" t="s">
+        <v>330</v>
       </c>
       <c r="C179" s="15"/>
       <c r="D179" s="15"/>
+      <c r="G179" s="12">
+        <v>2</v>
+      </c>
       <c r="H179" s="14"/>
     </row>
-    <row r="180" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B180" s="18" t="s">
+      <c r="B180" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="C180" s="15"/>
+      <c r="D180" s="15"/>
+      <c r="H180" s="14"/>
+    </row>
+    <row r="181" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B181" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="C181" s="15"/>
+      <c r="D181" s="15"/>
+      <c r="H181" s="14"/>
+    </row>
+    <row r="182" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B182" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C182" s="15"/>
+      <c r="D182" s="15"/>
+      <c r="H182" s="14"/>
+    </row>
+    <row r="183" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B183" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C180" s="18"/>
-      <c r="D180" s="18"/>
-      <c r="E180" s="3" t="s">
+      <c r="C183" s="18"/>
+      <c r="D183" s="18"/>
+      <c r="E183" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="G180" s="3">
+      <c r="G183" s="3">
         <v>3</v>
       </c>
-      <c r="H180" s="27"/>
-    </row>
-    <row r="181" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A181" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="B181" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="H181" s="6"/>
-    </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="B182" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="G182">
-        <v>3</v>
-      </c>
-      <c r="H182" s="6"/>
-    </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="12" t="s">
-        <v>336</v>
-      </c>
-      <c r="B183" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="G183">
-        <v>3</v>
-      </c>
-      <c r="H183" s="6"/>
-    </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H183" s="27"/>
+    </row>
+    <row r="184" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A184" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="B184" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="G184">
-        <v>3</v>
+      <c r="B184" s="17" t="s">
+        <v>322</v>
       </c>
       <c r="H184" s="6"/>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
         <v>336</v>
       </c>
       <c r="B185" s="7" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="G185">
         <v>3</v>
       </c>
       <c r="H185" s="6"/>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
         <v>336</v>
       </c>
       <c r="B186" s="7" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="G186">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H186" s="6"/>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>336</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="G187">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H187" s="6"/>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
         <v>336</v>
       </c>
       <c r="B188" s="7" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="G188">
         <v>3</v>
       </c>
       <c r="H188" s="6"/>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
         <v>336</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="G189">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H189" s="6"/>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
         <v>336</v>
       </c>
       <c r="B190" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="G190">
+        <v>2</v>
+      </c>
+      <c r="H190" s="6"/>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A191" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="G191">
+        <v>3</v>
+      </c>
+      <c r="H191" s="6"/>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A192" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B192" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="G192">
+        <v>3</v>
+      </c>
+      <c r="H192" s="6"/>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B193" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="G190">
+      <c r="G193">
         <v>3</v>
-      </c>
-      <c r="H190" s="6"/>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A191" s="12"/>
-      <c r="B191" s="7" t="s">
-        <v>357</v>
-      </c>
-      <c r="H191" s="6"/>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A192" s="12"/>
-      <c r="H192" s="6"/>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A193" s="12"/>
-      <c r="B193" s="7" t="s">
-        <v>381</v>
       </c>
       <c r="H193" s="6"/>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="12"/>
       <c r="B194" s="7" t="s">
-        <v>382</v>
+        <v>357</v>
       </c>
       <c r="H194" s="6"/>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="12"/>
-      <c r="B195" s="7" t="s">
+      <c r="H195" s="6"/>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196" s="12"/>
+      <c r="B196" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="H196" s="6"/>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197" s="12"/>
+      <c r="B197" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="H197" s="6"/>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="12"/>
+      <c r="B198" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="H195" s="6"/>
-    </row>
-    <row r="196" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B196" s="17" t="s">
+      <c r="H198" s="6"/>
+    </row>
+    <row r="199" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B199" s="17" t="s">
         <v>337</v>
       </c>
-      <c r="H196" s="6"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B197" s="15" t="s">
+      <c r="H199" s="6"/>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B200" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="H197" s="6"/>
-    </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="7" t="s">
+      <c r="H200" s="6"/>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B201" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="G198">
-        <v>2</v>
-      </c>
-      <c r="H198" s="6"/>
-    </row>
-    <row r="199" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="12" t="s">
+      <c r="G201">
+        <v>2</v>
+      </c>
+      <c r="H201" s="6"/>
+    </row>
+    <row r="202" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="B199" s="15" t="s">
+      <c r="B202" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="C199" s="15"/>
-      <c r="D199" s="15"/>
-      <c r="H199" s="14"/>
-    </row>
-    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="B200" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E200" t="s">
-        <v>134</v>
-      </c>
-      <c r="G200">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="12" t="s">
-        <v>318</v>
-      </c>
-      <c r="B201" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="G201">
-        <v>9</v>
-      </c>
-      <c r="I201" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="12"/>
-      <c r="B202" s="7" t="s">
-        <v>380</v>
-      </c>
-      <c r="G202">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C202" s="15"/>
+      <c r="D202" s="15"/>
+      <c r="H202" s="14"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
         <v>318</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>332</v>
+        <v>135</v>
+      </c>
+      <c r="E203" t="s">
+        <v>134</v>
       </c>
       <c r="G203">
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="12" t="s">
         <v>318</v>
       </c>
       <c r="B204" s="7" t="s">
-        <v>256</v>
+        <v>331</v>
       </c>
       <c r="G204">
-        <v>2</v>
-      </c>
-      <c r="H204" s="6"/>
-    </row>
-    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I204" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205" s="12"/>
+      <c r="B205" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="B205" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="G205">
-        <v>0</v>
-      </c>
-      <c r="I205" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="12"/>
       <c r="B206" s="7" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="G206">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
-        <v>300</v>
-      </c>
-      <c r="B207" s="8" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="B207" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G207">
+        <v>2</v>
+      </c>
+      <c r="H207" s="6"/>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="12" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="B208" s="7" t="s">
-        <v>301</v>
+        <v>121</v>
       </c>
       <c r="G208">
         <v>0</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="12" t="s">
-        <v>300</v>
-      </c>
+      <c r="I208" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A209" s="12"/>
       <c r="B209" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E209" t="s">
-        <v>134</v>
+        <v>349</v>
       </c>
       <c r="G209">
-        <v>0</v>
-      </c>
-      <c r="H209" s="6">
-        <v>42702</v>
-      </c>
-      <c r="I209" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="B210" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C210" s="9"/>
-      <c r="D210" s="9"/>
-      <c r="G210">
-        <v>0</v>
-      </c>
-      <c r="H210" s="6">
-        <v>42702</v>
-      </c>
-      <c r="I210" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B210" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
         <v>300</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E211" t="s">
-        <v>134</v>
+        <v>301</v>
       </c>
       <c r="G211">
         <v>0</v>
       </c>
-      <c r="H211" s="6">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="12" t="s">
         <v>300</v>
       </c>
       <c r="B212" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E212" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G212">
         <v>0</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H212" s="6">
+        <v>42702</v>
+      </c>
+      <c r="I212" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="B213" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="E213" t="s">
-        <v>136</v>
-      </c>
+      <c r="B213" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C213" s="9"/>
+      <c r="D213" s="9"/>
       <c r="G213">
         <v>0</v>
       </c>
       <c r="H213" s="6">
-        <v>42697</v>
+        <v>42702</v>
       </c>
       <c r="I213" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="12" t="s">
         <v>300</v>
       </c>
       <c r="B214" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E214" t="s">
+        <v>134</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
+      <c r="H214" s="6">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A215" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B215" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E215" t="s">
+        <v>136</v>
+      </c>
+      <c r="G215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A216" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B216" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E216" t="s">
+        <v>136</v>
+      </c>
+      <c r="G216">
+        <v>0</v>
+      </c>
+      <c r="H216" s="6">
+        <v>42697</v>
+      </c>
+      <c r="I216" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A217" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B217" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="G214">
-        <v>2</v>
-      </c>
-      <c r="H214" s="6"/>
-    </row>
-    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="12"/>
-      <c r="B215" s="13" t="s">
+      <c r="G217">
+        <v>2</v>
+      </c>
+      <c r="H217" s="6"/>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A218" s="12"/>
+      <c r="B218" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="G215">
+      <c r="G218">
         <v>9</v>
       </c>
-      <c r="H215" s="6"/>
-    </row>
-    <row r="216" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="B216" s="17" t="s">
+      <c r="H218" s="6"/>
+    </row>
+    <row r="219" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+      <c r="B219" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C216" s="17"/>
-      <c r="D216" s="17"/>
-    </row>
-    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B217" s="8" t="s">
+      <c r="C219" s="17"/>
+      <c r="D219" s="17"/>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B220" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="G217">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B218" t="s">
+      <c r="G220">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
         <v>316</v>
       </c>
-      <c r="C218" s="7" t="s">
+      <c r="C221" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="D218" s="28">
+      <c r="D221" s="28">
         <v>42775</v>
       </c>
-      <c r="G218">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B219" s="7" t="s">
+      <c r="G221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B222" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="G219">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
+      <c r="G222">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
         <v>308</v>
       </c>
-      <c r="C220" s="7" t="s">
+      <c r="C223" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="D220" s="28">
+      <c r="D223" s="28">
         <v>42775</v>
       </c>
-      <c r="G220">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B221" s="7" t="s">
+      <c r="G223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B224" s="7" t="s">
         <v>385</v>
       </c>
-      <c r="G221">
-        <v>2</v>
-      </c>
-      <c r="H221" s="6"/>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B222" s="8" t="s">
+      <c r="G224">
+        <v>2</v>
+      </c>
+      <c r="H224" s="6"/>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B225" s="8" t="s">
         <v>359</v>
-      </c>
-      <c r="H222" s="6"/>
-    </row>
-    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B223" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="G223">
-        <v>3</v>
-      </c>
-      <c r="H223" s="6"/>
-    </row>
-    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B224" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="G224">
-        <v>3</v>
-      </c>
-      <c r="H224" s="6"/>
-    </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B225" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="G225">
-        <v>3</v>
       </c>
       <c r="H225" s="6"/>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B226" s="7" t="s">
-        <v>384</v>
+        <v>360</v>
+      </c>
+      <c r="G226">
+        <v>3</v>
       </c>
       <c r="H226" s="6"/>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B227" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="G227">
+        <v>3</v>
+      </c>
+      <c r="H227" s="6"/>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B228" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="G228">
+        <v>3</v>
+      </c>
+      <c r="H228" s="6"/>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B229" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="H229" s="6"/>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B230" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="H227" s="6"/>
-    </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B228" s="8" t="s">
+      <c r="H230" s="6"/>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B231" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="C228" s="8"/>
-      <c r="D228" s="8"/>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A229">
-        <v>1</v>
-      </c>
-      <c r="B229" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E229" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="230" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A230">
-        <v>2</v>
-      </c>
-      <c r="B230" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E230" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A231">
-        <v>3</v>
-      </c>
-      <c r="B231" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="E231" t="s">
-        <v>211</v>
-      </c>
+      <c r="C231" s="8"/>
+      <c r="D231" s="8"/>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232">
+        <v>1</v>
+      </c>
+      <c r="B232" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E232" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>2</v>
+      </c>
+      <c r="B233" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E233" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>3</v>
+      </c>
+      <c r="B234" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E234" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A235">
         <v>4</v>
       </c>
-      <c r="B232" s="7" t="s">
+      <c r="B235" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
         <v>175</v>
       </c>
-      <c r="B233" s="7" t="s">
+      <c r="B236" s="7" t="s">
         <v>193</v>
-      </c>
-      <c r="E233" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B234" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="E234" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B235" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E235" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B236" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="E236" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B237" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E237" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B238" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="E238" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B239" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E239" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B240" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="E237" t="s">
+      <c r="E240" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B238" s="7" t="s">
+    <row r="241" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B241" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="E238" t="s">
+      <c r="E241" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B239" s="10" t="s">
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B242" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C239" s="10"/>
-      <c r="D239" s="10"/>
-    </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B240" s="7" t="s">
+      <c r="C242" s="10"/>
+      <c r="D242" s="10"/>
+    </row>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B243" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E243" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B241" s="7" t="s">
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B244" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B242" s="7" t="s">
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B245" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B243" s="7" t="s">
+    <row r="246" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B246" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B244" s="7" t="s">
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B247" s="7" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B245" s="7" t="s">
+    <row r="248" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B248" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="E245" t="s">
+      <c r="E248" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="7" t="s">
+    <row r="249" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B249" s="7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B247" s="7" t="s">
+    <row r="250" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B250" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E247" t="s">
+      <c r="E250" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B248" s="7" t="s">
+    <row r="251" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B251" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="E248" t="s">
+      <c r="E251" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B249" s="10" t="s">
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B252" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="C249" s="10"/>
-      <c r="D249" s="10"/>
-    </row>
-    <row r="250" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B250" s="7" t="s">
+      <c r="C252" s="10"/>
+      <c r="D252" s="10"/>
+    </row>
+    <row r="253" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B253" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="E250" t="s">
+      <c r="E253" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B251" s="7" t="s">
+    <row r="254" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B254" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="E251" t="s">
+      <c r="E254" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B252" s="7" t="s">
+    <row r="255" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B255" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B253" s="7" t="s">
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B256" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A254">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A257">
         <v>1</v>
       </c>
-      <c r="B254" s="7" t="s">
+      <c r="B257" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="G254">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A255">
-        <v>2</v>
-      </c>
-      <c r="B255" s="7" t="s">
+      <c r="G257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>2</v>
+      </c>
+      <c r="B258" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B256" s="7" t="s">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B259" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="G256">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="257" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B257" s="7" t="s">
+      <c r="G259">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B260" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="G257">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="258" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B258" s="7" t="s">
+      <c r="G260">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B261" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="G258">
+      <c r="G261">
         <v>3</v>
       </c>
     </row>
-    <row r="259" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B259" s="7" t="s">
+    <row r="262" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B262" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="G259">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="260" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B260" s="7" t="s">
+      <c r="G262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B263" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="G260">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="261" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B261" s="7" t="s">
+      <c r="G263">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B264" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="E261" t="s">
+      <c r="E264" t="s">
         <v>220</v>
-      </c>
-      <c r="G261">
-        <v>0</v>
-      </c>
-      <c r="H261" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="262" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B262" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="E262" t="s">
-        <v>221</v>
-      </c>
-      <c r="G262">
-        <v>0</v>
-      </c>
-      <c r="H262" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="263" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B263" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="E263" t="s">
-        <v>222</v>
-      </c>
-      <c r="G263">
-        <v>0</v>
-      </c>
-      <c r="H263" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="264" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B264" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="G264">
         <v>0</v>
@@ -5656,9 +5678,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="265" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B265" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
+      </c>
+      <c r="E265" t="s">
+        <v>221</v>
       </c>
       <c r="G265">
         <v>0</v>
@@ -5667,9 +5692,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="266" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B266" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
+      </c>
+      <c r="E266" t="s">
+        <v>222</v>
       </c>
       <c r="G266">
         <v>0</v>
@@ -5678,19 +5706,46 @@
         <v>145</v>
       </c>
     </row>
-    <row r="268" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B267" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="G267">
+        <v>0</v>
+      </c>
+      <c r="H267" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B268" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G268">
+        <v>0</v>
+      </c>
+      <c r="H268" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B269" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="G269">
+        <v>0</v>
+      </c>
+      <c r="H269" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B271" s="7" t="s">
         <v>219</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:I266">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A7:I269"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="84" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
1. Incorrect display of value in DDAS.WebSite / investigator-summary.component.ts corrected: return this.Investigator.SitesSearched.filter(x => x.Exclude == false); 2. User Roles : do not show app-admin role when creating a new user - if logged in user is not AppAdmin 3. WebSite / About us -- Clarity logo added
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -2567,10 +2567,10 @@
   <dimension ref="A1:J278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B232" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B199" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="H239" sqref="H239"/>
+      <selection pane="bottomRight" activeCell="H228" sqref="H228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2975,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>2</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>2</v>
       </c>
@@ -3073,7 +3073,7 @@
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="1:8" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" s="12" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>2</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="9" t="s">
         <v>363</v>
@@ -3692,7 +3692,7 @@
       </c>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>2</v>
       </c>
@@ -3710,7 +3710,7 @@
       </c>
       <c r="I77" s="14"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>2</v>
       </c>
@@ -3725,7 +3725,7 @@
       </c>
       <c r="I78" s="6"/>
     </row>
-    <row r="79" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>2</v>
       </c>
@@ -3847,7 +3847,7 @@
       </c>
       <c r="I85" s="6"/>
     </row>
-    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12"/>
       <c r="B86" s="7" t="s">
         <v>390</v>
@@ -3870,7 +3870,7 @@
       </c>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12"/>
       <c r="B87" s="7" t="s">
         <v>391</v>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12"/>
       <c r="B88" s="7" t="s">
         <v>393</v>
@@ -3980,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>2</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
         <v>2</v>
       </c>
@@ -4261,7 +4261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B116" s="18" t="s">
         <v>371</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
         <v>2</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12"/>
       <c r="B134" s="7" t="s">
         <v>377</v>
@@ -4528,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
         <v>2</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
         <v>1</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12"/>
       <c r="B151" s="9" t="s">
         <v>388</v>
@@ -4662,7 +4662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
       <c r="B152" s="9" t="s">
         <v>389</v>
@@ -4678,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12"/>
       <c r="B153" s="9" t="s">
         <v>385</v>
@@ -4771,7 +4771,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12"/>
       <c r="B162" s="7" t="s">
         <v>345</v>
@@ -4863,7 +4863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
         <v>1</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
         <v>1</v>
       </c>
@@ -4956,7 +4956,7 @@
         <v>42702</v>
       </c>
     </row>
-    <row r="175" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B175" s="13" t="s">
         <v>346</v>
       </c>
@@ -5040,7 +5040,7 @@
       <c r="E180" s="15"/>
       <c r="I180" s="14"/>
     </row>
-    <row r="181" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>1</v>
       </c>
@@ -5058,7 +5058,7 @@
       </c>
       <c r="I181" s="14"/>
     </row>
-    <row r="182" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
         <v>1</v>
       </c>
@@ -5109,7 +5109,7 @@
       <c r="E185" s="15"/>
       <c r="I185" s="14"/>
     </row>
-    <row r="186" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
         <v>1</v>
       </c>
@@ -5136,7 +5136,7 @@
       </c>
       <c r="I187" s="6"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="12" t="s">
         <v>335</v>
       </c>
@@ -5148,7 +5148,7 @@
       </c>
       <c r="I188" s="6"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
         <v>335</v>
       </c>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="I189" s="6"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
         <v>335</v>
       </c>
@@ -5172,7 +5172,7 @@
       </c>
       <c r="I190" s="6"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
         <v>335</v>
       </c>
@@ -5196,7 +5196,7 @@
       </c>
       <c r="I192" s="6"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>335</v>
       </c>
@@ -5208,7 +5208,7 @@
       </c>
       <c r="I193" s="6"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
         <v>335</v>
       </c>
@@ -5220,7 +5220,7 @@
       </c>
       <c r="I194" s="6"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
         <v>335</v>
       </c>
@@ -5232,7 +5232,7 @@
       </c>
       <c r="I195" s="6"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
         <v>335</v>
       </c>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="I203" s="6"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B204" s="7" t="s">
         <v>352</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
         <v>317</v>
       </c>
@@ -5386,7 +5386,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="7" t="s">
         <v>348</v>
@@ -5505,7 +5505,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>299</v>
       </c>
@@ -5535,7 +5535,7 @@
       <c r="D223" s="16"/>
       <c r="E223" s="16"/>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B224" s="8" t="s">
         <v>262</v>
       </c>
@@ -5543,7 +5543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
         <v>315</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B226" s="7" t="s">
         <v>349</v>
       </c>
@@ -5605,7 +5605,7 @@
       </c>
       <c r="I230" s="6"/>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B231" s="7" t="s">
         <v>360</v>
       </c>
@@ -5614,7 +5614,7 @@
       </c>
       <c r="I231" s="6"/>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B232" s="7" t="s">
         <v>361</v>
       </c>
@@ -5629,7 +5629,7 @@
       </c>
       <c r="I233" s="6"/>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B234" s="7" t="s">
         <v>357</v>
       </c>
@@ -5638,7 +5638,7 @@
       </c>
       <c r="I234" s="6"/>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B235" s="7" t="s">
         <v>402</v>
       </c>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="I235" s="6"/>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B236" s="7" t="s">
         <v>403</v>
       </c>
@@ -5656,7 +5656,7 @@
       </c>
       <c r="I236" s="6"/>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B237" s="7" t="s">
         <v>404</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B266" s="7" t="s">
         <v>198</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B267" s="7" t="s">
         <v>199</v>
       </c>
@@ -5899,7 +5899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="B268" s="7" t="s">
         <v>200</v>
       </c>
@@ -6008,8 +6008,6 @@
     <filterColumn colId="7">
       <filters blank="1">
         <filter val="1"/>
-        <filter val="2"/>
-        <filter val="3"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Updated Clincial Investigator Inspection section: Classification codes bug corrected.
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="-45" windowWidth="15780" windowHeight="7830" tabRatio="375" activeTab="3"/>
+    <workbookView xWindow="135" yWindow="-45" windowWidth="17295" windowHeight="7830" tabRatio="375" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="418">
   <si>
     <t>Reports</t>
   </si>
@@ -2644,10 +2644,10 @@
   <dimension ref="A1:J291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomRight" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,7 +3108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="9" t="s">
         <v>367</v>
@@ -3123,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="28" t="s">
         <v>410</v>
@@ -3143,8 +3143,11 @@
       <c r="I34" s="31">
         <v>42834</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>2</v>
       </c>
@@ -3155,7 +3158,7 @@
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="1:9" s="12" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="12" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>2</v>
       </c>
@@ -3169,7 +3172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>2</v>
       </c>
@@ -3183,7 +3186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>2</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>2</v>
       </c>
@@ -3211,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>2</v>
       </c>
@@ -3225,7 +3228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>2</v>
       </c>
@@ -3246,7 +3249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>2</v>
       </c>
@@ -3270,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12"/>
       <c r="B43" s="9" t="s">
         <v>361</v>
@@ -3285,7 +3288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="9" t="s">
         <v>368</v>
@@ -3300,7 +3303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>2</v>
       </c>
@@ -3311,7 +3314,7 @@
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>2</v>
       </c>
@@ -3325,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>2</v>
       </c>
@@ -3339,7 +3342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>2</v>
       </c>
@@ -3353,7 +3356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>2</v>
       </c>
@@ -3367,7 +3370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="12"/>
       <c r="B50" s="9" t="s">
         <v>365</v>
@@ -3382,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12"/>
       <c r="B51" s="9" t="s">
         <v>371</v>
@@ -3397,7 +3400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>2</v>
       </c>
@@ -3411,7 +3414,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>2</v>
       </c>
@@ -3425,7 +3428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>2</v>
       </c>
@@ -3436,7 +3439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="12" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="12" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>2</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="12" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" s="12" customFormat="1" ht="18.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>2</v>
       </c>
@@ -3478,7 +3481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>392</v>
       </c>
@@ -3498,7 +3501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="28" t="s">
         <v>413</v>
       </c>
@@ -3515,8 +3518,11 @@
       <c r="I58" s="31">
         <v>42834</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J58" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="28" t="s">
         <v>409</v>
       </c>
@@ -3533,8 +3539,11 @@
       <c r="I59" s="31">
         <v>42834</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="28" t="s">
         <v>414</v>
       </c>
@@ -3545,8 +3554,11 @@
       <c r="G60" s="32"/>
       <c r="H60" s="32"/>
       <c r="I60" s="32"/>
-    </row>
-    <row r="61" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="34" t="s">
         <v>412</v>
       </c>
@@ -3564,7 +3576,7 @@
         <v>42842</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="28" t="s">
         <v>407</v>
       </c>
@@ -3583,8 +3595,11 @@
       <c r="I62" s="31">
         <v>42834</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>2</v>
       </c>
@@ -3595,7 +3610,7 @@
       <c r="D63" s="27"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>2</v>
       </c>
@@ -3609,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>2</v>
       </c>
@@ -3623,7 +3638,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
         <v>2</v>
       </c>
@@ -3637,7 +3652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>2</v>
       </c>
@@ -3651,7 +3666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
         <v>2</v>
       </c>
@@ -3665,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>2</v>
       </c>
@@ -3679,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B70" s="9" t="s">
         <v>293</v>
       </c>
@@ -3690,7 +3705,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>2</v>
       </c>
@@ -3709,7 +3724,7 @@
       </c>
       <c r="I71" s="6"/>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
         <v>2</v>
       </c>
@@ -3727,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>2</v>
       </c>
@@ -3745,7 +3760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="30" t="s">
         <v>411</v>
@@ -3765,8 +3780,11 @@
       <c r="I74" s="31">
         <v>42834</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>2</v>
       </c>
@@ -3783,7 +3801,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>2</v>
       </c>
@@ -3797,7 +3815,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>2</v>
       </c>
@@ -3814,7 +3832,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="78" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
         <v>2</v>
       </c>
@@ -3831,7 +3849,7 @@
         <v>42698</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>2</v>
       </c>
@@ -3845,7 +3863,7 @@
         <v>42697</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>2</v>
       </c>
@@ -4358,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="20" t="s">
         <v>342</v>
@@ -4367,7 +4385,7 @@
       <c r="D113" s="19"/>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="20" t="s">
         <v>340</v>
@@ -4376,7 +4394,7 @@
       <c r="D114" s="19"/>
       <c r="E114" s="19"/>
     </row>
-    <row r="115" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="20" t="s">
         <v>341</v>
@@ -4385,7 +4403,7 @@
       <c r="D115" s="19"/>
       <c r="E115" s="19"/>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
         <v>2</v>
       </c>
@@ -4396,7 +4414,7 @@
       <c r="D116" s="8"/>
       <c r="E116" s="8"/>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>2</v>
       </c>
@@ -4407,7 +4425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>2</v>
       </c>
@@ -4418,7 +4436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>2</v>
       </c>
@@ -4429,7 +4447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
         <v>2</v>
       </c>
@@ -4440,7 +4458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>2</v>
       </c>
@@ -4451,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>2</v>
       </c>
@@ -4462,7 +4480,7 @@
       <c r="D122" s="8"/>
       <c r="E122" s="8"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="12"/>
       <c r="B123" s="28" t="s">
         <v>417</v>
@@ -4483,7 +4501,7 @@
         <v>42842</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
       <c r="B124" s="28" t="s">
         <v>408</v>
@@ -4505,8 +4523,11 @@
       <c r="I124" s="31">
         <v>42834</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J124" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="28" t="s">
         <v>406</v>
@@ -4525,7 +4546,7 @@
         <v>42842</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="12"/>
       <c r="B126" s="28" t="s">
         <v>405</v>
@@ -4547,8 +4568,11 @@
       <c r="I126" s="31">
         <v>42834</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J126" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
         <v>2</v>
       </c>
@@ -4569,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
VerD1.5.0 1. Single Match Findings in Findings  Display, pagination etc.  Add to Compliance Form
2. Add Findings for Institute

3. Default Sites
 List, Add, Delete
 Web Site
 API
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="-45" windowWidth="17295" windowHeight="7830" tabRatio="375" activeTab="3"/>
+    <workbookView xWindow="135" yWindow="-45" windowWidth="20355" windowHeight="7830" tabRatio="375" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,14 @@
     <sheet name="Actions - Post - Demo1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$J$289</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$J$294</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="424">
   <si>
     <t>Reports</t>
   </si>
@@ -1431,6 +1431,24 @@
   </si>
   <si>
     <t>Sam Site Converting from Live to DB</t>
+  </si>
+  <si>
+    <t>Deferred</t>
+  </si>
+  <si>
+    <t>Clarifications required from ICON</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>Institute related Findings - Changes in Compliance Form</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Authroisation in API Controllers</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1533,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1538,11 +1556,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1610,20 +1665,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2641,13 +2751,13 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J291"/>
+  <dimension ref="A1:K296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="J61" sqref="J61"/>
+      <selection pane="bottomRight" activeCell="H238" sqref="H238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2726,7 +2836,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
@@ -2786,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>2</v>
       </c>
@@ -3013,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>2</v>
       </c>
@@ -3052,7 +3162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>2</v>
       </c>
@@ -3080,7 +3190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>2</v>
       </c>
@@ -3123,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12"/>
       <c r="B34" s="28" t="s">
         <v>410</v>
@@ -3138,7 +3248,7 @@
       <c r="F34" s="30"/>
       <c r="G34" s="30"/>
       <c r="H34" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="31">
         <v>42834</v>
@@ -3147,7 +3257,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>2</v>
       </c>
@@ -3158,19 +3268,23 @@
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
     </row>
-    <row r="36" spans="1:10" s="12" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="18" t="s">
+    <row r="36" spans="1:10" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="H36" s="12">
-        <v>2</v>
-      </c>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52">
+        <v>2</v>
+      </c>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
     </row>
     <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
@@ -3273,20 +3387,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="9" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="52"/>
+      <c r="B43" s="54" t="s">
         <v>361</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="G43" t="s">
+      <c r="C43" s="55"/>
+      <c r="D43" s="56"/>
+      <c r="E43" s="56"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57" t="s">
         <v>318</v>
       </c>
-      <c r="H43">
-        <v>2</v>
-      </c>
+      <c r="H43" s="57">
+        <v>2</v>
+      </c>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
     </row>
     <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
@@ -3303,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>2</v>
       </c>
@@ -3400,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>2</v>
       </c>
@@ -3501,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" s="28" t="s">
         <v>413</v>
       </c>
@@ -3514,7 +3631,9 @@
       <c r="E58" s="29"/>
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
+      <c r="H58" s="32">
+        <v>0</v>
+      </c>
       <c r="I58" s="31">
         <v>42834</v>
       </c>
@@ -3522,7 +3641,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" s="28" t="s">
         <v>409</v>
       </c>
@@ -3535,7 +3654,9 @@
       <c r="E59" s="29"/>
       <c r="F59" s="32"/>
       <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
+      <c r="H59" s="32">
+        <v>0</v>
+      </c>
       <c r="I59" s="31">
         <v>42834</v>
       </c>
@@ -3543,63 +3664,77 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="28" t="s">
+    <row r="60" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="35" t="s">
         <v>414</v>
       </c>
-      <c r="C60" s="33"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
+      <c r="C60" s="35" t="s">
+        <v>397</v>
+      </c>
+      <c r="D60" s="36">
+        <v>42831</v>
+      </c>
+      <c r="E60" s="36"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37">
+        <v>0</v>
+      </c>
+      <c r="I60" s="37"/>
       <c r="J60" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="34" t="s">
+      <c r="A61" s="52"/>
+      <c r="B61" s="58" t="s">
         <v>412</v>
       </c>
-      <c r="C61" s="34" t="s">
+      <c r="C61" s="58" t="s">
         <v>397</v>
       </c>
-      <c r="D61" s="35">
+      <c r="D61" s="59">
         <v>42831</v>
       </c>
-      <c r="E61" s="34"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="30"/>
-      <c r="I61" s="36">
+      <c r="E61" s="58"/>
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57">
+        <v>1</v>
+      </c>
+      <c r="I61" s="60">
         <v>42842</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="28" t="s">
+      <c r="J61" s="52" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="38" t="s">
         <v>407</v>
       </c>
-      <c r="C62" s="33" t="s">
+      <c r="C62" s="39" t="s">
         <v>397</v>
       </c>
-      <c r="D62" s="29">
+      <c r="D62" s="40">
         <v>42831</v>
       </c>
-      <c r="E62" s="29"/>
-      <c r="F62" s="32" t="s">
+      <c r="E62" s="40"/>
+      <c r="F62" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-      <c r="I62" s="31">
+      <c r="G62" s="41"/>
+      <c r="H62" s="41">
+        <v>0</v>
+      </c>
+      <c r="I62" s="42">
         <v>42834</v>
       </c>
       <c r="J62" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>2</v>
       </c>
@@ -3760,23 +3895,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12"/>
       <c r="B74" s="30" t="s">
         <v>411</v>
       </c>
-      <c r="C74" s="34" t="s">
+      <c r="C74" s="33" t="s">
         <v>397</v>
       </c>
-      <c r="D74" s="35">
+      <c r="D74" s="34">
         <v>42831</v>
       </c>
-      <c r="E74" s="35"/>
+      <c r="E74" s="34"/>
       <c r="F74" s="30" t="s">
         <v>133</v>
       </c>
       <c r="G74" s="30"/>
-      <c r="H74" s="30"/>
+      <c r="H74" s="30">
+        <v>0</v>
+      </c>
       <c r="I74" s="31">
         <v>42834</v>
       </c>
@@ -3784,7 +3921,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>2</v>
       </c>
@@ -3875,7 +4012,7 @@
       </c>
       <c r="I80" s="6"/>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>2</v>
       </c>
@@ -3887,7 +4024,7 @@
       </c>
       <c r="I81" s="6"/>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>2</v>
       </c>
@@ -3899,58 +4036,67 @@
       </c>
       <c r="I82" s="6"/>
     </row>
-    <row r="83" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" s="13" t="s">
+    <row r="83" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B83" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="12" t="s">
+      <c r="C83" s="55"/>
+      <c r="D83" s="55"/>
+      <c r="E83" s="55"/>
+      <c r="F83" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="H83" s="12">
+      <c r="G83" s="52"/>
+      <c r="H83" s="52">
         <v>3</v>
       </c>
-      <c r="I83" s="14"/>
-    </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B84" s="7" t="s">
+      <c r="I83" s="61"/>
+      <c r="J83" s="52"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="F84" t="s">
+      <c r="C84" s="58"/>
+      <c r="D84" s="58"/>
+      <c r="E84" s="58"/>
+      <c r="F84" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="H84">
+      <c r="G84" s="57"/>
+      <c r="H84" s="57">
         <v>3</v>
       </c>
-      <c r="I84" s="6"/>
-    </row>
-    <row r="85" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B85" s="13" t="s">
+      <c r="I84" s="60"/>
+      <c r="J84" s="57"/>
+    </row>
+    <row r="85" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B85" s="55" t="s">
         <v>271</v>
       </c>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="12" t="s">
+      <c r="C85" s="55"/>
+      <c r="D85" s="55"/>
+      <c r="E85" s="55"/>
+      <c r="F85" s="52" t="s">
         <v>272</v>
       </c>
-      <c r="H85" s="12">
+      <c r="G85" s="52"/>
+      <c r="H85" s="52">
         <v>3</v>
       </c>
-      <c r="I85" s="14"/>
-    </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="61"/>
+      <c r="J85" s="52"/>
+    </row>
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>2</v>
       </c>
@@ -3965,7 +4111,7 @@
       </c>
       <c r="I86" s="6"/>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>2</v>
       </c>
@@ -3977,7 +4123,7 @@
       </c>
       <c r="I87" s="6"/>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>2</v>
       </c>
@@ -3996,7 +4142,7 @@
       </c>
       <c r="I88" s="6"/>
     </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>2</v>
       </c>
@@ -4015,7 +4161,7 @@
       </c>
       <c r="I89" s="6"/>
     </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>2</v>
       </c>
@@ -4034,7 +4180,7 @@
       </c>
       <c r="I90" s="6"/>
     </row>
-    <row r="91" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>2</v>
       </c>
@@ -4054,7 +4200,7 @@
       </c>
       <c r="I91" s="6"/>
     </row>
-    <row r="92" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="7" t="s">
         <v>388</v>
@@ -4077,7 +4223,7 @@
       </c>
       <c r="I92" s="6"/>
     </row>
-    <row r="93" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
       <c r="B93" s="7" t="s">
         <v>389</v>
@@ -4100,7 +4246,7 @@
       </c>
       <c r="I93" s="6"/>
     </row>
-    <row r="94" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
       <c r="B94" s="7" t="s">
         <v>391</v>
@@ -4118,7 +4264,7 @@
       </c>
       <c r="I94" s="6"/>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
       <c r="B95" s="8" t="s">
         <v>404</v>
@@ -4130,49 +4276,59 @@
       <c r="H95" s="12"/>
       <c r="I95" s="6"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
-      <c r="B96" s="34" t="s">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="52"/>
+      <c r="B96" s="58" t="s">
         <v>415</v>
       </c>
-      <c r="C96" s="34" t="s">
+      <c r="C96" s="58" t="s">
         <v>397</v>
       </c>
-      <c r="D96" s="35">
+      <c r="D96" s="59">
         <v>42831</v>
       </c>
-      <c r="E96" s="35"/>
-      <c r="F96" s="30" t="s">
+      <c r="E96" s="59"/>
+      <c r="F96" s="57" t="s">
         <v>272</v>
       </c>
-      <c r="G96" s="32"/>
-      <c r="H96" s="32"/>
-      <c r="I96" s="36">
+      <c r="G96" s="52"/>
+      <c r="H96" s="52">
+        <v>1</v>
+      </c>
+      <c r="I96" s="60">
         <v>42842</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="12"/>
-      <c r="B97" s="34" t="s">
+      <c r="J96" s="62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="52"/>
+      <c r="B97" s="58" t="s">
         <v>416</v>
       </c>
-      <c r="C97" s="34" t="s">
+      <c r="C97" s="58" t="s">
         <v>397</v>
       </c>
-      <c r="D97" s="35">
+      <c r="D97" s="59">
         <v>42831</v>
       </c>
-      <c r="E97" s="35"/>
-      <c r="F97" s="30" t="s">
+      <c r="E97" s="59"/>
+      <c r="F97" s="57" t="s">
         <v>272</v>
       </c>
-      <c r="G97" s="32"/>
-      <c r="H97" s="32"/>
-      <c r="I97" s="36">
+      <c r="G97" s="52"/>
+      <c r="H97" s="52">
+        <v>1</v>
+      </c>
+      <c r="I97" s="60">
         <v>42842</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J97" s="62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
       <c r="B98" s="8" t="s">
         <v>373</v>
@@ -4183,7 +4339,7 @@
       <c r="H98" s="12"/>
       <c r="I98" s="6"/>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
       <c r="B99" s="7" t="s">
         <v>374</v>
@@ -4198,7 +4354,7 @@
       </c>
       <c r="I99" s="6"/>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>2</v>
       </c>
@@ -4212,7 +4368,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>2</v>
       </c>
@@ -4223,7 +4379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
         <v>2</v>
       </c>
@@ -4241,18 +4397,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" s="7" t="s">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="58" t="s">
         <v>403</v>
       </c>
-      <c r="H103">
+      <c r="C103" s="58"/>
+      <c r="D103" s="58"/>
+      <c r="E103" s="58"/>
+      <c r="F103" s="57"/>
+      <c r="G103" s="57"/>
+      <c r="H103" s="57">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I103" s="57"/>
+      <c r="J103" s="57"/>
+    </row>
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
         <v>2</v>
       </c>
@@ -4263,7 +4426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
       <c r="B105" s="7" t="s">
         <v>363</v>
@@ -4275,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
       <c r="B106" s="7" t="s">
         <v>364</v>
@@ -4287,7 +4450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>2</v>
       </c>
@@ -4301,7 +4464,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
         <v>2</v>
       </c>
@@ -4315,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>2</v>
       </c>
@@ -4333,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
         <v>2</v>
       </c>
@@ -4347,7 +4510,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
         <v>2</v>
       </c>
@@ -4358,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
         <v>2</v>
       </c>
@@ -4376,7 +4539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="20" t="s">
         <v>342</v>
@@ -4385,7 +4548,7 @@
       <c r="D113" s="19"/>
       <c r="E113" s="19"/>
     </row>
-    <row r="114" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="20" t="s">
         <v>340</v>
@@ -4394,7 +4557,7 @@
       <c r="D114" s="19"/>
       <c r="E114" s="19"/>
     </row>
-    <row r="115" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="12"/>
       <c r="B115" s="20" t="s">
         <v>341</v>
@@ -4403,7 +4566,7 @@
       <c r="D115" s="19"/>
       <c r="E115" s="19"/>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
         <v>2</v>
       </c>
@@ -4414,7 +4577,7 @@
       <c r="D116" s="8"/>
       <c r="E116" s="8"/>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>2</v>
       </c>
@@ -4425,7 +4588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
         <v>2</v>
       </c>
@@ -4436,18 +4599,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B119" s="7" t="s">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="58" t="s">
         <v>267</v>
       </c>
-      <c r="H119">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C119" s="58"/>
+      <c r="D119" s="58"/>
+      <c r="E119" s="58"/>
+      <c r="F119" s="57"/>
+      <c r="G119" s="57"/>
+      <c r="H119" s="57">
+        <v>2</v>
+      </c>
+      <c r="I119" s="57"/>
+      <c r="J119" s="57"/>
+    </row>
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
         <v>2</v>
       </c>
@@ -4458,7 +4628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>2</v>
       </c>
@@ -4469,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
         <v>2</v>
       </c>
@@ -4480,125 +4650,139 @@
       <c r="D122" s="8"/>
       <c r="E122" s="8"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A123" s="12"/>
-      <c r="B123" s="28" t="s">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="52"/>
+      <c r="B123" s="54" t="s">
         <v>417</v>
       </c>
-      <c r="C123" s="28" t="s">
+      <c r="C123" s="54" t="s">
         <v>397</v>
       </c>
-      <c r="D123" s="37">
+      <c r="D123" s="63">
         <v>42831</v>
       </c>
-      <c r="E123" s="38"/>
-      <c r="F123" s="30" t="s">
+      <c r="E123" s="64"/>
+      <c r="F123" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="G123" s="30"/>
-      <c r="H123" s="30"/>
-      <c r="I123" s="36">
+      <c r="G123" s="57"/>
+      <c r="H123" s="57">
+        <v>1</v>
+      </c>
+      <c r="I123" s="60">
         <v>42842</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J123" s="57" t="s">
+        <v>418</v>
+      </c>
+      <c r="K123" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12"/>
-      <c r="B124" s="28" t="s">
+      <c r="B124" s="43" t="s">
         <v>408</v>
       </c>
-      <c r="C124" s="28" t="s">
+      <c r="C124" s="43" t="s">
         <v>397</v>
       </c>
-      <c r="D124" s="37">
+      <c r="D124" s="44">
         <v>42831</v>
       </c>
-      <c r="E124" s="38"/>
-      <c r="F124" s="30" t="s">
+      <c r="E124" s="45"/>
+      <c r="F124" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="G124" s="30"/>
-      <c r="H124" s="30">
-        <v>0</v>
-      </c>
-      <c r="I124" s="31">
+      <c r="G124" s="46"/>
+      <c r="H124" s="46">
+        <v>0</v>
+      </c>
+      <c r="I124" s="47">
         <v>42834</v>
       </c>
       <c r="J124" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A125" s="12"/>
-      <c r="B125" s="28" t="s">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="52"/>
+      <c r="B125" s="54" t="s">
         <v>406</v>
       </c>
-      <c r="C125" s="34" t="s">
+      <c r="C125" s="58" t="s">
         <v>397</v>
       </c>
-      <c r="D125" s="35">
+      <c r="D125" s="59">
         <v>42831</v>
       </c>
-      <c r="E125" s="38"/>
-      <c r="F125" s="30"/>
-      <c r="G125" s="30"/>
-      <c r="H125" s="30"/>
-      <c r="I125" s="36">
+      <c r="E125" s="64"/>
+      <c r="F125" s="57"/>
+      <c r="G125" s="57"/>
+      <c r="H125" s="57">
+        <v>1</v>
+      </c>
+      <c r="I125" s="60">
         <v>42842</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A126" s="12"/>
-      <c r="B126" s="28" t="s">
+      <c r="J125" s="62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="52"/>
+      <c r="B126" s="54" t="s">
+        <v>421</v>
+      </c>
+      <c r="C126" s="58" t="s">
+        <v>397</v>
+      </c>
+      <c r="D126" s="59">
+        <v>42831</v>
+      </c>
+      <c r="E126" s="64"/>
+      <c r="F126" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="G126" s="57"/>
+      <c r="H126" s="52">
+        <v>1</v>
+      </c>
+      <c r="I126" s="60"/>
+      <c r="J126" s="62"/>
+    </row>
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="12"/>
+      <c r="B127" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="C126" s="34" t="s">
+      <c r="C127" s="48" t="s">
         <v>397</v>
       </c>
-      <c r="D126" s="35">
+      <c r="D127" s="49">
         <v>42831</v>
       </c>
-      <c r="E126" s="38"/>
-      <c r="F126" s="30" t="s">
+      <c r="E127" s="50"/>
+      <c r="F127" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="G126" s="30"/>
-      <c r="H126" s="30">
-        <v>0</v>
-      </c>
-      <c r="I126" s="31">
+      <c r="G127" s="51"/>
+      <c r="H127" s="51">
+        <v>0</v>
+      </c>
+      <c r="I127" s="42">
         <v>42834</v>
       </c>
-      <c r="J126" t="s">
+      <c r="J127" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="127" spans="1:10" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B127" s="22" t="s">
+    <row r="128" spans="1:11" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="22" t="s">
         <v>278</v>
-      </c>
-      <c r="C127" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="D127" s="19">
-        <v>42760</v>
-      </c>
-      <c r="E127" s="19"/>
-      <c r="F127" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="H127" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B128" s="23" t="s">
-        <v>291</v>
       </c>
       <c r="C128" s="13" t="s">
         <v>286</v>
@@ -4607,418 +4791,437 @@
         <v>42760</v>
       </c>
       <c r="E128" s="19"/>
-      <c r="F128" s="19" t="s">
+      <c r="F128" s="12" t="s">
         <v>138</v>
       </c>
       <c r="H128" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="18" t="s">
+    <row r="129" spans="1:10" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="C129" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="D129" s="19">
+        <v>42760</v>
+      </c>
+      <c r="E129" s="19"/>
+      <c r="F129" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="H129" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="52"/>
+      <c r="B130" s="53" t="s">
         <v>369</v>
       </c>
-      <c r="C129" s="13"/>
-      <c r="D129" s="19"/>
-      <c r="E129" s="19"/>
-      <c r="F129" s="19"/>
-      <c r="G129" s="12" t="s">
+      <c r="C130" s="55"/>
+      <c r="D130" s="56"/>
+      <c r="E130" s="56"/>
+      <c r="F130" s="56"/>
+      <c r="G130" s="52" t="s">
         <v>370</v>
       </c>
-      <c r="H129" s="12">
+      <c r="H130" s="52">
         <v>3</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B130" s="7" t="s">
+      <c r="I130" s="52"/>
+      <c r="J130" s="52"/>
+    </row>
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B131" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F131" t="s">
         <v>138</v>
       </c>
-      <c r="H130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B131" s="9" t="s">
+      <c r="H131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B132" s="9" t="s">
         <v>153</v>
-      </c>
-      <c r="C131" s="9"/>
-      <c r="D131" s="9"/>
-      <c r="E131" s="9"/>
-      <c r="H131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B132" s="9" t="s">
-        <v>162</v>
       </c>
       <c r="C132" s="9"/>
       <c r="D132" s="9"/>
       <c r="E132" s="9"/>
       <c r="H132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="H133">
         <v>9</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B133" s="7" t="s">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B134" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F134" t="s">
         <v>133</v>
       </c>
-      <c r="H133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="12"/>
-      <c r="B134" s="7" t="s">
+      <c r="H134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="12"/>
+      <c r="B135" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="H134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B135" s="7" t="s">
+      <c r="H135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B136" s="58" t="s">
         <v>396</v>
       </c>
-      <c r="D135" s="26">
+      <c r="C136" s="58"/>
+      <c r="D136" s="59">
         <v>42818</v>
       </c>
-      <c r="F135" t="s">
+      <c r="E136" s="58"/>
+      <c r="F136" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="H135">
+      <c r="G136" s="57"/>
+      <c r="H136" s="57">
         <v>1</v>
       </c>
-      <c r="I135" s="6">
+      <c r="I136" s="60">
         <v>42702</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B136" s="7" t="s">
+      <c r="J136" s="57"/>
+    </row>
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B137" s="7" t="s">
+      <c r="H137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A138" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B138" s="7" t="s">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A139" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B139" s="7" t="s">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A140" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B140" s="7" t="s">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A141" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B141" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B141" s="7" t="s">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A142" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B142" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B142" s="7" t="s">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B143" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B143" s="8" t="s">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B144" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C143" s="8"/>
-      <c r="D143" s="8"/>
-      <c r="E143" s="8"/>
-    </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B144" s="7" t="s">
+      <c r="C144" s="8"/>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8"/>
+    </row>
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="H144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B145" s="7" t="s">
+      <c r="H145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B146" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="H145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B146" s="7" t="s">
+      <c r="H146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="H146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="12"/>
-      <c r="B147" s="7" t="s">
+      <c r="H147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="12"/>
+      <c r="B148" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="H147">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B148" s="8" t="s">
+      <c r="H148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A149" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B149" s="8" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B149" t="s">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" t="s">
         <v>302</v>
       </c>
-      <c r="C149" s="7" t="s">
+      <c r="C150" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="D149" s="26">
+      <c r="D150" s="26">
         <v>42775</v>
       </c>
-      <c r="E149" s="26"/>
-      <c r="H149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B150" t="s">
+      <c r="E150" s="26"/>
+      <c r="H150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B151" t="s">
         <v>304</v>
       </c>
-      <c r="H150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B151" t="s">
+      <c r="H151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B152" t="s">
         <v>314</v>
       </c>
-      <c r="C151" s="7" t="s">
+      <c r="C152" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="D151" s="26">
+      <c r="D152" s="26">
         <v>42775</v>
       </c>
-      <c r="E151" s="26"/>
-      <c r="H151">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B152" s="7" t="s">
+      <c r="E152" s="26"/>
+      <c r="H152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A153" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B153" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="H152">
+      <c r="C153" s="58"/>
+      <c r="D153" s="58"/>
+      <c r="E153" s="58"/>
+      <c r="F153" s="57"/>
+      <c r="G153" s="57"/>
+      <c r="H153" s="57">
         <v>3</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B153" s="7" t="s">
+      <c r="I153" s="57"/>
+      <c r="J153" s="57"/>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A154" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B154" s="7" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B154" s="7" t="s">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B155" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A155" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B155" s="16" t="s">
+      <c r="H155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A156" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B156" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="D155" s="16"/>
-      <c r="E155" s="16"/>
-    </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B156" s="8" t="s">
+      <c r="D156" s="16"/>
+      <c r="E156" s="16"/>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A157" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B157" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D156" s="8"/>
-      <c r="E156" s="8"/>
-    </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B157" s="9" t="s">
+      <c r="D157" s="8"/>
+      <c r="E157" s="8"/>
+    </row>
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B158" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="H157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B158" s="9" t="s">
+      <c r="H158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B159" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="H158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="12"/>
-      <c r="B159" s="9" t="s">
+      <c r="H159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="12"/>
+      <c r="B160" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="H159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" ht="21" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B160" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D160" s="16"/>
-      <c r="E160" s="16"/>
-    </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A161" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B161" s="8" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B161" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D161" s="16"/>
+      <c r="E161" s="16"/>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B162" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="H162">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B162" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B163" s="8" t="s">
+      <c r="B163" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="H163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A164" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B164" s="8" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="12"/>
-      <c r="B164" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="C164" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="D164" s="26">
-        <v>42809</v>
-      </c>
-      <c r="E164" s="26"/>
-      <c r="H164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12"/>
       <c r="B165" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>286</v>
@@ -5031,10 +5234,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12"/>
       <c r="B166" s="9" t="s">
-        <v>383</v>
+        <v>387</v>
+      </c>
+      <c r="C166" s="7" t="s">
+        <v>286</v>
       </c>
       <c r="D166" s="26">
         <v>42809</v>
@@ -5044,39 +5250,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
-      <c r="B167" s="9"/>
-    </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="C168" s="8"/>
-    </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="D167" s="26">
+        <v>42809</v>
+      </c>
+      <c r="E167" s="26"/>
+      <c r="H167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A168" s="12"/>
+      <c r="B168" s="9"/>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B169" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C169" s="9"/>
-      <c r="D169" s="9"/>
-      <c r="E169" s="9"/>
-      <c r="H169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B169" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C169" s="8"/>
+    </row>
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="C170" s="9"/>
       <c r="D170" s="9"/>
@@ -5085,629 +5290,711 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B171" s="7" t="s">
-        <v>251</v>
-      </c>
+      <c r="B171" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C171" s="9"/>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9"/>
       <c r="H171">
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="H172">
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B173" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="H173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="12"/>
-      <c r="B174" s="10" t="s">
+      <c r="H174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A175" s="12"/>
+      <c r="B175" s="10" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="12"/>
-      <c r="B175" s="7" t="s">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A176" s="52"/>
+      <c r="B176" s="58" t="s">
         <v>343</v>
       </c>
-      <c r="H175">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B176" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C176" s="8"/>
-      <c r="D176" s="8"/>
-      <c r="E176" s="8"/>
-      <c r="H176" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C176" s="58"/>
+      <c r="D176" s="58"/>
+      <c r="E176" s="58"/>
+      <c r="F176" s="57"/>
+      <c r="G176" s="57"/>
+      <c r="H176" s="57">
+        <v>2</v>
+      </c>
+      <c r="I176" s="57"/>
+      <c r="J176" s="57"/>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B177" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="H177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B177" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C177" s="8"/>
+      <c r="D177" s="8"/>
+      <c r="E177" s="8"/>
+      <c r="H177" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="F178" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="H178">
         <v>0</v>
       </c>
-      <c r="I178" s="6">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>269</v>
+        <v>224</v>
+      </c>
+      <c r="F179" t="s">
+        <v>138</v>
       </c>
       <c r="H179">
         <v>0</v>
       </c>
-      <c r="I179" s="6"/>
-    </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I179" s="6">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="G180" t="s">
-        <v>138</v>
+        <v>269</v>
       </c>
       <c r="H180">
         <v>0</v>
       </c>
       <c r="I180" s="6"/>
     </row>
-    <row r="181" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B181" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C181" s="13"/>
-      <c r="D181" s="13"/>
-      <c r="E181" s="13"/>
-      <c r="H181" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B181" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="G181" t="s">
+        <v>138</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+      <c r="I181" s="6"/>
+    </row>
+    <row r="182" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="C182" s="13"/>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
-      <c r="G182" t="s">
+      <c r="H182" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B183" s="55" t="s">
+        <v>254</v>
+      </c>
+      <c r="C183" s="55"/>
+      <c r="D183" s="55"/>
+      <c r="E183" s="55"/>
+      <c r="F183" s="52"/>
+      <c r="G183" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="H182" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="12" t="s">
+      <c r="H183" s="52">
+        <v>2</v>
+      </c>
+      <c r="I183" s="52"/>
+      <c r="J183" s="52"/>
+    </row>
+    <row r="184" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B183" s="13" t="s">
+      <c r="B184" s="55" t="s">
         <v>257</v>
       </c>
-      <c r="C183" s="13"/>
-      <c r="D183" s="13"/>
-      <c r="E183" s="13"/>
-      <c r="G183" t="s">
+      <c r="C184" s="55"/>
+      <c r="D184" s="55"/>
+      <c r="E184" s="55"/>
+      <c r="F184" s="52"/>
+      <c r="G184" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="H183" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B184" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="G184" t="s">
-        <v>138</v>
-      </c>
-      <c r="H184">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H184" s="52">
+        <v>2</v>
+      </c>
+      <c r="I184" s="52"/>
+      <c r="J184" s="52"/>
+    </row>
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B185" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C185" s="13"/>
-      <c r="D185" s="13"/>
-      <c r="E185" s="13"/>
-      <c r="H185" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B185" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G185" t="s">
+        <v>138</v>
+      </c>
+      <c r="H185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B186" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="H186">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B186" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C186" s="13"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="13"/>
+      <c r="H186" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B187" s="13" t="s">
+      <c r="B187" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B188" s="13" t="s">
         <v>118</v>
-      </c>
-      <c r="C187" s="13"/>
-      <c r="D187" s="13"/>
-      <c r="E187" s="13"/>
-      <c r="F187" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H187" s="12">
-        <v>0</v>
-      </c>
-      <c r="I187" s="14">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B188" s="13" t="s">
-        <v>344</v>
       </c>
       <c r="C188" s="13"/>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
+      <c r="F188" s="12" t="s">
+        <v>133</v>
+      </c>
       <c r="H188" s="12">
-        <v>2</v>
-      </c>
-      <c r="I188" s="14"/>
-    </row>
-    <row r="189" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B189" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I188" s="14">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="52"/>
+      <c r="B189" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="C189" s="55"/>
+      <c r="D189" s="55"/>
+      <c r="E189" s="55"/>
+      <c r="F189" s="52"/>
+      <c r="G189" s="52"/>
+      <c r="H189" s="52">
+        <v>2</v>
+      </c>
+      <c r="I189" s="61"/>
+      <c r="J189" s="52"/>
+    </row>
+    <row r="190" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="52"/>
+      <c r="B190" s="55" t="s">
         <v>398</v>
       </c>
-      <c r="C189" s="13"/>
-      <c r="D189" s="13"/>
-      <c r="E189" s="13"/>
-      <c r="H189" s="12">
+      <c r="C190" s="55"/>
+      <c r="D190" s="55"/>
+      <c r="E190" s="55"/>
+      <c r="F190" s="52"/>
+      <c r="G190" s="52"/>
+      <c r="H190" s="52">
         <v>1</v>
       </c>
-      <c r="I189" s="14"/>
-    </row>
-    <row r="190" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B190" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="C190" s="15"/>
-      <c r="D190" s="15"/>
-      <c r="E190" s="15"/>
-      <c r="F190" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H190" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I190" s="14"/>
-    </row>
-    <row r="191" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I190" s="61"/>
+      <c r="J190" s="52"/>
+    </row>
+    <row r="191" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B191" s="18" t="s">
-        <v>402</v>
+      <c r="B191" s="15" t="s">
+        <v>259</v>
       </c>
       <c r="C191" s="15"/>
       <c r="D191" s="15"/>
       <c r="E191" s="15"/>
-      <c r="H191" s="12">
+      <c r="F191" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H191" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I191" s="14"/>
+    </row>
+    <row r="192" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="I191" s="14"/>
-    </row>
-    <row r="192" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="12" t="s">
+      <c r="B192" s="53" t="s">
+        <v>402</v>
+      </c>
+      <c r="C192" s="65"/>
+      <c r="D192" s="65"/>
+      <c r="E192" s="65"/>
+      <c r="F192" s="52"/>
+      <c r="G192" s="52"/>
+      <c r="H192" s="52">
         <v>1</v>
       </c>
-      <c r="B192" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="C192" s="15"/>
-      <c r="D192" s="15"/>
-      <c r="E192" s="15"/>
-      <c r="H192" s="12">
-        <v>0</v>
-      </c>
-      <c r="I192" s="14"/>
-    </row>
-    <row r="193" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I192" s="61"/>
+      <c r="J192" s="52"/>
+    </row>
+    <row r="193" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B193" s="18" t="s">
-        <v>324</v>
+        <v>345</v>
       </c>
       <c r="C193" s="15"/>
       <c r="D193" s="15"/>
       <c r="E193" s="15"/>
+      <c r="H193" s="12">
+        <v>0</v>
+      </c>
       <c r="I193" s="14"/>
     </row>
-    <row r="194" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B194" s="15" t="s">
-        <v>261</v>
+      <c r="B194" s="18" t="s">
+        <v>324</v>
       </c>
       <c r="C194" s="15"/>
       <c r="D194" s="15"/>
       <c r="E194" s="15"/>
-      <c r="F194" s="12" t="s">
+      <c r="I194" s="14"/>
+    </row>
+    <row r="195" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B195" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="C195" s="65"/>
+      <c r="D195" s="65"/>
+      <c r="E195" s="65"/>
+      <c r="F195" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="H194" s="12">
-        <v>2</v>
-      </c>
-      <c r="I194" s="14"/>
-    </row>
-    <row r="195" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="12" t="s">
+      <c r="G195" s="52"/>
+      <c r="H195" s="52">
+        <v>2</v>
+      </c>
+      <c r="I195" s="61"/>
+      <c r="J195" s="52"/>
+    </row>
+    <row r="196" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B195" s="18" t="s">
+      <c r="B196" s="53" t="s">
         <v>327</v>
       </c>
-      <c r="C195" s="15"/>
-      <c r="D195" s="15"/>
-      <c r="E195" s="15"/>
-      <c r="H195" s="12">
-        <v>2</v>
-      </c>
-      <c r="I195" s="14"/>
-    </row>
-    <row r="196" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B196" s="15" t="s">
-        <v>325</v>
-      </c>
-      <c r="C196" s="15"/>
-      <c r="D196" s="15"/>
-      <c r="E196" s="15"/>
-      <c r="I196" s="14"/>
-    </row>
-    <row r="197" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C196" s="65"/>
+      <c r="D196" s="65"/>
+      <c r="E196" s="65"/>
+      <c r="F196" s="52"/>
+      <c r="G196" s="52"/>
+      <c r="H196" s="52">
+        <v>2</v>
+      </c>
+      <c r="I196" s="61"/>
+      <c r="J196" s="52"/>
+    </row>
+    <row r="197" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B197" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C197" s="15"/>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
       <c r="I197" s="14"/>
     </row>
-    <row r="198" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B198" s="15" t="s">
-        <v>270</v>
+        <v>326</v>
       </c>
       <c r="C198" s="15"/>
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
       <c r="I198" s="14"/>
     </row>
-    <row r="199" spans="1:9" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B199" s="13" t="s">
+      <c r="B199" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="C199" s="15"/>
+      <c r="D199" s="15"/>
+      <c r="E199" s="15"/>
+      <c r="I199" s="14"/>
+    </row>
+    <row r="200" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B200" s="55" t="s">
         <v>253</v>
       </c>
-      <c r="C199" s="13"/>
-      <c r="D199" s="13"/>
-      <c r="E199" s="13"/>
-      <c r="F199" s="12" t="s">
+      <c r="C200" s="55"/>
+      <c r="D200" s="55"/>
+      <c r="E200" s="55"/>
+      <c r="F200" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="H199" s="12">
+      <c r="G200" s="52"/>
+      <c r="H200" s="52">
         <v>3</v>
       </c>
-      <c r="I199" s="14"/>
-    </row>
-    <row r="200" spans="1:9" ht="21" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A200" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="B200" s="16" t="s">
-        <v>319</v>
-      </c>
-      <c r="I200" s="6"/>
-    </row>
-    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I200" s="61"/>
+      <c r="J200" s="52"/>
+    </row>
+    <row r="201" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A201" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="B201" s="7" t="s">
+      <c r="B201" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="I201" s="6"/>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" s="52" t="s">
+        <v>333</v>
+      </c>
+      <c r="B202" s="58" t="s">
         <v>320</v>
       </c>
-      <c r="H201">
+      <c r="C202" s="58"/>
+      <c r="D202" s="58"/>
+      <c r="E202" s="58"/>
+      <c r="F202" s="57"/>
+      <c r="G202" s="57"/>
+      <c r="H202" s="57">
         <v>3</v>
       </c>
-      <c r="I201" s="6"/>
-    </row>
-    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="12" t="s">
+      <c r="I202" s="60"/>
+      <c r="J202" s="57"/>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="B202" s="7" t="s">
+      <c r="B203" s="58" t="s">
         <v>321</v>
       </c>
-      <c r="H202">
+      <c r="C203" s="58"/>
+      <c r="D203" s="58"/>
+      <c r="E203" s="58"/>
+      <c r="F203" s="57"/>
+      <c r="G203" s="57"/>
+      <c r="H203" s="57">
         <v>3</v>
       </c>
-      <c r="I202" s="6"/>
-    </row>
-    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="12" t="s">
+      <c r="I203" s="60"/>
+      <c r="J203" s="57"/>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="B203" s="7" t="s">
+      <c r="B204" s="58" t="s">
         <v>336</v>
       </c>
-      <c r="H203">
+      <c r="C204" s="58"/>
+      <c r="D204" s="58"/>
+      <c r="E204" s="58"/>
+      <c r="F204" s="57"/>
+      <c r="G204" s="57"/>
+      <c r="H204" s="57">
         <v>3</v>
       </c>
-      <c r="I203" s="6"/>
-    </row>
-    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="12" t="s">
+      <c r="I204" s="60"/>
+      <c r="J204" s="57"/>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="B204" s="7" t="s">
+      <c r="B205" s="58" t="s">
         <v>331</v>
       </c>
-      <c r="H204">
+      <c r="C205" s="58"/>
+      <c r="D205" s="58"/>
+      <c r="E205" s="58"/>
+      <c r="F205" s="57"/>
+      <c r="G205" s="57"/>
+      <c r="H205" s="57">
         <v>3</v>
       </c>
-      <c r="I204" s="6"/>
-    </row>
-    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="B205" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="H205">
-        <v>0</v>
-      </c>
-      <c r="I205" s="6"/>
-    </row>
-    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I205" s="60"/>
+      <c r="J205" s="57"/>
+    </row>
+    <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="12" t="s">
         <v>333</v>
       </c>
       <c r="B206" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="H206">
+        <v>0</v>
+      </c>
+      <c r="I206" s="6"/>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" s="52" t="s">
+        <v>333</v>
+      </c>
+      <c r="B207" s="58" t="s">
         <v>360</v>
       </c>
-      <c r="H206">
-        <v>2</v>
-      </c>
-      <c r="I206" s="6"/>
-    </row>
-    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="12" t="s">
+      <c r="C207" s="58"/>
+      <c r="D207" s="58"/>
+      <c r="E207" s="58"/>
+      <c r="F207" s="57"/>
+      <c r="G207" s="57"/>
+      <c r="H207" s="57">
+        <v>2</v>
+      </c>
+      <c r="I207" s="60"/>
+      <c r="J207" s="57"/>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="B207" s="7" t="s">
+      <c r="B208" s="58" t="s">
         <v>338</v>
       </c>
-      <c r="H207">
+      <c r="C208" s="58"/>
+      <c r="D208" s="58"/>
+      <c r="E208" s="58"/>
+      <c r="F208" s="57"/>
+      <c r="G208" s="57"/>
+      <c r="H208" s="57">
         <v>3</v>
       </c>
-      <c r="I207" s="6"/>
-    </row>
-    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="12" t="s">
+      <c r="I208" s="60"/>
+      <c r="J208" s="57"/>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A209" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="B208" s="7" t="s">
+      <c r="B209" s="58" t="s">
         <v>339</v>
       </c>
-      <c r="H208">
+      <c r="C209" s="58"/>
+      <c r="D209" s="58"/>
+      <c r="E209" s="58"/>
+      <c r="F209" s="57"/>
+      <c r="G209" s="57"/>
+      <c r="H209" s="57">
         <v>3</v>
       </c>
-      <c r="I208" s="6"/>
-    </row>
-    <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="12" t="s">
+      <c r="I209" s="60"/>
+      <c r="J209" s="57"/>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A210" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="B209" s="7" t="s">
+      <c r="B210" s="58" t="s">
         <v>337</v>
       </c>
-      <c r="H209">
+      <c r="C210" s="58"/>
+      <c r="D210" s="58"/>
+      <c r="E210" s="58"/>
+      <c r="F210" s="57"/>
+      <c r="G210" s="57"/>
+      <c r="H210" s="57">
         <v>3</v>
       </c>
-      <c r="I209" s="6"/>
-    </row>
-    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="12"/>
-      <c r="B210" s="7" t="s">
+      <c r="I210" s="60"/>
+      <c r="J210" s="57"/>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A211" s="12"/>
+      <c r="B211" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="I210" s="6"/>
-    </row>
-    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="12"/>
       <c r="I211" s="6"/>
     </row>
-    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="12"/>
-      <c r="B212" s="7" t="s">
-        <v>378</v>
-      </c>
       <c r="I212" s="6"/>
     </row>
-    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="12"/>
       <c r="B213" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I213" s="6"/>
     </row>
-    <row r="214" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="I214" s="6"/>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215" s="12"/>
+      <c r="B215" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="I214" s="6"/>
-    </row>
-    <row r="215" spans="1:10" ht="21" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B215" s="16" t="s">
+      <c r="I215" s="6"/>
+    </row>
+    <row r="216" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B216" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="I215" s="6"/>
-    </row>
-    <row r="216" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B216" s="15" t="s">
+      <c r="I216" s="6"/>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B217" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="I216" s="6"/>
-    </row>
-    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B217" s="7" t="s">
+      <c r="I217" s="6"/>
+    </row>
+    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B218" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="H217">
-        <v>0</v>
-      </c>
-      <c r="I217" s="6"/>
-    </row>
-    <row r="218" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H218">
+        <v>0</v>
+      </c>
       <c r="I218" s="6"/>
     </row>
-    <row r="219" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="B219" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="C219" s="15"/>
-      <c r="D219" s="15"/>
-      <c r="E219" s="15"/>
-      <c r="I219" s="14"/>
-    </row>
-    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I219" s="6"/>
+    </row>
+    <row r="220" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A220" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="B220" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F220" t="s">
-        <v>133</v>
-      </c>
-      <c r="H220">
-        <v>0</v>
-      </c>
+      <c r="B220" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="C220" s="15"/>
+      <c r="D220" s="15"/>
+      <c r="E220" s="15"/>
+      <c r="I220" s="14"/>
     </row>
     <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>315</v>
       </c>
       <c r="B221" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F221" t="s">
+        <v>133</v>
+      </c>
+      <c r="H221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="B222" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="H221">
+      <c r="H222">
         <v>9</v>
       </c>
-      <c r="J221" t="s">
+      <c r="J222" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="12"/>
-      <c r="B222" s="7" t="s">
+    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="12"/>
+      <c r="B223" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="H222">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="B223" s="7" t="s">
-        <v>329</v>
       </c>
       <c r="H223">
         <v>0</v>
@@ -5718,53 +6005,60 @@
         <v>315</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>255</v>
+        <v>329</v>
       </c>
       <c r="H224">
         <v>0</v>
       </c>
-      <c r="I224" s="6"/>
     </row>
     <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
         <v>315</v>
       </c>
       <c r="B225" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="H225">
+        <v>0</v>
+      </c>
+      <c r="I225" s="6"/>
+    </row>
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="B226" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="H225">
-        <v>0</v>
-      </c>
-      <c r="J225" t="s">
+      <c r="H226">
+        <v>0</v>
+      </c>
+      <c r="J226" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="12"/>
-      <c r="B226" s="7" t="s">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A227" s="52"/>
+      <c r="B227" s="58" t="s">
         <v>346</v>
       </c>
-      <c r="H226">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="B227" s="8" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C227" s="58"/>
+      <c r="D227" s="58"/>
+      <c r="E227" s="58"/>
+      <c r="F227" s="57"/>
+      <c r="G227" s="57"/>
+      <c r="H227" s="57">
+        <v>2</v>
+      </c>
+      <c r="I227" s="57"/>
+      <c r="J227" s="57"/>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="B228" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="H228">
-        <v>0</v>
+      <c r="B228" s="8" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -5772,31 +6066,22 @@
         <v>297</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F229" t="s">
-        <v>133</v>
+        <v>298</v>
       </c>
       <c r="H229">
         <v>0</v>
-      </c>
-      <c r="I229" s="6">
-        <v>42702</v>
-      </c>
-      <c r="J229" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="B230" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C230" s="9"/>
-      <c r="D230" s="9"/>
-      <c r="E230" s="9"/>
+      <c r="B230" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F230" t="s">
+        <v>133</v>
+      </c>
       <c r="H230">
         <v>0</v>
       </c>
@@ -5811,17 +6096,20 @@
       <c r="A231" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="B231" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F231" t="s">
-        <v>133</v>
-      </c>
+      <c r="B231" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C231" s="9"/>
+      <c r="D231" s="9"/>
+      <c r="E231" s="9"/>
       <c r="H231">
         <v>0</v>
       </c>
       <c r="I231" s="6">
         <v>42702</v>
+      </c>
+      <c r="J231" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -5829,13 +6117,16 @@
         <v>297</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="F232" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H232">
         <v>0</v>
+      </c>
+      <c r="I232" s="6">
+        <v>42702</v>
       </c>
     </row>
     <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -5843,19 +6134,13 @@
         <v>297</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F233" t="s">
         <v>135</v>
       </c>
       <c r="H233">
         <v>0</v>
-      </c>
-      <c r="I233" s="6">
-        <v>42697</v>
-      </c>
-      <c r="J233" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -5863,486 +6148,582 @@
         <v>297</v>
       </c>
       <c r="B234" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F234" t="s">
+        <v>135</v>
+      </c>
+      <c r="H234">
+        <v>0</v>
+      </c>
+      <c r="I234" s="6">
+        <v>42697</v>
+      </c>
+      <c r="J234" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B235" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="H234">
-        <v>0</v>
-      </c>
-      <c r="I234" s="6"/>
-    </row>
-    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="12"/>
-      <c r="B235" s="13" t="s">
+      <c r="H235">
+        <v>0</v>
+      </c>
+      <c r="I235" s="6"/>
+    </row>
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="12"/>
+      <c r="B236" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="H235">
+      <c r="H236">
         <v>9</v>
       </c>
-      <c r="I235" s="6"/>
-    </row>
-    <row r="236" spans="1:10" ht="21" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B236" s="16" t="s">
+      <c r="I236" s="6"/>
+    </row>
+    <row r="237" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B237" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C236" s="16"/>
-      <c r="D236" s="16"/>
-      <c r="E236" s="16"/>
-    </row>
-    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B237" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="H237">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B238" t="s">
-        <v>313</v>
-      </c>
-      <c r="C238" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="D238" s="26">
-        <v>42775</v>
-      </c>
-      <c r="E238" s="26"/>
+      <c r="C237" s="16"/>
+      <c r="D237" s="16"/>
+      <c r="E237" s="16"/>
+    </row>
+    <row r="238" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B238" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="C238" s="16"/>
+      <c r="D238" s="16"/>
+      <c r="E238" s="16"/>
       <c r="H238">
         <v>2</v>
       </c>
     </row>
-    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B239" s="7" t="s">
-        <v>347</v>
-      </c>
-      <c r="H239">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B240" t="s">
-        <v>305</v>
-      </c>
-      <c r="C240" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="D240" s="26">
-        <v>42775</v>
-      </c>
-      <c r="E240" s="26"/>
-      <c r="H240">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B241" s="7" t="s">
-        <v>382</v>
-      </c>
+    <row r="239" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B239" s="16"/>
+      <c r="C239" s="16"/>
+      <c r="D239" s="16"/>
+      <c r="E239" s="16"/>
+    </row>
+    <row r="240" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B240" s="64" t="s">
+        <v>422</v>
+      </c>
+      <c r="C240" s="16"/>
+      <c r="D240" s="16"/>
+      <c r="E240" s="16"/>
+    </row>
+    <row r="241" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B241" s="57" t="s">
+        <v>423</v>
+      </c>
+      <c r="C241" s="16"/>
+      <c r="D241" s="16"/>
+      <c r="E241" s="16"/>
       <c r="H241">
         <v>1</v>
       </c>
-      <c r="I241" s="6"/>
-    </row>
-    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B242" s="8" t="s">
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A242" s="57"/>
+      <c r="B242" s="64" t="s">
+        <v>262</v>
+      </c>
+      <c r="C242" s="58"/>
+      <c r="D242" s="58"/>
+      <c r="E242" s="58"/>
+      <c r="F242" s="57"/>
+      <c r="G242" s="57"/>
+      <c r="H242" s="57">
+        <v>2</v>
+      </c>
+      <c r="I242" s="57"/>
+      <c r="J242" s="57"/>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A243" s="57"/>
+      <c r="B243" s="57" t="s">
+        <v>313</v>
+      </c>
+      <c r="C243" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D243" s="59">
+        <v>42775</v>
+      </c>
+      <c r="E243" s="59"/>
+      <c r="F243" s="57"/>
+      <c r="G243" s="57"/>
+      <c r="H243" s="57">
+        <v>2</v>
+      </c>
+      <c r="I243" s="57"/>
+      <c r="J243" s="57"/>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A244" s="57"/>
+      <c r="B244" s="58" t="s">
+        <v>347</v>
+      </c>
+      <c r="C244" s="58"/>
+      <c r="D244" s="58"/>
+      <c r="E244" s="58"/>
+      <c r="F244" s="57"/>
+      <c r="G244" s="57"/>
+      <c r="H244" s="57">
+        <v>1</v>
+      </c>
+      <c r="I244" s="57"/>
+      <c r="J244" s="57"/>
+    </row>
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B245" t="s">
+        <v>305</v>
+      </c>
+      <c r="C245" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D245" s="26">
+        <v>42775</v>
+      </c>
+      <c r="E245" s="26"/>
+      <c r="H245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A246" s="57"/>
+      <c r="B246" s="58" t="s">
+        <v>382</v>
+      </c>
+      <c r="C246" s="58"/>
+      <c r="D246" s="58"/>
+      <c r="E246" s="58"/>
+      <c r="F246" s="57"/>
+      <c r="G246" s="57"/>
+      <c r="H246" s="57">
+        <v>0</v>
+      </c>
+      <c r="I246" s="60"/>
+      <c r="J246" s="57"/>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B247" s="8" t="s">
         <v>356</v>
       </c>
-      <c r="I242" s="6"/>
-    </row>
-    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B243" s="7" t="s">
+      <c r="I247" s="6"/>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A248" s="57"/>
+      <c r="B248" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="H243">
+      <c r="C248" s="58"/>
+      <c r="D248" s="58"/>
+      <c r="E248" s="58"/>
+      <c r="F248" s="57"/>
+      <c r="G248" s="57"/>
+      <c r="H248" s="57">
         <v>1</v>
       </c>
-      <c r="I243" s="6"/>
-    </row>
-    <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B244" s="7" t="s">
+      <c r="I248" s="60"/>
+      <c r="J248" s="57"/>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A249" s="57"/>
+      <c r="B249" s="58" t="s">
         <v>358</v>
       </c>
-      <c r="H244">
+      <c r="C249" s="58"/>
+      <c r="D249" s="58"/>
+      <c r="E249" s="58"/>
+      <c r="F249" s="57"/>
+      <c r="G249" s="57"/>
+      <c r="H249" s="57">
+        <v>2</v>
+      </c>
+      <c r="I249" s="60"/>
+      <c r="J249" s="57"/>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A250" s="57"/>
+      <c r="B250" s="58" t="s">
+        <v>359</v>
+      </c>
+      <c r="C250" s="58"/>
+      <c r="D250" s="58"/>
+      <c r="E250" s="58"/>
+      <c r="F250" s="57"/>
+      <c r="G250" s="57"/>
+      <c r="H250" s="57">
+        <v>2</v>
+      </c>
+      <c r="I250" s="60"/>
+      <c r="J250" s="57"/>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B251" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="I251" s="6"/>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A252" s="57"/>
+      <c r="B252" s="58" t="s">
+        <v>355</v>
+      </c>
+      <c r="C252" s="58"/>
+      <c r="D252" s="58"/>
+      <c r="E252" s="58"/>
+      <c r="F252" s="57"/>
+      <c r="G252" s="57"/>
+      <c r="H252" s="57">
+        <v>2</v>
+      </c>
+      <c r="I252" s="60"/>
+      <c r="J252" s="57"/>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A253" s="57"/>
+      <c r="B253" s="58" t="s">
+        <v>399</v>
+      </c>
+      <c r="C253" s="58"/>
+      <c r="D253" s="58"/>
+      <c r="E253" s="58"/>
+      <c r="F253" s="57"/>
+      <c r="G253" s="57"/>
+      <c r="H253" s="57">
+        <v>2</v>
+      </c>
+      <c r="I253" s="60"/>
+      <c r="J253" s="57"/>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A254" s="57"/>
+      <c r="B254" s="58" t="s">
+        <v>400</v>
+      </c>
+      <c r="C254" s="58"/>
+      <c r="D254" s="58"/>
+      <c r="E254" s="58"/>
+      <c r="F254" s="57"/>
+      <c r="G254" s="57"/>
+      <c r="H254" s="57">
+        <v>2</v>
+      </c>
+      <c r="I254" s="60"/>
+      <c r="J254" s="57"/>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A255" s="57"/>
+      <c r="B255" s="58" t="s">
+        <v>401</v>
+      </c>
+      <c r="C255" s="58"/>
+      <c r="D255" s="58"/>
+      <c r="E255" s="58"/>
+      <c r="F255" s="57"/>
+      <c r="G255" s="57"/>
+      <c r="H255" s="57">
+        <v>2</v>
+      </c>
+      <c r="I255" s="60"/>
+      <c r="J255" s="57"/>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B256" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C256" s="8"/>
+      <c r="D256" s="8"/>
+      <c r="E256" s="8"/>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>1</v>
+      </c>
+      <c r="B257" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="F257" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>2</v>
+      </c>
+      <c r="B258" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F258" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A259">
         <v>3</v>
       </c>
-      <c r="I244" s="6"/>
-    </row>
-    <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B245" s="7" t="s">
-        <v>359</v>
-      </c>
-      <c r="H245">
+      <c r="B259" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="F259" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>4</v>
+      </c>
+      <c r="B260" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>174</v>
+      </c>
+      <c r="B261" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="F261" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B262" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F262" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B263" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F263" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B264" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="F264" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B265" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="F265" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B266" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="F266" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B267" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C267" s="10"/>
+      <c r="D267" s="10"/>
+      <c r="E267" s="10"/>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B268" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F268" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B269" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B270" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B271" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B272" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B273" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F273" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="274" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B274" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="275" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B275" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="F275" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B276" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F276" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B277" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C277" s="10"/>
+      <c r="D277" s="10"/>
+      <c r="E277" s="10"/>
+    </row>
+    <row r="278" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B278" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F278" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B279" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F279" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="280" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B280" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B281" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>1</v>
+      </c>
+      <c r="B282" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="H282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>2</v>
+      </c>
+      <c r="B283" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A284" s="57"/>
+      <c r="B284" s="58" t="s">
+        <v>198</v>
+      </c>
+      <c r="C284" s="58"/>
+      <c r="D284" s="58"/>
+      <c r="E284" s="58"/>
+      <c r="F284" s="57"/>
+      <c r="G284" s="57"/>
+      <c r="H284" s="57">
+        <v>2</v>
+      </c>
+      <c r="I284" s="57"/>
+      <c r="J284" s="57"/>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A285" s="57"/>
+      <c r="B285" s="58" t="s">
+        <v>199</v>
+      </c>
+      <c r="C285" s="58"/>
+      <c r="D285" s="58"/>
+      <c r="E285" s="58"/>
+      <c r="F285" s="57"/>
+      <c r="G285" s="57"/>
+      <c r="H285" s="57">
+        <v>2</v>
+      </c>
+      <c r="I285" s="57"/>
+      <c r="J285" s="57"/>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A286" s="57"/>
+      <c r="B286" s="58" t="s">
+        <v>200</v>
+      </c>
+      <c r="C286" s="58"/>
+      <c r="D286" s="58"/>
+      <c r="E286" s="58"/>
+      <c r="F286" s="57"/>
+      <c r="G286" s="57"/>
+      <c r="H286" s="57">
         <v>3</v>
       </c>
-      <c r="I245" s="6"/>
-    </row>
-    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B246" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="I246" s="6"/>
-    </row>
-    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="7" t="s">
-        <v>355</v>
-      </c>
-      <c r="H247">
-        <v>2</v>
-      </c>
-      <c r="I247" s="6"/>
-    </row>
-    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B248" s="7" t="s">
-        <v>399</v>
-      </c>
-      <c r="H248">
-        <v>2</v>
-      </c>
-      <c r="I248" s="6"/>
-    </row>
-    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B249" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="H249">
-        <v>2</v>
-      </c>
-      <c r="I249" s="6"/>
-    </row>
-    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B250" s="7" t="s">
-        <v>401</v>
-      </c>
-      <c r="H250">
-        <v>2</v>
-      </c>
-      <c r="I250" s="6"/>
-    </row>
-    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="C251" s="8"/>
-      <c r="D251" s="8"/>
-      <c r="E251" s="8"/>
-    </row>
-    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A252">
-        <v>1</v>
-      </c>
-      <c r="B252" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="F252" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="253" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A253">
-        <v>2</v>
-      </c>
-      <c r="B253" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="F253" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A254">
-        <v>3</v>
-      </c>
-      <c r="B254" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="F254" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A255">
-        <v>4</v>
-      </c>
-      <c r="B255" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>174</v>
-      </c>
-      <c r="B256" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="F256" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="257" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B257" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="F257" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="258" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B258" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="F258" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="259" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B259" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="F259" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="260" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B260" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="F260" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="261" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B261" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="F261" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="262" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B262" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C262" s="10"/>
-      <c r="D262" s="10"/>
-      <c r="E262" s="10"/>
-    </row>
-    <row r="263" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B263" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="F263" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="264" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B264" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="265" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B265" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="266" spans="2:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B266" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="267" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B267" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="268" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B268" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="F268" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="269" spans="2:6" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B269" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="270" spans="2:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B270" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="F270" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="271" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B271" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F271" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="272" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B272" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C272" s="10"/>
-      <c r="D272" s="10"/>
-      <c r="E272" s="10"/>
-    </row>
-    <row r="273" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B273" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="F273" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="274" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B274" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F274" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="275" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B275" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B276" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A277">
-        <v>1</v>
-      </c>
-      <c r="B277" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="H277">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A278">
-        <v>2</v>
-      </c>
-      <c r="B278" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B279" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="H279">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B280" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="H280">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B281" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="H281">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="282" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B282" s="7" t="s">
+      <c r="I286" s="57"/>
+      <c r="J286" s="57"/>
+    </row>
+    <row r="287" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B287" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="H282">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B283" s="7" t="s">
+      <c r="H287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B288" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="H283">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B284" s="7" t="s">
+      <c r="H288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B289" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="F284" t="s">
+      <c r="F289" t="s">
         <v>219</v>
-      </c>
-      <c r="H284">
-        <v>0</v>
-      </c>
-      <c r="I284" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B285" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="F285" t="s">
-        <v>220</v>
-      </c>
-      <c r="H285">
-        <v>0</v>
-      </c>
-      <c r="I285" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B286" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F286" t="s">
-        <v>221</v>
-      </c>
-      <c r="H286">
-        <v>0</v>
-      </c>
-      <c r="I286" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="287" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B287" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="H287">
-        <v>0</v>
-      </c>
-      <c r="I287" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B288" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="H288">
-        <v>0</v>
-      </c>
-      <c r="I288" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="289" spans="2:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B289" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="H289">
         <v>0</v>
@@ -6351,16 +6732,91 @@
         <v>144</v>
       </c>
     </row>
-    <row r="291" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B290" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F290" t="s">
+        <v>220</v>
+      </c>
+      <c r="H290">
+        <v>0</v>
+      </c>
+      <c r="I290" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B291" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="F291" t="s">
+        <v>221</v>
+      </c>
+      <c r="H291">
+        <v>0</v>
+      </c>
+      <c r="I291" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B292" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="H292">
+        <v>0</v>
+      </c>
+      <c r="I292" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B293" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H293">
+        <v>0</v>
+      </c>
+      <c r="I293" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B294" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H294">
+        <v>0</v>
+      </c>
+      <c r="I294" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A295" s="57"/>
+      <c r="B295" s="58"/>
+      <c r="C295" s="58"/>
+      <c r="D295" s="58"/>
+      <c r="E295" s="58"/>
+      <c r="F295" s="57"/>
+      <c r="G295" s="57"/>
+      <c r="H295" s="57"/>
+      <c r="I295" s="57"/>
+      <c r="J295" s="57"/>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B296" s="7" t="s">
         <v>218</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:J289">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="ICON"/>
+  <autoFilter ref="A7:J294">
+    <filterColumn colId="7">
+      <filters blank="1">
+        <filter val="1"/>
+        <filter val="2"/>
+        <filter val="3"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Bug Corrections in data Extractor Devp Institute Fingins WIP
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -13,14 +13,14 @@
     <sheet name="Actions - Post - Demo1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$J$293</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Actions - Post - Demo1'!$A$7:$J$298</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="426">
   <si>
     <t>Reports</t>
   </si>
@@ -1430,12 +1430,6 @@
     <t>Sam Site Converting from Live to DB</t>
   </si>
   <si>
-    <t>Clarifications required from ICON</t>
-  </si>
-  <si>
-    <t>WIP</t>
-  </si>
-  <si>
     <t>Institute related Findings - Changes in Compliance Form</t>
   </si>
   <si>
@@ -1443,6 +1437,24 @@
   </si>
   <si>
     <t>Authroisation in API Controllers</t>
+  </si>
+  <si>
+    <t>Sort List in descending oder</t>
+  </si>
+  <si>
+    <t>The Source Date of SDN website (12th site in ICSF) is displaying wrong date as 17th Mar instead of the correct one 13th Apr.</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Incorect Page Number in footer.  ICSFs going more than 2 pages are having the pagination error and could you please see if this could be fixed by any means.</t>
+  </si>
+  <si>
+    <t>User List in pop up must be in alphabetical order</t>
   </si>
 </sst>
 </file>
@@ -2745,18 +2757,18 @@
   <sheetPr filterMode="1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K295"/>
+  <dimension ref="A1:K300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B247" sqref="B247"/>
+      <selection pane="bottomRight" activeCell="H179" sqref="H179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.85546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" style="7" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" style="7" customWidth="1"/>
@@ -4420,108 +4432,114 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="8" t="s">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="12"/>
+      <c r="B106" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D106" s="26">
+        <v>42845</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-      <c r="H106" t="s">
+      <c r="C107" s="8"/>
+      <c r="D107" s="8"/>
+      <c r="E107" s="8"/>
+      <c r="H107" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="9" t="s">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="C107" s="9"/>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9"/>
-      <c r="H107">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B108" s="24" t="s">
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="H108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="C108" s="19" t="s">
+      <c r="C109" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="D108" s="19">
+      <c r="D109" s="19">
         <v>42760</v>
       </c>
-      <c r="E108" s="19"/>
-      <c r="H108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A109" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" s="10" t="s">
+      <c r="E109" s="19"/>
+      <c r="H109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="C109" s="9"/>
-      <c r="D109" s="9"/>
-      <c r="E109" s="9"/>
-      <c r="H109" t="s">
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="H110" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B110" s="7" t="s">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="H110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" s="20" t="s">
+      <c r="H111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="20" t="s">
         <v>281</v>
       </c>
-      <c r="C111" s="19" t="s">
+      <c r="C112" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="D111" s="19">
+      <c r="D112" s="19">
         <v>42760</v>
       </c>
-      <c r="E111" s="19"/>
-      <c r="H111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A112" s="12"/>
-      <c r="B112" s="20" t="s">
-        <v>342</v>
-      </c>
-      <c r="C112" s="19"/>
-      <c r="D112" s="19"/>
       <c r="E112" s="19"/>
+      <c r="H112">
+        <v>0</v>
+      </c>
     </row>
     <row r="113" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="12"/>
       <c r="B113" s="20" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C113" s="19"/>
       <c r="D113" s="19"/>
@@ -4530,164 +4548,136 @@
     <row r="114" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="12"/>
       <c r="B114" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C114" s="19"/>
       <c r="D114" s="19"/>
       <c r="E114" s="19"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A115" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" s="8" t="s">
+    <row r="115" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A115" s="12"/>
+      <c r="B115" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="C115" s="19"/>
+      <c r="D115" s="19"/>
+      <c r="E115" s="19"/>
+    </row>
+    <row r="116" spans="1:11" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="12"/>
+      <c r="B116" s="20" t="s">
+        <v>420</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D116" s="26">
+        <v>42845</v>
+      </c>
+      <c r="E116" s="19"/>
+      <c r="H116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>353</v>
       </c>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-    </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B116" s="7" t="s">
+      <c r="C117" s="8"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
+    </row>
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="H116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B117" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="H117">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B118" s="58" t="s">
-        <v>267</v>
-      </c>
-      <c r="C118" s="58"/>
-      <c r="D118" s="58"/>
-      <c r="E118" s="58"/>
-      <c r="F118" s="57"/>
-      <c r="G118" s="57"/>
-      <c r="H118" s="57">
-        <v>2</v>
-      </c>
-      <c r="I118" s="57"/>
-      <c r="J118" s="57"/>
+      <c r="H118">
+        <v>0</v>
+      </c>
     </row>
     <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B119" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="H119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="58" t="s">
+        <v>267</v>
+      </c>
+      <c r="C120" s="58"/>
+      <c r="D120" s="58"/>
+      <c r="E120" s="58"/>
+      <c r="F120" s="57"/>
+      <c r="G120" s="57"/>
+      <c r="H120" s="57">
+        <v>2</v>
+      </c>
+      <c r="I120" s="57"/>
+      <c r="J120" s="57"/>
+    </row>
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="H119">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B120" s="7" t="s">
+      <c r="H121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B122" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="H120">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A121" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B121" s="8" t="s">
+      <c r="H122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B123" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A122" s="52"/>
-      <c r="B122" s="54" t="s">
-        <v>416</v>
-      </c>
-      <c r="C122" s="54" t="s">
-        <v>397</v>
-      </c>
-      <c r="D122" s="63">
-        <v>42831</v>
-      </c>
-      <c r="E122" s="64"/>
-      <c r="F122" s="57" t="s">
-        <v>133</v>
-      </c>
-      <c r="G122" s="57"/>
-      <c r="H122" s="57">
-        <v>1</v>
-      </c>
-      <c r="I122" s="60">
-        <v>42842</v>
-      </c>
-      <c r="J122" s="57" t="s">
-        <v>418</v>
-      </c>
-      <c r="K122" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="12"/>
-      <c r="B123" s="43" t="s">
-        <v>408</v>
-      </c>
-      <c r="C123" s="43" t="s">
-        <v>397</v>
-      </c>
-      <c r="D123" s="44">
-        <v>42831</v>
-      </c>
-      <c r="E123" s="45"/>
-      <c r="F123" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="G123" s="46"/>
-      <c r="H123" s="46">
-        <v>0</v>
-      </c>
-      <c r="I123" s="47">
-        <v>42834</v>
-      </c>
-      <c r="J123" t="s">
-        <v>144</v>
-      </c>
+      <c r="C123" s="8"/>
+      <c r="D123" s="8"/>
+      <c r="E123" s="8"/>
     </row>
     <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="52"/>
       <c r="B124" s="54" t="s">
-        <v>406</v>
-      </c>
-      <c r="C124" s="58" t="s">
+        <v>416</v>
+      </c>
+      <c r="C124" s="54" t="s">
         <v>397</v>
       </c>
-      <c r="D124" s="59">
+      <c r="D124" s="63">
         <v>42831</v>
       </c>
       <c r="E124" s="64"/>
-      <c r="F124" s="57"/>
+      <c r="F124" s="57" t="s">
+        <v>133</v>
+      </c>
       <c r="G124" s="57"/>
       <c r="H124" s="57">
         <v>0</v>
@@ -4698,229 +4688,266 @@
       <c r="J124" s="62" t="s">
         <v>144</v>
       </c>
+      <c r="K124" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="52"/>
-      <c r="B125" s="54" t="s">
-        <v>419</v>
-      </c>
-      <c r="C125" s="58" t="s">
+      <c r="A125" s="12"/>
+      <c r="B125" s="43" t="s">
+        <v>408</v>
+      </c>
+      <c r="C125" s="43" t="s">
         <v>397</v>
       </c>
-      <c r="D125" s="59">
+      <c r="D125" s="44">
         <v>42831</v>
       </c>
-      <c r="E125" s="64"/>
-      <c r="F125" s="52" t="s">
+      <c r="E125" s="45"/>
+      <c r="F125" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="G125" s="46"/>
+      <c r="H125" s="46">
+        <v>0</v>
+      </c>
+      <c r="I125" s="47">
+        <v>42834</v>
+      </c>
+      <c r="J125" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="52"/>
+      <c r="B126" s="54" t="s">
+        <v>406</v>
+      </c>
+      <c r="C126" s="58" t="s">
+        <v>397</v>
+      </c>
+      <c r="D126" s="59">
+        <v>42831</v>
+      </c>
+      <c r="E126" s="64"/>
+      <c r="F126" s="57"/>
+      <c r="G126" s="57"/>
+      <c r="H126" s="57">
+        <v>0</v>
+      </c>
+      <c r="I126" s="60">
+        <v>42842</v>
+      </c>
+      <c r="J126" s="62" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="52"/>
+      <c r="B127" s="54" t="s">
+        <v>417</v>
+      </c>
+      <c r="C127" s="58" t="s">
+        <v>397</v>
+      </c>
+      <c r="D127" s="59">
+        <v>42831</v>
+      </c>
+      <c r="E127" s="64"/>
+      <c r="F127" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="G125" s="57"/>
-      <c r="H125" s="52">
-        <v>0</v>
-      </c>
-      <c r="I125" s="60"/>
-      <c r="J125" s="62"/>
-    </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="12"/>
-      <c r="B126" s="38" t="s">
+      <c r="G127" s="57"/>
+      <c r="H127" s="52">
+        <v>0</v>
+      </c>
+      <c r="I127" s="60"/>
+      <c r="J127" s="62"/>
+    </row>
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="12"/>
+      <c r="B128" s="38" t="s">
         <v>405</v>
       </c>
-      <c r="C126" s="48" t="s">
+      <c r="C128" s="48" t="s">
         <v>397</v>
       </c>
-      <c r="D126" s="49">
+      <c r="D128" s="49">
         <v>42831</v>
       </c>
-      <c r="E126" s="50"/>
-      <c r="F126" s="51" t="s">
+      <c r="E128" s="50"/>
+      <c r="F128" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="G126" s="51"/>
-      <c r="H126" s="51">
-        <v>0</v>
-      </c>
-      <c r="I126" s="42">
+      <c r="G128" s="51"/>
+      <c r="H128" s="51">
+        <v>0</v>
+      </c>
+      <c r="I128" s="42">
         <v>42834</v>
       </c>
-      <c r="J126" t="s">
+      <c r="J128" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="127" spans="1:11" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B127" s="22" t="s">
+    <row r="129" spans="1:10" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B129" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="C127" s="13" t="s">
+      <c r="C129" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="D127" s="19">
+      <c r="D129" s="19">
         <v>42760</v>
       </c>
-      <c r="E127" s="19"/>
-      <c r="F127" s="12" t="s">
+      <c r="E129" s="19"/>
+      <c r="F129" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="H127" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B128" s="23" t="s">
+      <c r="H129" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" s="12" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B130" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="C128" s="13" t="s">
+      <c r="C130" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="D128" s="19">
+      <c r="D130" s="19">
         <v>42760</v>
       </c>
-      <c r="E128" s="19"/>
-      <c r="F128" s="19" t="s">
+      <c r="E130" s="19"/>
+      <c r="F130" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="H128" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="52"/>
-      <c r="B129" s="53" t="s">
+      <c r="H130" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="52"/>
+      <c r="B131" s="53" t="s">
         <v>369</v>
       </c>
-      <c r="C129" s="55"/>
-      <c r="D129" s="56"/>
-      <c r="E129" s="56"/>
-      <c r="F129" s="56"/>
-      <c r="G129" s="52" t="s">
+      <c r="C131" s="55"/>
+      <c r="D131" s="56"/>
+      <c r="E131" s="56"/>
+      <c r="F131" s="56"/>
+      <c r="G131" s="52" t="s">
         <v>370</v>
       </c>
-      <c r="H129" s="52">
+      <c r="H131" s="52">
         <v>3</v>
       </c>
-      <c r="I129" s="52"/>
-      <c r="J129" s="52"/>
-    </row>
-    <row r="130" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B130" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="F130" t="s">
-        <v>138</v>
-      </c>
-      <c r="H130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="C131" s="9"/>
-      <c r="D131" s="9"/>
-      <c r="E131" s="9"/>
-      <c r="H131">
-        <v>0</v>
-      </c>
+      <c r="I131" s="52"/>
+      <c r="J131" s="52"/>
     </row>
     <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B132" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C132" s="9"/>
-      <c r="D132" s="9"/>
-      <c r="E132" s="9"/>
+      <c r="B132" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F132" t="s">
+        <v>138</v>
+      </c>
       <c r="H132">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B133" s="7" t="s">
+      <c r="B133" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="H133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="H134">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B135" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="F133" t="s">
+      <c r="F135" t="s">
         <v>133</v>
       </c>
-      <c r="H133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="12"/>
-      <c r="B134" s="7" t="s">
+      <c r="H135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="12"/>
+      <c r="B136" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="H134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A135" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B135" s="58" t="s">
+      <c r="H136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B137" s="58" t="s">
         <v>396</v>
       </c>
-      <c r="C135" s="58"/>
-      <c r="D135" s="59">
+      <c r="C137" s="58"/>
+      <c r="D137" s="59">
         <v>42818</v>
       </c>
-      <c r="E135" s="58"/>
-      <c r="F135" s="57" t="s">
+      <c r="E137" s="58"/>
+      <c r="F137" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="G135" s="57"/>
-      <c r="H135" s="57">
-        <v>1</v>
-      </c>
-      <c r="I135" s="60">
+      <c r="G137" s="57"/>
+      <c r="H137" s="57">
+        <v>0</v>
+      </c>
+      <c r="I137" s="60">
         <v>42702</v>
       </c>
-      <c r="J135" s="57"/>
-    </row>
-    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B136" s="7" t="s">
+      <c r="J137" s="57"/>
+    </row>
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B138" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A137" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A138" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B138" s="7" t="s">
-        <v>123</v>
+      <c r="H138">
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
@@ -4928,7 +4955,7 @@
         <v>2</v>
       </c>
       <c r="B139" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
@@ -4936,7 +4963,7 @@
         <v>2</v>
       </c>
       <c r="B140" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
@@ -4944,7 +4971,7 @@
         <v>2</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
@@ -4952,97 +4979,84 @@
         <v>2</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B143" s="8" t="s">
+      <c r="B143" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A145" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B145" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="C143" s="8"/>
-      <c r="D143" s="8"/>
-      <c r="E143" s="8"/>
-    </row>
-    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B144" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="H144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B145" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="H145">
-        <v>0</v>
-      </c>
+      <c r="C145" s="8"/>
+      <c r="D145" s="8"/>
+      <c r="E145" s="8"/>
     </row>
     <row r="146" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B146" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="H146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="H147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B148" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="H146">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="12"/>
-      <c r="B147" s="7" t="s">
+      <c r="H148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="12"/>
+      <c r="B149" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="H147">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A148" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B148" s="8" t="s">
+      <c r="H149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A150" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" s="8" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B149" t="s">
-        <v>302</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="D149" s="26">
-        <v>42775</v>
-      </c>
-      <c r="E149" s="26"/>
-      <c r="H149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B150" t="s">
-        <v>304</v>
-      </c>
-      <c r="H150">
-        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -5050,7 +5064,7 @@
         <v>2</v>
       </c>
       <c r="B151" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>303</v>
@@ -5064,400 +5078,402 @@
       </c>
     </row>
     <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B152" s="58" t="s">
+      <c r="A152" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B152" t="s">
+        <v>304</v>
+      </c>
+      <c r="H152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B153" t="s">
+        <v>314</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="D153" s="26">
+        <v>42775</v>
+      </c>
+      <c r="E153" s="26"/>
+      <c r="H153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="B154" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="C152" s="58"/>
-      <c r="D152" s="58"/>
-      <c r="E152" s="58"/>
-      <c r="F152" s="57"/>
-      <c r="G152" s="57"/>
-      <c r="H152" s="57">
+      <c r="C154" s="58"/>
+      <c r="D154" s="58"/>
+      <c r="E154" s="58"/>
+      <c r="F154" s="57"/>
+      <c r="G154" s="57"/>
+      <c r="H154" s="57">
         <v>3</v>
       </c>
-      <c r="I152" s="57"/>
-      <c r="J152" s="57"/>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A153" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B153" s="7" t="s">
+      <c r="I154" s="57"/>
+      <c r="J154" s="57"/>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A155" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B155" s="7" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B154" s="7" t="s">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B156" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H154">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A155" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B155" s="16" t="s">
+      <c r="H156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="12"/>
+      <c r="B157" t="s">
+        <v>424</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D157" s="26">
+        <v>42845</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="F157" t="s">
+        <v>138</v>
+      </c>
+      <c r="G157" t="s">
+        <v>318</v>
+      </c>
+      <c r="H157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A158" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B158" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="D155" s="16"/>
-      <c r="E155" s="16"/>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A156" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B156" s="8" t="s">
+      <c r="D158" s="16"/>
+      <c r="E158" s="16"/>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A159" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B159" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D156" s="8"/>
-      <c r="E156" s="8"/>
-    </row>
-    <row r="157" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B157" s="9" t="s">
+      <c r="D159" s="8"/>
+      <c r="E159" s="8"/>
+    </row>
+    <row r="160" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B160" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="H157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B158" s="9" t="s">
+      <c r="H160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B161" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="H158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="12"/>
-      <c r="B159" s="9" t="s">
+      <c r="H161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="12"/>
+      <c r="B162" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="H159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A160" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B160" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D160" s="16"/>
-      <c r="E160" s="16"/>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A161" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B162" s="9" t="s">
-        <v>330</v>
-      </c>
       <c r="H162">
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A163" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B163" s="8" t="s">
+      <c r="B163" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D163" s="16"/>
+      <c r="E163" s="16"/>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A164" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B165" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A166" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B166" s="8" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="12"/>
-      <c r="B164" s="9" t="s">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="12"/>
+      <c r="B167" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="C164" s="7" t="s">
+      <c r="C167" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="D164" s="26">
+      <c r="D167" s="26">
         <v>42809</v>
       </c>
-      <c r="E164" s="26"/>
-      <c r="H164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="12"/>
-      <c r="B165" s="9" t="s">
+      <c r="E167" s="26"/>
+      <c r="H167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="12"/>
+      <c r="B168" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="C165" s="7" t="s">
+      <c r="C168" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="D165" s="26">
+      <c r="D168" s="26">
         <v>42809</v>
       </c>
-      <c r="E165" s="26"/>
-      <c r="H165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="12"/>
-      <c r="B166" s="9" t="s">
+      <c r="E168" s="26"/>
+      <c r="H168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="12"/>
+      <c r="B169" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="D166" s="26">
+      <c r="D169" s="26">
         <v>42809</v>
       </c>
-      <c r="E166" s="26"/>
-      <c r="H166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A167" s="12"/>
-      <c r="B167" s="9"/>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A168" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>250</v>
-      </c>
-      <c r="C168" s="8"/>
-    </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B169" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="C169" s="9"/>
-      <c r="D169" s="9"/>
-      <c r="E169" s="9"/>
+      <c r="E169" s="26"/>
       <c r="H169">
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B170" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C170" s="9"/>
-      <c r="D170" s="9"/>
-      <c r="E170" s="9"/>
-      <c r="H170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A170" s="12"/>
+      <c r="B170" s="9"/>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B171" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="H171">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B171" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C171" s="8"/>
+    </row>
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B172" s="7" t="s">
-        <v>239</v>
-      </c>
+      <c r="B172" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="C172" s="9"/>
+      <c r="D172" s="9"/>
+      <c r="E172" s="9"/>
       <c r="H172">
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B173" s="7" t="s">
-        <v>233</v>
-      </c>
+      <c r="B173" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C173" s="9"/>
+      <c r="D173" s="9"/>
+      <c r="E173" s="9"/>
       <c r="H173">
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A174" s="12"/>
-      <c r="B174" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="52"/>
-      <c r="B175" s="58" t="s">
-        <v>343</v>
-      </c>
-      <c r="C175" s="58"/>
-      <c r="D175" s="58"/>
-      <c r="E175" s="58"/>
-      <c r="F175" s="57"/>
-      <c r="G175" s="57"/>
-      <c r="H175" s="57">
-        <v>2</v>
-      </c>
-      <c r="I175" s="57"/>
-      <c r="J175" s="57"/>
-    </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="H174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="H175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B176" s="8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C176" s="8"/>
-      <c r="D176" s="8"/>
-      <c r="E176" s="8"/>
-      <c r="H176" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="12" t="s">
+      <c r="B176" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="H176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A177" s="12"/>
+      <c r="B177" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="52"/>
+      <c r="B178" s="58" t="s">
+        <v>343</v>
+      </c>
+      <c r="C178" s="58"/>
+      <c r="D178" s="58"/>
+      <c r="E178" s="58"/>
+      <c r="F178" s="57"/>
+      <c r="G178" s="57"/>
+      <c r="H178" s="57">
+        <v>2</v>
+      </c>
+      <c r="I178" s="57"/>
+      <c r="J178" s="57"/>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A179" s="52"/>
+      <c r="B179" s="58" t="s">
+        <v>425</v>
+      </c>
+      <c r="C179" s="58"/>
+      <c r="D179" s="59">
+        <v>42850</v>
+      </c>
+      <c r="E179" s="58"/>
+      <c r="F179" s="57"/>
+      <c r="G179" s="57"/>
+      <c r="H179" s="52">
         <v>1</v>
       </c>
-      <c r="B177" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="H177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B178" s="7" t="s">
-        <v>224</v>
-      </c>
-      <c r="F178" t="s">
-        <v>138</v>
-      </c>
-      <c r="H178">
-        <v>0</v>
-      </c>
-      <c r="I178" s="6">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B179" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="H179">
-        <v>0</v>
-      </c>
-      <c r="I179" s="6"/>
-    </row>
-    <row r="180" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I179" s="57"/>
+      <c r="J179" s="57"/>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B180" s="7" t="s">
-        <v>227</v>
-      </c>
-      <c r="G180" t="s">
-        <v>138</v>
-      </c>
-      <c r="H180">
-        <v>0</v>
-      </c>
-      <c r="I180" s="6"/>
-    </row>
-    <row r="181" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B180" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C180" s="8"/>
+      <c r="D180" s="8"/>
+      <c r="E180" s="8"/>
+      <c r="H180" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B181" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C181" s="13"/>
-      <c r="D181" s="13"/>
-      <c r="E181" s="13"/>
-      <c r="H181" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="182" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="52" t="s">
+      <c r="B181" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B182" s="55" t="s">
-        <v>254</v>
-      </c>
-      <c r="C182" s="55"/>
-      <c r="D182" s="55"/>
-      <c r="E182" s="55"/>
-      <c r="F182" s="52"/>
-      <c r="G182" s="57" t="s">
+      <c r="B182" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="F182" t="s">
         <v>138</v>
       </c>
-      <c r="H182" s="52">
-        <v>2</v>
-      </c>
-      <c r="I182" s="52"/>
-      <c r="J182" s="52"/>
-    </row>
-    <row r="183" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="52" t="s">
+      <c r="H182">
+        <v>0</v>
+      </c>
+      <c r="I182" s="6">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B183" s="55" t="s">
-        <v>257</v>
-      </c>
-      <c r="C183" s="55"/>
-      <c r="D183" s="55"/>
-      <c r="E183" s="55"/>
-      <c r="F183" s="52"/>
-      <c r="G183" s="57" t="s">
-        <v>138</v>
-      </c>
-      <c r="H183" s="52">
-        <v>2</v>
-      </c>
-      <c r="I183" s="52"/>
-      <c r="J183" s="52"/>
+      <c r="B183" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="H183">
+        <v>0</v>
+      </c>
+      <c r="I183" s="6"/>
     </row>
     <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B184" s="7" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="G184" t="s">
         <v>138</v>
@@ -5465,13 +5481,14 @@
       <c r="H184">
         <v>0</v>
       </c>
+      <c r="I184" s="6"/>
     </row>
     <row r="185" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C185" s="13"/>
       <c r="D185" s="13"/>
@@ -5480,158 +5497,161 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="12" t="s">
+    <row r="186" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B186" s="7" t="s">
-        <v>222</v>
-      </c>
-      <c r="H186">
-        <v>0</v>
-      </c>
+      <c r="B186" s="55" t="s">
+        <v>254</v>
+      </c>
+      <c r="C186" s="55"/>
+      <c r="D186" s="55"/>
+      <c r="E186" s="55"/>
+      <c r="F186" s="52"/>
+      <c r="G186" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="H186" s="52">
+        <v>2</v>
+      </c>
+      <c r="I186" s="52"/>
+      <c r="J186" s="52"/>
     </row>
     <row r="187" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="12" t="s">
+      <c r="A187" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B187" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C187" s="13"/>
-      <c r="D187" s="13"/>
-      <c r="E187" s="13"/>
-      <c r="F187" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="H187" s="12">
-        <v>0</v>
-      </c>
-      <c r="I187" s="14">
-        <v>42702</v>
-      </c>
-    </row>
-    <row r="188" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="52"/>
-      <c r="B188" s="55" t="s">
-        <v>344</v>
-      </c>
-      <c r="C188" s="55"/>
-      <c r="D188" s="55"/>
-      <c r="E188" s="55"/>
-      <c r="F188" s="52"/>
-      <c r="G188" s="52"/>
-      <c r="H188" s="52">
-        <v>2</v>
-      </c>
-      <c r="I188" s="61"/>
-      <c r="J188" s="52"/>
-    </row>
-    <row r="189" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="52"/>
-      <c r="B189" s="55" t="s">
-        <v>398</v>
-      </c>
-      <c r="C189" s="55"/>
-      <c r="D189" s="55"/>
-      <c r="E189" s="55"/>
-      <c r="F189" s="52"/>
-      <c r="G189" s="52"/>
-      <c r="H189" s="52">
+      <c r="B187" s="55" t="s">
+        <v>257</v>
+      </c>
+      <c r="C187" s="55"/>
+      <c r="D187" s="55"/>
+      <c r="E187" s="55"/>
+      <c r="F187" s="52"/>
+      <c r="G187" s="57" t="s">
+        <v>138</v>
+      </c>
+      <c r="H187" s="52">
+        <v>2</v>
+      </c>
+      <c r="I187" s="52"/>
+      <c r="J187" s="52"/>
+    </row>
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I189" s="61"/>
-      <c r="J189" s="52"/>
-    </row>
-    <row r="190" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B188" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="G188" t="s">
+        <v>138</v>
+      </c>
+      <c r="H188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B189" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C189" s="13"/>
+      <c r="D189" s="13"/>
+      <c r="E189" s="13"/>
+      <c r="H189" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B190" s="15" t="s">
+      <c r="B190" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="H190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B191" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C191" s="13"/>
+      <c r="D191" s="13"/>
+      <c r="E191" s="13"/>
+      <c r="F191" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H191" s="12">
+        <v>0</v>
+      </c>
+      <c r="I191" s="14">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="52"/>
+      <c r="B192" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="C192" s="55"/>
+      <c r="D192" s="55"/>
+      <c r="E192" s="55"/>
+      <c r="F192" s="52"/>
+      <c r="G192" s="52"/>
+      <c r="H192" s="52">
+        <v>2</v>
+      </c>
+      <c r="I192" s="61"/>
+      <c r="J192" s="52"/>
+    </row>
+    <row r="193" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="52"/>
+      <c r="B193" s="55" t="s">
+        <v>398</v>
+      </c>
+      <c r="C193" s="55"/>
+      <c r="D193" s="55"/>
+      <c r="E193" s="55"/>
+      <c r="F193" s="52"/>
+      <c r="G193" s="52"/>
+      <c r="H193" s="52">
+        <v>1</v>
+      </c>
+      <c r="I193" s="61"/>
+      <c r="J193" s="52"/>
+    </row>
+    <row r="194" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B194" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="C190" s="15"/>
-      <c r="D190" s="15"/>
-      <c r="E190" s="15"/>
-      <c r="F190" s="12" t="s">
+      <c r="C194" s="15"/>
+      <c r="D194" s="15"/>
+      <c r="E194" s="15"/>
+      <c r="F194" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="H190" s="12" t="s">
+      <c r="H194" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="I190" s="14"/>
-    </row>
-    <row r="191" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B191" s="53" t="s">
-        <v>402</v>
-      </c>
-      <c r="C191" s="65"/>
-      <c r="D191" s="65"/>
-      <c r="E191" s="65"/>
-      <c r="F191" s="52"/>
-      <c r="G191" s="52"/>
-      <c r="H191" s="52">
-        <v>1</v>
-      </c>
-      <c r="I191" s="61"/>
-      <c r="J191" s="52"/>
-    </row>
-    <row r="192" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B192" s="18" t="s">
-        <v>345</v>
-      </c>
-      <c r="C192" s="15"/>
-      <c r="D192" s="15"/>
-      <c r="E192" s="15"/>
-      <c r="H192" s="12">
-        <v>0</v>
-      </c>
-      <c r="I192" s="14"/>
-    </row>
-    <row r="193" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B193" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="C193" s="15"/>
-      <c r="D193" s="15"/>
-      <c r="E193" s="15"/>
-      <c r="I193" s="14"/>
-    </row>
-    <row r="194" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="52" t="s">
-        <v>1</v>
-      </c>
-      <c r="B194" s="65" t="s">
-        <v>261</v>
-      </c>
-      <c r="C194" s="65"/>
-      <c r="D194" s="65"/>
-      <c r="E194" s="65"/>
-      <c r="F194" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="G194" s="52"/>
-      <c r="H194" s="52">
-        <v>2</v>
-      </c>
-      <c r="I194" s="61"/>
-      <c r="J194" s="52"/>
-    </row>
-    <row r="195" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I194" s="14"/>
+    </row>
+    <row r="195" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="52" t="s">
         <v>1</v>
       </c>
       <c r="B195" s="53" t="s">
-        <v>327</v>
+        <v>402</v>
       </c>
       <c r="C195" s="65"/>
       <c r="D195" s="65"/>
@@ -5639,166 +5659,165 @@
       <c r="F195" s="52"/>
       <c r="G195" s="52"/>
       <c r="H195" s="52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I195" s="61"/>
       <c r="J195" s="52"/>
     </row>
-    <row r="196" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B196" s="15" t="s">
-        <v>325</v>
+      <c r="B196" s="18" t="s">
+        <v>345</v>
       </c>
       <c r="C196" s="15"/>
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
+      <c r="H196" s="12">
+        <v>0</v>
+      </c>
       <c r="I196" s="14"/>
     </row>
     <row r="197" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B197" s="15" t="s">
-        <v>326</v>
+      <c r="B197" s="18" t="s">
+        <v>324</v>
       </c>
       <c r="C197" s="15"/>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
       <c r="I197" s="14"/>
     </row>
-    <row r="198" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="12" t="s">
+    <row r="198" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B198" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="C198" s="15"/>
-      <c r="D198" s="15"/>
-      <c r="E198" s="15"/>
-      <c r="I198" s="14"/>
+      <c r="B198" s="65" t="s">
+        <v>261</v>
+      </c>
+      <c r="C198" s="65"/>
+      <c r="D198" s="65"/>
+      <c r="E198" s="65"/>
+      <c r="F198" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="G198" s="52"/>
+      <c r="H198" s="52">
+        <v>2</v>
+      </c>
+      <c r="I198" s="61"/>
+      <c r="J198" s="52"/>
     </row>
     <row r="199" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B199" s="55" t="s">
-        <v>253</v>
-      </c>
-      <c r="C199" s="55"/>
-      <c r="D199" s="55"/>
-      <c r="E199" s="55"/>
-      <c r="F199" s="52" t="s">
-        <v>133</v>
-      </c>
+      <c r="B199" s="53" t="s">
+        <v>327</v>
+      </c>
+      <c r="C199" s="65"/>
+      <c r="D199" s="65"/>
+      <c r="E199" s="65"/>
+      <c r="F199" s="52"/>
       <c r="G199" s="52"/>
       <c r="H199" s="52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I199" s="61"/>
       <c r="J199" s="52"/>
     </row>
-    <row r="200" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A200" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B200" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="C200" s="15"/>
+      <c r="D200" s="15"/>
+      <c r="E200" s="15"/>
+      <c r="I200" s="14"/>
+    </row>
+    <row r="201" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B201" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="C201" s="15"/>
+      <c r="D201" s="15"/>
+      <c r="E201" s="15"/>
+      <c r="I201" s="14"/>
+    </row>
+    <row r="202" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B202" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="C202" s="15"/>
+      <c r="D202" s="15"/>
+      <c r="E202" s="15"/>
+      <c r="I202" s="14"/>
+    </row>
+    <row r="203" spans="1:10" s="12" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B203" s="55" t="s">
+        <v>253</v>
+      </c>
+      <c r="C203" s="55"/>
+      <c r="D203" s="55"/>
+      <c r="E203" s="55"/>
+      <c r="F203" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="G203" s="52"/>
+      <c r="H203" s="52">
+        <v>3</v>
+      </c>
+      <c r="I203" s="61"/>
+      <c r="J203" s="52"/>
+    </row>
+    <row r="204" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A204" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="B200" s="16" t="s">
+      <c r="B204" s="16" t="s">
         <v>319</v>
       </c>
-      <c r="I200" s="6"/>
-    </row>
-    <row r="201" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="52" t="s">
+      <c r="I204" s="6"/>
+    </row>
+    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="52" t="s">
         <v>333</v>
       </c>
-      <c r="B201" s="58" t="s">
+      <c r="B205" s="58" t="s">
         <v>320</v>
       </c>
-      <c r="C201" s="58"/>
-      <c r="D201" s="58"/>
-      <c r="E201" s="58"/>
-      <c r="F201" s="57"/>
-      <c r="G201" s="57"/>
-      <c r="H201" s="57">
+      <c r="C205" s="58"/>
+      <c r="D205" s="58"/>
+      <c r="E205" s="58"/>
+      <c r="F205" s="57"/>
+      <c r="G205" s="57"/>
+      <c r="H205" s="57">
         <v>3</v>
       </c>
-      <c r="I201" s="60"/>
-      <c r="J201" s="57"/>
-    </row>
-    <row r="202" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="52" t="s">
-        <v>333</v>
-      </c>
-      <c r="B202" s="58" t="s">
-        <v>321</v>
-      </c>
-      <c r="C202" s="58"/>
-      <c r="D202" s="58"/>
-      <c r="E202" s="58"/>
-      <c r="F202" s="57"/>
-      <c r="G202" s="57"/>
-      <c r="H202" s="57">
-        <v>3</v>
-      </c>
-      <c r="I202" s="60"/>
-      <c r="J202" s="57"/>
-    </row>
-    <row r="203" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="52" t="s">
-        <v>333</v>
-      </c>
-      <c r="B203" s="58" t="s">
-        <v>336</v>
-      </c>
-      <c r="C203" s="58"/>
-      <c r="D203" s="58"/>
-      <c r="E203" s="58"/>
-      <c r="F203" s="57"/>
-      <c r="G203" s="57"/>
-      <c r="H203" s="57">
-        <v>3</v>
-      </c>
-      <c r="I203" s="60"/>
-      <c r="J203" s="57"/>
-    </row>
-    <row r="204" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="52" t="s">
-        <v>333</v>
-      </c>
-      <c r="B204" s="58" t="s">
-        <v>331</v>
-      </c>
-      <c r="C204" s="58"/>
-      <c r="D204" s="58"/>
-      <c r="E204" s="58"/>
-      <c r="F204" s="57"/>
-      <c r="G204" s="57"/>
-      <c r="H204" s="57">
-        <v>3</v>
-      </c>
-      <c r="I204" s="60"/>
-      <c r="J204" s="57"/>
-    </row>
-    <row r="205" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="12" t="s">
-        <v>333</v>
-      </c>
-      <c r="B205" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="H205">
-        <v>0</v>
-      </c>
-      <c r="I205" s="6"/>
+      <c r="I205" s="60"/>
+      <c r="J205" s="57"/>
     </row>
     <row r="206" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="52" t="s">
         <v>333</v>
       </c>
       <c r="B206" s="58" t="s">
-        <v>360</v>
+        <v>321</v>
       </c>
       <c r="C206" s="58"/>
       <c r="D206" s="58"/>
@@ -5806,7 +5825,7 @@
       <c r="F206" s="57"/>
       <c r="G206" s="57"/>
       <c r="H206" s="57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I206" s="60"/>
       <c r="J206" s="57"/>
@@ -5816,7 +5835,7 @@
         <v>333</v>
       </c>
       <c r="B207" s="58" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C207" s="58"/>
       <c r="D207" s="58"/>
@@ -5834,7 +5853,7 @@
         <v>333</v>
       </c>
       <c r="B208" s="58" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C208" s="58"/>
       <c r="D208" s="58"/>
@@ -5848,255 +5867,253 @@
       <c r="J208" s="57"/>
     </row>
     <row r="209" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="52" t="s">
+      <c r="A209" s="12" t="s">
         <v>333</v>
       </c>
-      <c r="B209" s="58" t="s">
+      <c r="B209" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="H209">
+        <v>0</v>
+      </c>
+      <c r="I209" s="6"/>
+    </row>
+    <row r="210" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="52" t="s">
+        <v>333</v>
+      </c>
+      <c r="B210" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C210" s="58"/>
+      <c r="D210" s="58"/>
+      <c r="E210" s="58"/>
+      <c r="F210" s="57"/>
+      <c r="G210" s="57"/>
+      <c r="H210" s="57">
+        <v>2</v>
+      </c>
+      <c r="I210" s="60"/>
+      <c r="J210" s="57"/>
+    </row>
+    <row r="211" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="52" t="s">
+        <v>333</v>
+      </c>
+      <c r="B211" s="58" t="s">
+        <v>338</v>
+      </c>
+      <c r="C211" s="58"/>
+      <c r="D211" s="58"/>
+      <c r="E211" s="58"/>
+      <c r="F211" s="57"/>
+      <c r="G211" s="57"/>
+      <c r="H211" s="57">
+        <v>3</v>
+      </c>
+      <c r="I211" s="60"/>
+      <c r="J211" s="57"/>
+    </row>
+    <row r="212" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="52" t="s">
+        <v>333</v>
+      </c>
+      <c r="B212" s="58" t="s">
+        <v>339</v>
+      </c>
+      <c r="C212" s="58"/>
+      <c r="D212" s="58"/>
+      <c r="E212" s="58"/>
+      <c r="F212" s="57"/>
+      <c r="G212" s="57"/>
+      <c r="H212" s="57">
+        <v>3</v>
+      </c>
+      <c r="I212" s="60"/>
+      <c r="J212" s="57"/>
+    </row>
+    <row r="213" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="52" t="s">
+        <v>333</v>
+      </c>
+      <c r="B213" s="58" t="s">
         <v>337</v>
       </c>
-      <c r="C209" s="58"/>
-      <c r="D209" s="58"/>
-      <c r="E209" s="58"/>
-      <c r="F209" s="57"/>
-      <c r="G209" s="57"/>
-      <c r="H209" s="57">
+      <c r="C213" s="58"/>
+      <c r="D213" s="58"/>
+      <c r="E213" s="58"/>
+      <c r="F213" s="57"/>
+      <c r="G213" s="57"/>
+      <c r="H213" s="57">
         <v>3</v>
       </c>
-      <c r="I209" s="60"/>
-      <c r="J209" s="57"/>
-    </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A210" s="12"/>
-      <c r="B210" s="7" t="s">
-        <v>354</v>
-      </c>
-      <c r="I210" s="6"/>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A211" s="12"/>
-      <c r="I211" s="6"/>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A212" s="12"/>
-      <c r="B212" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="I212" s="6"/>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A213" s="12"/>
-      <c r="B213" s="7" t="s">
-        <v>379</v>
-      </c>
-      <c r="I213" s="6"/>
+      <c r="I213" s="60"/>
+      <c r="J213" s="57"/>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="12"/>
       <c r="B214" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="I214" s="6"/>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215" s="12"/>
+      <c r="I215" s="6"/>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216" s="12"/>
+      <c r="B216" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="I216" s="6"/>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217" s="12"/>
+      <c r="B217" s="7" t="s">
+        <v>379</v>
+      </c>
+      <c r="I217" s="6"/>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A218" s="12"/>
+      <c r="B218" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="I214" s="6"/>
-    </row>
-    <row r="215" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B215" s="16" t="s">
+      <c r="I218" s="6"/>
+    </row>
+    <row r="219" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B219" s="16" t="s">
         <v>334</v>
       </c>
-      <c r="I215" s="6"/>
-    </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B216" s="15" t="s">
+      <c r="I219" s="6"/>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B220" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="I216" s="6"/>
-    </row>
-    <row r="217" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B217" s="7" t="s">
+      <c r="I220" s="6"/>
+    </row>
+    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B221" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="H217">
-        <v>0</v>
-      </c>
-      <c r="I217" s="6"/>
-    </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I218" s="6"/>
-    </row>
-    <row r="219" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="B219" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="C219" s="15"/>
-      <c r="D219" s="15"/>
-      <c r="E219" s="15"/>
-      <c r="I219" s="14"/>
-    </row>
-    <row r="220" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="B220" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="F220" t="s">
-        <v>133</v>
-      </c>
-      <c r="H220">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="221" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="12" t="s">
-        <v>315</v>
-      </c>
-      <c r="B221" s="7" t="s">
-        <v>328</v>
-      </c>
       <c r="H221">
-        <v>9</v>
-      </c>
-      <c r="J221" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="222" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="12"/>
-      <c r="B222" s="7" t="s">
-        <v>377</v>
-      </c>
-      <c r="H222">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="223" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I221" s="6"/>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I222" s="6"/>
+    </row>
+    <row r="223" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="B223" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="H223">
-        <v>0</v>
-      </c>
+      <c r="B223" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="C223" s="15"/>
+      <c r="D223" s="15"/>
+      <c r="E223" s="15"/>
+      <c r="I223" s="14"/>
     </row>
     <row r="224" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="12" t="s">
         <v>315</v>
       </c>
       <c r="B224" s="7" t="s">
-        <v>255</v>
+        <v>134</v>
+      </c>
+      <c r="F224" t="s">
+        <v>133</v>
       </c>
       <c r="H224">
         <v>0</v>
       </c>
-      <c r="I224" s="6"/>
     </row>
     <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
         <v>315</v>
       </c>
       <c r="B225" s="7" t="s">
-        <v>120</v>
+        <v>328</v>
       </c>
       <c r="H225">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J225" t="s">
-        <v>144</v>
+        <v>376</v>
       </c>
     </row>
     <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="52"/>
-      <c r="B226" s="58" t="s">
-        <v>346</v>
-      </c>
-      <c r="C226" s="58"/>
-      <c r="D226" s="58"/>
-      <c r="E226" s="58"/>
-      <c r="F226" s="57"/>
-      <c r="G226" s="57"/>
-      <c r="H226" s="57">
-        <v>2</v>
-      </c>
-      <c r="I226" s="57"/>
-      <c r="J226" s="57"/>
-    </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A226" s="12"/>
+      <c r="B226" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="H226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="B227" s="8" t="s">
-        <v>297</v>
+        <v>315</v>
+      </c>
+      <c r="B227" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="H227">
+        <v>0</v>
       </c>
     </row>
     <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="B228" s="7" t="s">
-        <v>298</v>
+        <v>255</v>
       </c>
       <c r="H228">
         <v>0</v>
       </c>
+      <c r="I228" s="6"/>
     </row>
     <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="B229" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F229" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="H229">
         <v>0</v>
-      </c>
-      <c r="I229" s="6">
-        <v>42702</v>
       </c>
       <c r="J229" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="12" t="s">
-        <v>297</v>
-      </c>
-      <c r="B230" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="C230" s="9"/>
-      <c r="D230" s="9"/>
-      <c r="E230" s="9"/>
-      <c r="H230">
-        <v>0</v>
-      </c>
-      <c r="I230" s="6">
-        <v>42702</v>
-      </c>
-      <c r="J230" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="52"/>
+      <c r="B230" s="58" t="s">
+        <v>346</v>
+      </c>
+      <c r="C230" s="58"/>
+      <c r="D230" s="58"/>
+      <c r="E230" s="58"/>
+      <c r="F230" s="57"/>
+      <c r="G230" s="57"/>
+      <c r="H230" s="57">
+        <v>2</v>
+      </c>
+      <c r="I230" s="57"/>
+      <c r="J230" s="57"/>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="B231" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F231" t="s">
-        <v>133</v>
-      </c>
-      <c r="H231">
-        <v>0</v>
-      </c>
-      <c r="I231" s="6">
-        <v>42702</v>
+      <c r="B231" s="8" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
@@ -6104,10 +6121,7 @@
         <v>297</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F232" t="s">
-        <v>135</v>
+        <v>298</v>
       </c>
       <c r="H232">
         <v>0</v>
@@ -6118,16 +6132,16 @@
         <v>297</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F233" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H233">
         <v>0</v>
       </c>
       <c r="I233" s="6">
-        <v>42697</v>
+        <v>42702</v>
       </c>
       <c r="J233" t="s">
         <v>144</v>
@@ -6137,177 +6151,204 @@
       <c r="A234" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="B234" s="7" t="s">
+      <c r="B234" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C234" s="9"/>
+      <c r="D234" s="9"/>
+      <c r="E234" s="9"/>
+      <c r="H234">
+        <v>0</v>
+      </c>
+      <c r="I234" s="6">
+        <v>42702</v>
+      </c>
+      <c r="J234" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B235" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="F235" t="s">
+        <v>133</v>
+      </c>
+      <c r="H235">
+        <v>0</v>
+      </c>
+      <c r="I235" s="6">
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B236" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="F236" t="s">
+        <v>135</v>
+      </c>
+      <c r="H236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B237" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F237" t="s">
+        <v>135</v>
+      </c>
+      <c r="H237">
+        <v>0</v>
+      </c>
+      <c r="I237" s="6">
+        <v>42697</v>
+      </c>
+      <c r="J237" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B238" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="H234">
-        <v>0</v>
-      </c>
-      <c r="I234" s="6"/>
-    </row>
-    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="12"/>
-      <c r="B235" s="13" t="s">
+      <c r="H238">
+        <v>0</v>
+      </c>
+      <c r="I238" s="6"/>
+    </row>
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="12"/>
+      <c r="B239" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="H235">
+      <c r="H239">
         <v>9</v>
       </c>
-      <c r="I235" s="6"/>
-    </row>
-    <row r="236" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B236" s="16" t="s">
+      <c r="I239" s="6"/>
+    </row>
+    <row r="240" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="12"/>
+      <c r="B240" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="C240" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D240" s="26">
+        <v>42845</v>
+      </c>
+      <c r="E240" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="F240" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G240" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="H240">
+        <v>0</v>
+      </c>
+      <c r="I240" s="6"/>
+    </row>
+    <row r="241" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B241" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="C236" s="16"/>
-      <c r="D236" s="16"/>
-      <c r="E236" s="16"/>
-    </row>
-    <row r="237" spans="1:10" ht="21" hidden="1" x14ac:dyDescent="0.35">
-      <c r="B237" s="64" t="s">
+      <c r="C241" s="16"/>
+      <c r="D241" s="16"/>
+      <c r="E241" s="16"/>
+    </row>
+    <row r="242" spans="1:10" ht="21" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B242" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="C237" s="16"/>
-      <c r="D237" s="16"/>
-      <c r="E237" s="16"/>
-      <c r="H237">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="238" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B238" s="16"/>
-      <c r="C238" s="16"/>
-      <c r="D238" s="16"/>
-      <c r="E238" s="16"/>
-    </row>
-    <row r="239" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B239" s="64" t="s">
-        <v>420</v>
-      </c>
-      <c r="C239" s="16"/>
-      <c r="D239" s="16"/>
-      <c r="E239" s="16"/>
-    </row>
-    <row r="240" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B240" s="57" t="s">
-        <v>421</v>
-      </c>
-      <c r="C240" s="16"/>
-      <c r="D240" s="16"/>
-      <c r="E240" s="16"/>
-      <c r="H240">
+      <c r="C242" s="16"/>
+      <c r="D242" s="16"/>
+      <c r="E242" s="16"/>
+      <c r="H242">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B243" s="16"/>
+      <c r="C243" s="16"/>
+      <c r="D243" s="16"/>
+      <c r="E243" s="16"/>
+    </row>
+    <row r="244" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B244" s="64" t="s">
+        <v>418</v>
+      </c>
+      <c r="C244" s="16"/>
+      <c r="D244" s="16"/>
+      <c r="E244" s="16"/>
+    </row>
+    <row r="245" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="B245" s="57" t="s">
+        <v>419</v>
+      </c>
+      <c r="C245" s="16"/>
+      <c r="D245" s="16"/>
+      <c r="E245" s="16"/>
+      <c r="H245">
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="57"/>
-      <c r="B241" s="64" t="s">
+    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="57"/>
+      <c r="B246" s="64" t="s">
         <v>262</v>
       </c>
-      <c r="C241" s="58"/>
-      <c r="D241" s="58"/>
-      <c r="E241" s="58"/>
-      <c r="F241" s="57"/>
-      <c r="G241" s="57"/>
-      <c r="H241" s="57">
-        <v>2</v>
-      </c>
-      <c r="I241" s="57"/>
-      <c r="J241" s="57"/>
-    </row>
-    <row r="242" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="57"/>
-      <c r="B242" s="57" t="s">
-        <v>313</v>
-      </c>
-      <c r="C242" s="58" t="s">
-        <v>303</v>
-      </c>
-      <c r="D242" s="59">
-        <v>42775</v>
-      </c>
-      <c r="E242" s="59"/>
-      <c r="F242" s="57"/>
-      <c r="G242" s="57"/>
-      <c r="H242" s="57">
-        <v>2</v>
-      </c>
-      <c r="I242" s="57"/>
-      <c r="J242" s="57"/>
-    </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A243" s="57"/>
-      <c r="B243" s="58" t="s">
-        <v>347</v>
-      </c>
-      <c r="C243" s="58"/>
-      <c r="D243" s="58"/>
-      <c r="E243" s="58"/>
-      <c r="F243" s="57"/>
-      <c r="G243" s="57"/>
-      <c r="H243" s="57">
-        <v>1</v>
-      </c>
-      <c r="I243" s="57"/>
-      <c r="J243" s="57"/>
-    </row>
-    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B244" t="s">
-        <v>305</v>
-      </c>
-      <c r="C244" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="D244" s="26">
-        <v>42775</v>
-      </c>
-      <c r="E244" s="26"/>
-      <c r="H244">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="57"/>
-      <c r="B245" s="58" t="s">
-        <v>382</v>
-      </c>
-      <c r="C245" s="58"/>
-      <c r="D245" s="58"/>
-      <c r="E245" s="58"/>
-      <c r="F245" s="57"/>
-      <c r="G245" s="57"/>
-      <c r="H245" s="57">
-        <v>0</v>
-      </c>
-      <c r="I245" s="60"/>
-      <c r="J245" s="57"/>
-    </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B246" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="I246" s="6"/>
+      <c r="C246" s="58"/>
+      <c r="D246" s="58"/>
+      <c r="E246" s="58"/>
+      <c r="F246" s="57"/>
+      <c r="G246" s="57"/>
+      <c r="H246" s="57">
+        <v>2</v>
+      </c>
+      <c r="I246" s="57"/>
+      <c r="J246" s="57"/>
     </row>
     <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="57"/>
-      <c r="B247" s="58" t="s">
-        <v>357</v>
-      </c>
-      <c r="C247" s="58"/>
-      <c r="D247" s="58"/>
-      <c r="E247" s="58"/>
+      <c r="B247" s="57" t="s">
+        <v>313</v>
+      </c>
+      <c r="C247" s="58" t="s">
+        <v>303</v>
+      </c>
+      <c r="D247" s="59">
+        <v>42775</v>
+      </c>
+      <c r="E247" s="59"/>
       <c r="F247" s="57"/>
       <c r="G247" s="57"/>
       <c r="H247" s="57">
         <v>2</v>
       </c>
-      <c r="I247" s="60"/>
+      <c r="I247" s="57"/>
       <c r="J247" s="57"/>
     </row>
-    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="57"/>
       <c r="B248" s="58" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="C248" s="58"/>
       <c r="D248" s="58"/>
@@ -6315,53 +6356,52 @@
       <c r="F248" s="57"/>
       <c r="G248" s="57"/>
       <c r="H248" s="57">
-        <v>2</v>
-      </c>
-      <c r="I248" s="60"/>
+        <v>1</v>
+      </c>
+      <c r="I248" s="57"/>
       <c r="J248" s="57"/>
     </row>
     <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="57"/>
-      <c r="B249" s="58" t="s">
-        <v>359</v>
-      </c>
-      <c r="C249" s="58"/>
-      <c r="D249" s="58"/>
-      <c r="E249" s="58"/>
-      <c r="F249" s="57"/>
-      <c r="G249" s="57"/>
-      <c r="H249" s="57">
-        <v>2</v>
-      </c>
-      <c r="I249" s="60"/>
-      <c r="J249" s="57"/>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B250" s="7" t="s">
-        <v>381</v>
-      </c>
-      <c r="I250" s="6"/>
-    </row>
-    <row r="251" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="57"/>
-      <c r="B251" s="58" t="s">
-        <v>355</v>
-      </c>
-      <c r="C251" s="58"/>
-      <c r="D251" s="58"/>
-      <c r="E251" s="58"/>
-      <c r="F251" s="57"/>
-      <c r="G251" s="57"/>
-      <c r="H251" s="57">
-        <v>2</v>
-      </c>
-      <c r="I251" s="60"/>
-      <c r="J251" s="57"/>
+      <c r="B249" t="s">
+        <v>305</v>
+      </c>
+      <c r="C249" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D249" s="26">
+        <v>42775</v>
+      </c>
+      <c r="E249" s="26"/>
+      <c r="H249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="57"/>
+      <c r="B250" s="58" t="s">
+        <v>382</v>
+      </c>
+      <c r="C250" s="58"/>
+      <c r="D250" s="58"/>
+      <c r="E250" s="58"/>
+      <c r="F250" s="57"/>
+      <c r="G250" s="57"/>
+      <c r="H250" s="57">
+        <v>0</v>
+      </c>
+      <c r="I250" s="60"/>
+      <c r="J250" s="57"/>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B251" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="I251" s="6"/>
     </row>
     <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="57"/>
       <c r="B252" s="58" t="s">
-        <v>399</v>
+        <v>357</v>
       </c>
       <c r="C252" s="58"/>
       <c r="D252" s="58"/>
@@ -6377,7 +6417,7 @@
     <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="57"/>
       <c r="B253" s="58" t="s">
-        <v>400</v>
+        <v>358</v>
       </c>
       <c r="C253" s="58"/>
       <c r="D253" s="58"/>
@@ -6393,7 +6433,7 @@
     <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="57"/>
       <c r="B254" s="58" t="s">
-        <v>401</v>
+        <v>359</v>
       </c>
       <c r="C254" s="58"/>
       <c r="D254" s="58"/>
@@ -6407,354 +6447,363 @@
       <c r="J254" s="57"/>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B255" s="8" t="s">
+      <c r="B255" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="I255" s="6"/>
+    </row>
+    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="57"/>
+      <c r="B256" s="58" t="s">
+        <v>355</v>
+      </c>
+      <c r="C256" s="58"/>
+      <c r="D256" s="58"/>
+      <c r="E256" s="58"/>
+      <c r="F256" s="57"/>
+      <c r="G256" s="57"/>
+      <c r="H256" s="57">
+        <v>2</v>
+      </c>
+      <c r="I256" s="60"/>
+      <c r="J256" s="57"/>
+    </row>
+    <row r="257" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="57"/>
+      <c r="B257" s="58" t="s">
+        <v>399</v>
+      </c>
+      <c r="C257" s="58"/>
+      <c r="D257" s="58"/>
+      <c r="E257" s="58"/>
+      <c r="F257" s="57"/>
+      <c r="G257" s="57"/>
+      <c r="H257" s="57">
+        <v>2</v>
+      </c>
+      <c r="I257" s="60"/>
+      <c r="J257" s="57"/>
+    </row>
+    <row r="258" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="57"/>
+      <c r="B258" s="58" t="s">
+        <v>400</v>
+      </c>
+      <c r="C258" s="58"/>
+      <c r="D258" s="58"/>
+      <c r="E258" s="58"/>
+      <c r="F258" s="57"/>
+      <c r="G258" s="57"/>
+      <c r="H258" s="57">
+        <v>2</v>
+      </c>
+      <c r="I258" s="60"/>
+      <c r="J258" s="57"/>
+    </row>
+    <row r="259" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="57"/>
+      <c r="B259" s="58" t="s">
+        <v>401</v>
+      </c>
+      <c r="C259" s="58"/>
+      <c r="D259" s="58"/>
+      <c r="E259" s="58"/>
+      <c r="F259" s="57"/>
+      <c r="G259" s="57"/>
+      <c r="H259" s="57">
+        <v>2</v>
+      </c>
+      <c r="I259" s="60"/>
+      <c r="J259" s="57"/>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B260" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="C255" s="8"/>
-      <c r="D255" s="8"/>
-      <c r="E255" s="8"/>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A256">
+      <c r="C260" s="8"/>
+      <c r="D260" s="8"/>
+      <c r="E260" s="8"/>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A261">
         <v>1</v>
       </c>
-      <c r="B256" s="7" t="s">
+      <c r="B261" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="F256" t="s">
+      <c r="F261" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="257" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A257">
-        <v>2</v>
-      </c>
-      <c r="B257" s="7" t="s">
+    <row r="262" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>2</v>
+      </c>
+      <c r="B262" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="F257" t="s">
+      <c r="F262" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A258">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A263">
         <v>3</v>
       </c>
-      <c r="B258" s="7" t="s">
+      <c r="B263" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="F258" t="s">
+      <c r="F263" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A259">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A264">
         <v>4</v>
       </c>
-      <c r="B259" s="7" t="s">
+      <c r="B264" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A260" t="s">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
         <v>174</v>
       </c>
-      <c r="B260" s="7" t="s">
+      <c r="B265" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="F260" t="s">
+      <c r="F265" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B261" s="7" t="s">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B266" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="F261" t="s">
+      <c r="F266" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B262" s="7" t="s">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B267" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="F262" t="s">
+      <c r="F267" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B263" s="7" t="s">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B268" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="F263" t="s">
+      <c r="F268" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="264" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B264" s="7" t="s">
+    <row r="269" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B269" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="F264" t="s">
+      <c r="F269" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="265" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B265" s="7" t="s">
+    <row r="270" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B270" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="F265" t="s">
+      <c r="F270" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B266" s="10" t="s">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B271" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C266" s="10"/>
-      <c r="D266" s="10"/>
-      <c r="E266" s="10"/>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B267" s="7" t="s">
+      <c r="C271" s="10"/>
+      <c r="D271" s="10"/>
+      <c r="E271" s="10"/>
+    </row>
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B272" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="F267" t="s">
+      <c r="F272" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B268" s="7" t="s">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B273" s="7" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B269" s="7" t="s">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B274" s="7" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="270" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B270" s="7" t="s">
+    <row r="275" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B275" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B271" s="7" t="s">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B276" s="7" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="272" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B272" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="F272" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="273" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B273" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="274" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B274" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="F274" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B275" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="F275" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B276" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="C276" s="10"/>
-      <c r="D276" s="10"/>
-      <c r="E276" s="10"/>
     </row>
     <row r="277" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B277" s="7" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F277" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="278" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B278" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="F278" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="279" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B279" s="7" t="s">
-        <v>186</v>
+        <v>194</v>
+      </c>
+      <c r="F279" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B280" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="F280" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B281" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C281" s="10"/>
+      <c r="D281" s="10"/>
+      <c r="E281" s="10"/>
+    </row>
+    <row r="282" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B282" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="F282" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="283" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B283" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="F283" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B284" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B285" s="7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="281" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A281">
+    <row r="286" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A286">
         <v>1</v>
       </c>
-      <c r="B281" s="7" t="s">
+      <c r="B286" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="H281">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A282">
-        <v>2</v>
-      </c>
-      <c r="B282" s="7" t="s">
+      <c r="H286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>2</v>
+      </c>
+      <c r="B287" s="7" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="283" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A283" s="57"/>
-      <c r="B283" s="58" t="s">
+    <row r="288" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="57"/>
+      <c r="B288" s="58" t="s">
         <v>198</v>
       </c>
-      <c r="C283" s="58"/>
-      <c r="D283" s="58"/>
-      <c r="E283" s="58"/>
-      <c r="F283" s="57"/>
-      <c r="G283" s="57"/>
-      <c r="H283" s="57">
-        <v>2</v>
-      </c>
-      <c r="I283" s="57"/>
-      <c r="J283" s="57"/>
-    </row>
-    <row r="284" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="57"/>
-      <c r="B284" s="58" t="s">
+      <c r="C288" s="58"/>
+      <c r="D288" s="58"/>
+      <c r="E288" s="58"/>
+      <c r="F288" s="57"/>
+      <c r="G288" s="57"/>
+      <c r="H288" s="57">
+        <v>2</v>
+      </c>
+      <c r="I288" s="57"/>
+      <c r="J288" s="57"/>
+    </row>
+    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="57"/>
+      <c r="B289" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="C284" s="58"/>
-      <c r="D284" s="58"/>
-      <c r="E284" s="58"/>
-      <c r="F284" s="57"/>
-      <c r="G284" s="57"/>
-      <c r="H284" s="57">
-        <v>2</v>
-      </c>
-      <c r="I284" s="57"/>
-      <c r="J284" s="57"/>
-    </row>
-    <row r="285" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="57"/>
-      <c r="B285" s="58" t="s">
+      <c r="C289" s="58"/>
+      <c r="D289" s="58"/>
+      <c r="E289" s="58"/>
+      <c r="F289" s="57"/>
+      <c r="G289" s="57"/>
+      <c r="H289" s="57">
+        <v>2</v>
+      </c>
+      <c r="I289" s="57"/>
+      <c r="J289" s="57"/>
+    </row>
+    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="57"/>
+      <c r="B290" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="C285" s="58"/>
-      <c r="D285" s="58"/>
-      <c r="E285" s="58"/>
-      <c r="F285" s="57"/>
-      <c r="G285" s="57"/>
-      <c r="H285" s="57">
+      <c r="C290" s="58"/>
+      <c r="D290" s="58"/>
+      <c r="E290" s="58"/>
+      <c r="F290" s="57"/>
+      <c r="G290" s="57"/>
+      <c r="H290" s="57">
         <v>3</v>
       </c>
-      <c r="I285" s="57"/>
-      <c r="J285" s="57"/>
-    </row>
-    <row r="286" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B286" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="H286">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="287" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B287" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="H287">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="288" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B288" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="F288" t="s">
-        <v>219</v>
-      </c>
-      <c r="H288">
-        <v>0</v>
-      </c>
-      <c r="I288" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B289" s="7" t="s">
-        <v>203</v>
-      </c>
-      <c r="F289" t="s">
-        <v>220</v>
-      </c>
-      <c r="H289">
-        <v>0</v>
-      </c>
-      <c r="I289" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B290" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="F290" t="s">
-        <v>221</v>
-      </c>
-      <c r="H290">
-        <v>0</v>
-      </c>
-      <c r="I290" t="s">
-        <v>144</v>
-      </c>
+      <c r="I290" s="57"/>
+      <c r="J290" s="57"/>
     </row>
     <row r="291" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B291" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H291">
         <v>0</v>
-      </c>
-      <c r="I291" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="292" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B292" s="7" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="H292">
         <v>0</v>
-      </c>
-      <c r="I292" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B293" s="7" t="s">
-        <v>207</v>
+        <v>202</v>
+      </c>
+      <c r="F293" t="s">
+        <v>219</v>
       </c>
       <c r="H293">
         <v>0</v>
@@ -6763,25 +6812,86 @@
         <v>144</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A294" s="57"/>
-      <c r="B294" s="58"/>
-      <c r="C294" s="58"/>
-      <c r="D294" s="58"/>
-      <c r="E294" s="58"/>
-      <c r="F294" s="57"/>
-      <c r="G294" s="57"/>
-      <c r="H294" s="57"/>
-      <c r="I294" s="57"/>
-      <c r="J294" s="57"/>
-    </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B294" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="F294" t="s">
+        <v>220</v>
+      </c>
+      <c r="H294">
+        <v>0</v>
+      </c>
+      <c r="I294" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="B295" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="F295" t="s">
+        <v>221</v>
+      </c>
+      <c r="H295">
+        <v>0</v>
+      </c>
+      <c r="I295" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B296" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="H296">
+        <v>0</v>
+      </c>
+      <c r="I296" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B297" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H297">
+        <v>0</v>
+      </c>
+      <c r="I297" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B298" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="H298">
+        <v>0</v>
+      </c>
+      <c r="I298" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" s="57"/>
+      <c r="B299" s="58"/>
+      <c r="C299" s="58"/>
+      <c r="D299" s="58"/>
+      <c r="E299" s="58"/>
+      <c r="F299" s="57"/>
+      <c r="G299" s="57"/>
+      <c r="H299" s="57"/>
+      <c r="I299" s="57"/>
+      <c r="J299" s="57"/>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B300" s="7" t="s">
         <v>218</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:J293">
+  <autoFilter ref="A7:J298">
     <filterColumn colId="7">
       <filters blank="1">
         <filter val="1"/>

</xml_diff>

<commit_message>
added UserFullName while creating users
</commit_message>
<xml_diff>
--- a/Documents/Technical/ProjectPlan-Internal.xlsx
+++ b/Documents/Technical/ProjectPlan-Internal.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="135" yWindow="-45" windowWidth="20355" windowHeight="7830" tabRatio="375" activeTab="3"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="433">
   <si>
     <t>Reports</t>
   </si>
@@ -1473,6 +1473,9 @@
   </si>
   <si>
     <t>No longer required.</t>
+  </si>
+  <si>
+    <t>Added UserFullName into User collection</t>
   </si>
 </sst>
 </file>
@@ -2779,10 +2782,10 @@
   <dimension ref="A1:K302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="7" topLeftCell="B277" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="7" topLeftCell="B165" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="B256" sqref="B256"/>
+      <selection pane="bottomRight" activeCell="J194" sqref="J194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5558,7 +5561,9 @@
         <v>1</v>
       </c>
       <c r="I188" s="52"/>
-      <c r="J188" s="52"/>
+      <c r="J188" s="52" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="189" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="52" t="s">
@@ -5669,7 +5674,9 @@
         <v>1</v>
       </c>
       <c r="I195" s="61"/>
-      <c r="J195" s="52"/>
+      <c r="J195" s="52" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="196" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="12" t="s">
@@ -6952,7 +6959,7 @@
   </sheetData>
   <autoFilter ref="A7:J300">
     <filterColumn colId="7">
-      <filters blank="1">
+      <filters>
         <filter val="1"/>
       </filters>
     </filterColumn>

</xml_diff>